<commit_message>
3.0.3: force default value as "" on specified query params. fix bug on non-reuquired and non-default value props.
</commit_message>
<xml_diff>
--- a/meta/components/PlainBoxSample.xlsx
+++ b/meta/components/PlainBoxSample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoVueComponent/meta/components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EADD35-1C8D-ED43-A72C-96A6B49A0FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B4C9076-C8FA-4A4C-AAB1-529FC62BEB62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="2280" windowWidth="25200" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21480" yWindow="2260" windowWidth="25200" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VueComponent" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="122">
   <si>
     <t>パッケージ</t>
   </si>
@@ -411,10 +411,6 @@
   </si>
   <si>
     <t>string</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>""</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
@@ -994,6 +990,18 @@
   </si>
   <si>
     <t>plainbox</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>fuga</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>fur</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>"ふが"</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1691,27 +1699,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1720,38 +1727,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1763,8 +1763,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1797,18 +1797,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1818,12 +1816,12 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1837,16 +1835,16 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1865,56 +1863,56 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="47" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2329,8 +2327,8 @@
   </sheetPr>
   <dimension ref="A1:M96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2348,10 +2346,10 @@
   <sheetData>
     <row r="1" spans="1:11" ht="19">
       <c r="A1" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -2366,66 +2364,54 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="35"/>
+      <c r="F6" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="8"/>
-      <c r="F7" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="35"/>
+      <c r="F7" s="1" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="8"/>
-      <c r="F8" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="35"/>
+      <c r="F8" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="3" t="s">
@@ -2433,101 +2419,83 @@
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="D9" s="31"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="95" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="96"/>
+      <c r="C10" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="D9" s="33"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="35"/>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="106" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="107"/>
-      <c r="C10" s="10" t="s">
+      <c r="D10" s="31"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="95" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="96"/>
+      <c r="C11" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="D10" s="33"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="35"/>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="106" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="107"/>
-      <c r="C11" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="D11" s="33"/>
+      <c r="D11" s="31"/>
       <c r="E11" s="11"/>
-      <c r="F11" s="34" t="s">
+      <c r="F11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="35"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="106" t="s">
+      <c r="A12" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="107"/>
+      <c r="B12" s="96"/>
       <c r="C12" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="33"/>
+      <c r="D12" s="31"/>
       <c r="E12" s="11"/>
-      <c r="F12" s="34" t="s">
+      <c r="F12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="35"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="106" t="s">
+      <c r="A13" s="95" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="107"/>
-      <c r="C13" s="86" t="s">
-        <v>64</v>
-      </c>
-      <c r="D13" s="33"/>
+      <c r="B13" s="96"/>
+      <c r="C13" s="76" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="31"/>
       <c r="E13" s="11"/>
-      <c r="F13" s="34" t="s">
+      <c r="F13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="35"/>
     </row>
     <row r="14" spans="1:11" ht="45" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="108" t="s">
-        <v>72</v>
-      </c>
-      <c r="D14" s="109"/>
-      <c r="E14" s="110"/>
-      <c r="F14" s="65"/>
-      <c r="G14" s="65"/>
-      <c r="H14" s="65"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
+      <c r="C14" s="97" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="98"/>
+      <c r="E14" s="99"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="56"/>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="3" t="s">
@@ -2535,23 +2503,17 @@
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="8"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-    </row>
-    <row r="16" spans="1:11" s="32" customFormat="1">
-      <c r="A16" s="62" t="s">
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="63"/>
-      <c r="C16" s="64" t="s">
+      <c r="B16" s="13"/>
+      <c r="C16" s="55" t="s">
         <v>27</v>
       </c>
       <c r="D16" t="s">
@@ -2559,16 +2521,16 @@
       </c>
       <c r="E16"/>
       <c r="F16"/>
-      <c r="G16" s="66"/>
-      <c r="H16" s="66"/>
+      <c r="G16"/>
+      <c r="H16"/>
       <c r="I16"/>
     </row>
-    <row r="17" spans="1:13" s="32" customFormat="1">
-      <c r="A17" s="62" t="s">
+    <row r="17" spans="1:12">
+      <c r="A17" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="63"/>
-      <c r="C17" s="64" t="s">
+      <c r="B17" s="13"/>
+      <c r="C17" s="55" t="s">
         <v>14</v>
       </c>
       <c r="D17" t="s">
@@ -2576,48 +2538,48 @@
       </c>
       <c r="E17"/>
       <c r="F17"/>
-      <c r="G17" s="66"/>
-      <c r="H17" s="66"/>
+      <c r="G17"/>
+      <c r="H17"/>
       <c r="I17"/>
     </row>
-    <row r="18" spans="1:13" s="32" customFormat="1">
-      <c r="A18" s="62" t="s">
+    <row r="18" spans="1:12">
+      <c r="A18" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="63"/>
-      <c r="C18" s="64"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="55"/>
       <c r="D18" t="s">
         <v>36</v>
       </c>
       <c r="E18"/>
       <c r="F18"/>
-      <c r="G18" s="66"/>
-      <c r="H18" s="66"/>
+      <c r="G18"/>
+      <c r="H18"/>
       <c r="I18"/>
     </row>
-    <row r="19" spans="1:13" s="32" customFormat="1">
-      <c r="A19" s="62" t="s">
+    <row r="19" spans="1:12">
+      <c r="A19" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="63"/>
-      <c r="C19" s="64" t="s">
+      <c r="B19" s="13"/>
+      <c r="C19" s="55" t="s">
         <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E19"/>
       <c r="F19"/>
-      <c r="G19" s="66"/>
-      <c r="H19" s="66"/>
+      <c r="G19"/>
+      <c r="H19"/>
       <c r="I19"/>
     </row>
-    <row r="20" spans="1:13" s="32" customFormat="1">
-      <c r="A20" s="62" t="s">
+    <row r="20" spans="1:12">
+      <c r="A20" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="63"/>
-      <c r="C20" s="64" t="s">
+      <c r="B20" s="13"/>
+      <c r="C20" s="55" t="s">
         <v>14</v>
       </c>
       <c r="D20" t="s">
@@ -2625,65 +2587,65 @@
       </c>
       <c r="E20"/>
       <c r="F20"/>
-      <c r="G20" s="66"/>
-      <c r="H20" s="66"/>
+      <c r="G20"/>
+      <c r="H20"/>
       <c r="I20"/>
     </row>
-    <row r="21" spans="1:13" s="32" customFormat="1">
-      <c r="A21" s="62" t="s">
-        <v>77</v>
-      </c>
-      <c r="B21" s="63"/>
-      <c r="C21" s="64" t="s">
+    <row r="21" spans="1:12">
+      <c r="A21" s="54" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="13"/>
+      <c r="C21" s="55" t="s">
         <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E21"/>
       <c r="F21"/>
-      <c r="G21" s="66"/>
-      <c r="H21" s="66"/>
+      <c r="G21"/>
+      <c r="H21"/>
       <c r="I21"/>
     </row>
-    <row r="22" spans="1:13" s="32" customFormat="1">
-      <c r="A22" s="98" t="s">
-        <v>78</v>
-      </c>
-      <c r="B22" s="99"/>
-      <c r="C22" s="64" t="s">
+    <row r="22" spans="1:12">
+      <c r="A22" s="100" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="101"/>
+      <c r="C22" s="55" t="s">
         <v>14</v>
       </c>
       <c r="D22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E22"/>
       <c r="F22"/>
-      <c r="G22" s="66"/>
-      <c r="H22" s="66"/>
+      <c r="G22"/>
+      <c r="H22"/>
       <c r="I22"/>
     </row>
-    <row r="23" spans="1:13" s="32" customFormat="1">
-      <c r="A23" s="62" t="s">
+    <row r="23" spans="1:12">
+      <c r="A23" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="63"/>
-      <c r="C23" s="64" t="s">
+      <c r="B23" s="13"/>
+      <c r="C23" s="55" t="s">
         <v>14</v>
       </c>
       <c r="D23"/>
       <c r="E23"/>
       <c r="F23"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="66"/>
+      <c r="G23"/>
+      <c r="H23"/>
       <c r="I23"/>
     </row>
-    <row r="24" spans="1:13" s="32" customFormat="1">
-      <c r="A24" s="98" t="s">
+    <row r="24" spans="1:12">
+      <c r="A24" s="100" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="99"/>
-      <c r="C24" s="64" t="s">
+      <c r="B24" s="101"/>
+      <c r="C24" s="55" t="s">
         <v>14</v>
       </c>
       <c r="D24" t="s">
@@ -2691,1314 +2653,1205 @@
       </c>
       <c r="E24"/>
       <c r="F24"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="66"/>
+      <c r="G24"/>
+      <c r="H24"/>
       <c r="I24"/>
     </row>
-    <row r="25" spans="1:13" s="32" customFormat="1">
-      <c r="A25" s="98" t="s">
-        <v>65</v>
-      </c>
-      <c r="B25" s="99"/>
-      <c r="C25" s="64" t="s">
+    <row r="25" spans="1:12">
+      <c r="A25" s="100" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="101"/>
+      <c r="C25" s="55" t="s">
         <v>14</v>
       </c>
       <c r="D25"/>
       <c r="E25"/>
       <c r="F25"/>
-      <c r="G25" s="66"/>
-      <c r="H25" s="66"/>
+      <c r="G25"/>
+      <c r="H25"/>
       <c r="I25"/>
     </row>
-    <row r="26" spans="1:13" s="37" customFormat="1">
-      <c r="A26" s="34"/>
-      <c r="B26" s="36"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="34"/>
-      <c r="J26" s="34"/>
-      <c r="K26" s="34"/>
-    </row>
-    <row r="27" spans="1:13">
-      <c r="A27" s="30" t="s">
+    <row r="26" spans="1:12">
+      <c r="B26"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="71"/>
+      <c r="F27" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="72"/>
+      <c r="F28" s="57"/>
+      <c r="G28" s="57"/>
+      <c r="H28" s="57"/>
+      <c r="I28" s="57"/>
+      <c r="K28" s="37"/>
+      <c r="L28" s="37"/>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="43">
+        <v>1</v>
+      </c>
+      <c r="B29" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="58"/>
+      <c r="G29" s="58"/>
+      <c r="H29" s="58"/>
+      <c r="J29"/>
+      <c r="K29"/>
+      <c r="L29"/>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="43">
+        <v>2</v>
+      </c>
+      <c r="B30" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="C30" s="34"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="58"/>
+      <c r="G30" s="58"/>
+      <c r="H30" s="58"/>
+      <c r="J30"/>
+      <c r="K30"/>
+      <c r="L30"/>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="44"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="58"/>
+      <c r="H31" s="58"/>
+      <c r="J31"/>
+      <c r="K31"/>
+      <c r="L31"/>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32"/>
+      <c r="B32"/>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="F32"/>
+      <c r="G32"/>
+      <c r="H32"/>
+      <c r="I32"/>
+      <c r="J32"/>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="30"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="71"/>
+      <c r="F33" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="36"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="72"/>
+      <c r="F34" s="57"/>
+      <c r="G34" s="57"/>
+      <c r="H34" s="57"/>
+      <c r="I34" s="57"/>
+      <c r="K34" s="37"/>
+      <c r="L34" s="37"/>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="43">
+        <v>1</v>
+      </c>
+      <c r="B35" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="58"/>
+      <c r="G35" s="58"/>
+      <c r="H35" s="58"/>
+      <c r="J35"/>
+      <c r="K35"/>
+      <c r="L35"/>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="43">
+        <v>2</v>
+      </c>
+      <c r="B36" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" s="34"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="58"/>
+      <c r="G36" s="58"/>
+      <c r="H36" s="58"/>
+      <c r="J36"/>
+      <c r="K36"/>
+      <c r="L36"/>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="44"/>
+      <c r="B37" s="40"/>
+      <c r="C37" s="41"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="58"/>
+      <c r="G37" s="58"/>
+      <c r="H37" s="58"/>
+      <c r="J37"/>
+      <c r="K37"/>
+      <c r="L37"/>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" s="73"/>
+      <c r="B38" s="74"/>
+      <c r="C38" s="75"/>
+      <c r="D38" s="75"/>
+      <c r="E38" s="75"/>
+      <c r="F38" s="58"/>
+      <c r="G38" s="58"/>
+      <c r="H38" s="58"/>
+      <c r="J38"/>
+      <c r="K38"/>
+      <c r="L38"/>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="81"/>
-      <c r="F27" s="44" t="s">
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="71"/>
+      <c r="F39" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G27" s="44"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="44"/>
-      <c r="J27" s="43"/>
-      <c r="K27" s="43"/>
-      <c r="L27" s="43"/>
-      <c r="M27" s="43"/>
-    </row>
-    <row r="28" spans="1:13">
-      <c r="A28" s="47" t="s">
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="42" t="s">
+      <c r="B40" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="42"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="82"/>
-      <c r="F28" s="67"/>
-      <c r="G28" s="67"/>
-      <c r="H28" s="67"/>
-      <c r="I28" s="67"/>
-      <c r="J28" s="44"/>
-      <c r="K28" s="45"/>
-      <c r="L28" s="45"/>
-      <c r="M28" s="35"/>
-    </row>
-    <row r="29" spans="1:13">
-      <c r="A29" s="51">
-        <v>1</v>
-      </c>
-      <c r="B29" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="68"/>
-      <c r="G29" s="68"/>
-      <c r="H29" s="68"/>
-      <c r="I29" s="34"/>
-      <c r="J29" s="36"/>
-      <c r="K29" s="36"/>
-      <c r="L29" s="36"/>
-      <c r="M29" s="35"/>
-    </row>
-    <row r="30" spans="1:13">
-      <c r="A30" s="51">
-        <v>2</v>
-      </c>
-      <c r="B30" s="46" t="s">
-        <v>106</v>
-      </c>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="68"/>
-      <c r="G30" s="68"/>
-      <c r="H30" s="68"/>
-      <c r="I30" s="34"/>
-      <c r="J30" s="36"/>
-      <c r="K30" s="36"/>
-      <c r="L30" s="36"/>
-      <c r="M30" s="35"/>
-    </row>
-    <row r="31" spans="1:13">
-      <c r="A31" s="52"/>
-      <c r="B31" s="48"/>
-      <c r="C31" s="49"/>
-      <c r="D31" s="49"/>
-      <c r="E31" s="50"/>
-      <c r="F31" s="68"/>
-      <c r="G31" s="68"/>
-      <c r="H31" s="68"/>
-      <c r="I31" s="34"/>
-      <c r="J31" s="36"/>
-      <c r="K31" s="36"/>
-      <c r="L31" s="36"/>
-      <c r="M31" s="35"/>
-    </row>
-    <row r="32" spans="1:13">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="13"/>
-    </row>
-    <row r="33" spans="1:13">
-      <c r="A33" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="81"/>
-      <c r="F33" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="G33" s="44"/>
-      <c r="H33" s="44"/>
-      <c r="I33" s="44"/>
-      <c r="J33" s="43"/>
-      <c r="K33" s="43"/>
-      <c r="L33" s="43"/>
-      <c r="M33" s="43"/>
-    </row>
-    <row r="34" spans="1:13">
-      <c r="A34" s="47" t="s">
+      <c r="C40" s="36"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="72"/>
+      <c r="F40" s="57"/>
+      <c r="G40" s="57"/>
+      <c r="H40" s="57"/>
+      <c r="I40" s="57"/>
+      <c r="K40" s="37"/>
+      <c r="L40" s="37"/>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" s="43"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="58"/>
+      <c r="G41" s="58"/>
+      <c r="H41" s="58"/>
+      <c r="J41"/>
+      <c r="K41"/>
+      <c r="L41"/>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="43"/>
+      <c r="B42" s="38"/>
+      <c r="C42" s="34"/>
+      <c r="D42" s="34"/>
+      <c r="E42" s="35"/>
+      <c r="F42" s="58"/>
+      <c r="G42" s="58"/>
+      <c r="H42" s="58"/>
+      <c r="J42"/>
+      <c r="K42"/>
+      <c r="L42"/>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" s="44"/>
+      <c r="B43" s="40"/>
+      <c r="C43" s="41"/>
+      <c r="D43" s="41"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="58"/>
+      <c r="G43" s="58"/>
+      <c r="H43" s="58"/>
+      <c r="J43"/>
+      <c r="K43"/>
+      <c r="L43"/>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44"/>
+      <c r="B44"/>
+      <c r="C44"/>
+      <c r="D44"/>
+      <c r="E44"/>
+      <c r="F44"/>
+      <c r="G44"/>
+      <c r="H44"/>
+      <c r="I44"/>
+      <c r="J44"/>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B45" s="30"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="71"/>
+      <c r="F45" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="C34" s="42"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="82"/>
-      <c r="F34" s="67"/>
-      <c r="G34" s="67"/>
-      <c r="H34" s="67"/>
-      <c r="I34" s="67"/>
-      <c r="J34" s="44"/>
-      <c r="K34" s="45"/>
-      <c r="L34" s="45"/>
-      <c r="M34" s="35"/>
-    </row>
-    <row r="35" spans="1:13">
-      <c r="A35" s="51">
-        <v>1</v>
-      </c>
-      <c r="B35" s="46" t="s">
-        <v>61</v>
-      </c>
-      <c r="C35" s="38"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="39"/>
-      <c r="F35" s="68"/>
-      <c r="G35" s="68"/>
-      <c r="H35" s="68"/>
-      <c r="I35" s="34"/>
-      <c r="J35" s="36"/>
-      <c r="K35" s="36"/>
-      <c r="L35" s="36"/>
-      <c r="M35" s="35"/>
-    </row>
-    <row r="36" spans="1:13">
-      <c r="A36" s="51">
-        <v>2</v>
-      </c>
-      <c r="B36" s="46" t="s">
-        <v>62</v>
-      </c>
-      <c r="C36" s="40"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="68"/>
-      <c r="G36" s="68"/>
-      <c r="H36" s="68"/>
-      <c r="I36" s="34"/>
-      <c r="J36" s="36"/>
-      <c r="K36" s="36"/>
-      <c r="L36" s="36"/>
-      <c r="M36" s="35"/>
-    </row>
-    <row r="37" spans="1:13">
-      <c r="A37" s="52"/>
-      <c r="B37" s="48"/>
-      <c r="C37" s="49"/>
-      <c r="D37" s="49"/>
-      <c r="E37" s="50"/>
-      <c r="F37" s="68"/>
-      <c r="G37" s="68"/>
-      <c r="H37" s="68"/>
-      <c r="I37" s="34"/>
-      <c r="J37" s="36"/>
-      <c r="K37" s="36"/>
-      <c r="L37" s="36"/>
-      <c r="M37" s="35"/>
-    </row>
-    <row r="38" spans="1:13">
-      <c r="A38" s="83"/>
-      <c r="B38" s="84"/>
-      <c r="C38" s="85"/>
-      <c r="D38" s="85"/>
-      <c r="E38" s="85"/>
-      <c r="F38" s="68"/>
-      <c r="G38" s="68"/>
-      <c r="H38" s="68"/>
-      <c r="I38" s="34"/>
-      <c r="J38" s="36"/>
-      <c r="K38" s="36"/>
-      <c r="L38" s="36"/>
-      <c r="M38" s="35"/>
-    </row>
-    <row r="39" spans="1:13">
-      <c r="A39" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="B39" s="31"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="81"/>
-      <c r="F39" s="44" t="s">
+      <c r="B46" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="C46" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="D46" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="E46" s="72"/>
+      <c r="F46" s="57"/>
+      <c r="G46" s="57"/>
+      <c r="H46" s="57"/>
+      <c r="I46" s="57"/>
+      <c r="K46" s="37"/>
+      <c r="L46" s="37"/>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47" s="43"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="85"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="33"/>
+      <c r="F47" s="58"/>
+      <c r="G47" s="58"/>
+      <c r="H47" s="58"/>
+      <c r="J47"/>
+      <c r="K47"/>
+      <c r="L47"/>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48" s="43"/>
+      <c r="B48" s="38"/>
+      <c r="C48" s="86"/>
+      <c r="D48" s="34"/>
+      <c r="E48" s="35"/>
+      <c r="F48" s="58"/>
+      <c r="G48" s="58"/>
+      <c r="H48" s="58"/>
+      <c r="J48"/>
+      <c r="K48"/>
+      <c r="L48"/>
+    </row>
+    <row r="49" spans="1:13">
+      <c r="A49" s="44"/>
+      <c r="B49" s="40"/>
+      <c r="C49" s="87"/>
+      <c r="D49" s="41"/>
+      <c r="E49" s="42"/>
+      <c r="F49" s="58"/>
+      <c r="G49" s="58"/>
+      <c r="H49" s="58"/>
+      <c r="J49"/>
+      <c r="K49"/>
+      <c r="L49"/>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50" s="73"/>
+      <c r="B50" s="74"/>
+      <c r="C50" s="75"/>
+      <c r="D50" s="75"/>
+      <c r="E50" s="75"/>
+      <c r="F50" s="58"/>
+      <c r="G50" s="58"/>
+      <c r="H50" s="58"/>
+      <c r="J50"/>
+      <c r="K50"/>
+      <c r="L50"/>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="B51" s="30"/>
+      <c r="C51" s="30"/>
+      <c r="D51" s="30"/>
+      <c r="E51" s="71"/>
+      <c r="F51" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G39" s="44"/>
-      <c r="H39" s="44"/>
-      <c r="I39" s="44"/>
-      <c r="J39" s="43"/>
-      <c r="K39" s="43"/>
-      <c r="L39" s="43"/>
-      <c r="M39" s="43"/>
-    </row>
-    <row r="40" spans="1:13">
-      <c r="A40" s="47" t="s">
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="42" t="s">
+      <c r="B52" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="42"/>
-      <c r="D40" s="42"/>
-      <c r="E40" s="82"/>
-      <c r="F40" s="67"/>
-      <c r="G40" s="67"/>
-      <c r="H40" s="67"/>
-      <c r="I40" s="67"/>
-      <c r="J40" s="44"/>
-      <c r="K40" s="45"/>
-      <c r="L40" s="45"/>
-      <c r="M40" s="35"/>
-    </row>
-    <row r="41" spans="1:13">
-      <c r="A41" s="51"/>
-      <c r="B41" s="46"/>
-      <c r="C41" s="38"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="39"/>
-      <c r="F41" s="68"/>
-      <c r="G41" s="68"/>
-      <c r="H41" s="68"/>
-      <c r="I41" s="34"/>
-      <c r="J41" s="36"/>
-      <c r="K41" s="36"/>
-      <c r="L41" s="36"/>
-      <c r="M41" s="35"/>
-    </row>
-    <row r="42" spans="1:13">
-      <c r="A42" s="51"/>
-      <c r="B42" s="46"/>
-      <c r="C42" s="40"/>
-      <c r="D42" s="40"/>
-      <c r="E42" s="41"/>
-      <c r="F42" s="68"/>
-      <c r="G42" s="68"/>
-      <c r="H42" s="68"/>
-      <c r="I42" s="34"/>
-      <c r="J42" s="36"/>
-      <c r="K42" s="36"/>
-      <c r="L42" s="36"/>
-      <c r="M42" s="35"/>
-    </row>
-    <row r="43" spans="1:13">
-      <c r="A43" s="52"/>
-      <c r="B43" s="48"/>
-      <c r="C43" s="49"/>
-      <c r="D43" s="49"/>
-      <c r="E43" s="50"/>
-      <c r="F43" s="68"/>
-      <c r="G43" s="68"/>
-      <c r="H43" s="68"/>
-      <c r="I43" s="34"/>
-      <c r="J43" s="36"/>
-      <c r="K43" s="36"/>
-      <c r="L43" s="36"/>
-      <c r="M43" s="35"/>
-    </row>
-    <row r="44" spans="1:13">
-      <c r="A44" s="13"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
-      <c r="I44" s="13"/>
-      <c r="J44" s="13"/>
-    </row>
-    <row r="45" spans="1:13">
-      <c r="A45" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="B45" s="31"/>
-      <c r="C45" s="31"/>
-      <c r="D45" s="31"/>
-      <c r="E45" s="81"/>
-      <c r="F45" s="44" t="s">
-        <v>83</v>
-      </c>
-      <c r="G45" s="44"/>
-      <c r="H45" s="44"/>
-      <c r="I45" s="44"/>
-      <c r="J45" s="43"/>
-      <c r="K45" s="43"/>
-      <c r="L45" s="43"/>
-      <c r="M45" s="43"/>
-    </row>
-    <row r="46" spans="1:13">
-      <c r="A46" s="47" t="s">
-        <v>7</v>
-      </c>
-      <c r="B46" s="42" t="s">
-        <v>81</v>
-      </c>
-      <c r="C46" s="47" t="s">
-        <v>110</v>
-      </c>
-      <c r="D46" s="42" t="s">
-        <v>82</v>
-      </c>
-      <c r="E46" s="82"/>
-      <c r="F46" s="67"/>
-      <c r="G46" s="67"/>
-      <c r="H46" s="67"/>
-      <c r="I46" s="67"/>
-      <c r="J46" s="44"/>
-      <c r="K46" s="45"/>
-      <c r="L46" s="45"/>
-      <c r="M46" s="35"/>
-    </row>
-    <row r="47" spans="1:13">
-      <c r="A47" s="51"/>
-      <c r="B47" s="46"/>
-      <c r="C47" s="95"/>
-      <c r="D47" s="38"/>
-      <c r="E47" s="39"/>
-      <c r="F47" s="68"/>
-      <c r="G47" s="68"/>
-      <c r="H47" s="68"/>
-      <c r="I47" s="34"/>
-      <c r="J47" s="36"/>
-      <c r="K47" s="36"/>
-      <c r="L47" s="36"/>
-      <c r="M47" s="35"/>
-    </row>
-    <row r="48" spans="1:13">
-      <c r="A48" s="51"/>
-      <c r="B48" s="46"/>
-      <c r="C48" s="96"/>
-      <c r="D48" s="40"/>
-      <c r="E48" s="41"/>
-      <c r="F48" s="68"/>
-      <c r="G48" s="68"/>
-      <c r="H48" s="68"/>
-      <c r="I48" s="34"/>
-      <c r="J48" s="36"/>
-      <c r="K48" s="36"/>
-      <c r="L48" s="36"/>
-      <c r="M48" s="35"/>
-    </row>
-    <row r="49" spans="1:13">
-      <c r="A49" s="52"/>
-      <c r="B49" s="48"/>
-      <c r="C49" s="97"/>
-      <c r="D49" s="49"/>
-      <c r="E49" s="50"/>
-      <c r="F49" s="68"/>
-      <c r="G49" s="68"/>
-      <c r="H49" s="68"/>
-      <c r="I49" s="34"/>
-      <c r="J49" s="36"/>
-      <c r="K49" s="36"/>
-      <c r="L49" s="36"/>
-      <c r="M49" s="35"/>
-    </row>
-    <row r="50" spans="1:13">
-      <c r="A50" s="83"/>
-      <c r="B50" s="84"/>
-      <c r="C50" s="85"/>
-      <c r="D50" s="85"/>
-      <c r="E50" s="85"/>
-      <c r="F50" s="68"/>
-      <c r="G50" s="68"/>
-      <c r="H50" s="68"/>
-      <c r="I50" s="34"/>
-      <c r="J50" s="36"/>
-      <c r="K50" s="36"/>
-      <c r="L50" s="36"/>
-      <c r="M50" s="35"/>
-    </row>
-    <row r="51" spans="1:13">
-      <c r="A51" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="B51" s="31"/>
-      <c r="C51" s="31"/>
-      <c r="D51" s="31"/>
-      <c r="E51" s="81"/>
-      <c r="F51" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="G51" s="44"/>
-      <c r="H51" s="44"/>
-      <c r="I51" s="44"/>
-      <c r="J51" s="43"/>
-      <c r="K51" s="43"/>
-      <c r="L51" s="43"/>
-      <c r="M51" s="43"/>
-    </row>
-    <row r="52" spans="1:13">
-      <c r="A52" s="47" t="s">
-        <v>7</v>
-      </c>
-      <c r="B52" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="C52" s="42"/>
-      <c r="D52" s="42"/>
-      <c r="E52" s="82"/>
-      <c r="F52" s="67" t="s">
-        <v>104</v>
-      </c>
-      <c r="G52" s="67"/>
-      <c r="H52" s="67"/>
-      <c r="I52" s="67"/>
-      <c r="J52" s="44"/>
-      <c r="K52" s="45"/>
-      <c r="L52" s="45"/>
-      <c r="M52" s="35"/>
+      <c r="C52" s="36"/>
+      <c r="D52" s="36"/>
+      <c r="E52" s="72"/>
+      <c r="F52" s="57" t="s">
+        <v>103</v>
+      </c>
+      <c r="G52" s="57"/>
+      <c r="H52" s="57"/>
+      <c r="I52" s="57"/>
+      <c r="K52" s="37"/>
+      <c r="L52" s="37"/>
     </row>
     <row r="53" spans="1:13">
-      <c r="A53" s="51"/>
-      <c r="B53" s="46"/>
-      <c r="C53" s="38"/>
-      <c r="D53" s="38"/>
-      <c r="E53" s="39"/>
-      <c r="F53" s="68"/>
-      <c r="G53" s="68"/>
-      <c r="H53" s="68"/>
-      <c r="I53" s="34"/>
-      <c r="J53" s="36"/>
-      <c r="K53" s="36"/>
-      <c r="L53" s="36"/>
-      <c r="M53" s="35"/>
+      <c r="A53" s="43"/>
+      <c r="B53" s="38"/>
+      <c r="C53" s="32"/>
+      <c r="D53" s="32"/>
+      <c r="E53" s="33"/>
+      <c r="F53" s="58"/>
+      <c r="G53" s="58"/>
+      <c r="H53" s="58"/>
+      <c r="J53"/>
+      <c r="K53"/>
+      <c r="L53"/>
     </row>
     <row r="54" spans="1:13">
-      <c r="A54" s="51"/>
-      <c r="B54" s="46"/>
-      <c r="C54" s="40"/>
-      <c r="D54" s="40"/>
-      <c r="E54" s="41"/>
-      <c r="F54" s="68"/>
-      <c r="G54" s="68"/>
-      <c r="H54" s="68"/>
-      <c r="I54" s="34"/>
-      <c r="J54" s="36"/>
-      <c r="K54" s="36"/>
-      <c r="L54" s="36"/>
-      <c r="M54" s="35"/>
+      <c r="A54" s="43"/>
+      <c r="B54" s="38"/>
+      <c r="C54" s="34"/>
+      <c r="D54" s="34"/>
+      <c r="E54" s="35"/>
+      <c r="F54" s="58"/>
+      <c r="G54" s="58"/>
+      <c r="H54" s="58"/>
+      <c r="J54"/>
+      <c r="K54"/>
+      <c r="L54"/>
     </row>
     <row r="55" spans="1:13">
-      <c r="A55" s="52"/>
-      <c r="B55" s="48"/>
-      <c r="C55" s="49"/>
-      <c r="D55" s="49"/>
-      <c r="E55" s="50"/>
-      <c r="F55" s="68"/>
-      <c r="G55" s="68"/>
-      <c r="H55" s="68"/>
-      <c r="I55" s="34"/>
-      <c r="J55" s="36"/>
-      <c r="K55" s="36"/>
-      <c r="L55" s="36"/>
-      <c r="M55" s="35"/>
+      <c r="A55" s="44"/>
+      <c r="B55" s="40"/>
+      <c r="C55" s="41"/>
+      <c r="D55" s="41"/>
+      <c r="E55" s="42"/>
+      <c r="F55" s="58"/>
+      <c r="G55" s="58"/>
+      <c r="H55" s="58"/>
+      <c r="J55"/>
+      <c r="K55"/>
+      <c r="L55"/>
     </row>
     <row r="56" spans="1:13">
-      <c r="A56" s="13"/>
-      <c r="B56" s="13"/>
-      <c r="C56" s="13"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="13"/>
-      <c r="F56" s="13"/>
-      <c r="G56" s="13"/>
-      <c r="H56" s="13"/>
-      <c r="I56" s="13"/>
-      <c r="J56" s="13"/>
+      <c r="A56"/>
+      <c r="B56"/>
+      <c r="C56"/>
+      <c r="D56"/>
+      <c r="E56"/>
+      <c r="F56"/>
+      <c r="G56"/>
+      <c r="H56"/>
+      <c r="I56"/>
+      <c r="J56"/>
     </row>
     <row r="57" spans="1:13">
-      <c r="A57" s="13"/>
-      <c r="B57" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="C57" s="13"/>
-      <c r="D57" s="13"/>
-      <c r="E57" s="13"/>
-      <c r="F57" s="13"/>
-      <c r="G57" s="13"/>
-      <c r="H57" s="13"/>
-      <c r="I57" s="13"/>
-      <c r="J57" s="13"/>
+      <c r="A57"/>
+      <c r="B57" t="s">
+        <v>78</v>
+      </c>
+      <c r="C57"/>
+      <c r="D57"/>
+      <c r="E57"/>
+      <c r="F57"/>
+      <c r="G57"/>
+      <c r="H57"/>
+      <c r="I57"/>
+      <c r="J57"/>
     </row>
     <row r="58" spans="1:13">
       <c r="A58" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B58" s="14"/>
-      <c r="C58" s="14"/>
-      <c r="D58" s="14"/>
-      <c r="E58" s="14"/>
-      <c r="F58" s="14"/>
-      <c r="G58" s="14"/>
-      <c r="H58" s="14"/>
-      <c r="I58" s="14"/>
-      <c r="J58" s="14"/>
-      <c r="K58" s="14"/>
+        <v>97</v>
+      </c>
+      <c r="B58" s="13"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="13"/>
+      <c r="I58" s="13"/>
+      <c r="J58" s="13"/>
+      <c r="K58" s="13"/>
       <c r="L58" s="6"/>
-      <c r="M58" s="15"/>
+      <c r="M58" s="14"/>
     </row>
     <row r="59" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A59" s="101" t="s">
+      <c r="A59" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="B59" s="101" t="s">
+      <c r="B59" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="C59" s="100" t="s">
+      <c r="C59" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="D59" s="100" t="s">
+      <c r="D59" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="E59" s="100" t="s">
+      <c r="E59" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="F59" s="104" t="s">
+      <c r="F59" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="G59" s="104" t="s">
+      <c r="G59" s="92" t="s">
         <v>16</v>
       </c>
       <c r="H59" s="102" t="s">
-        <v>107</v>
-      </c>
-      <c r="I59" s="100" t="s">
+        <v>106</v>
+      </c>
+      <c r="I59" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="J59" s="100"/>
-      <c r="K59" s="16"/>
-      <c r="L59" s="17"/>
+      <c r="J59" s="91"/>
+      <c r="K59" s="15"/>
+      <c r="L59" s="16"/>
       <c r="M59" s="9"/>
     </row>
     <row r="60" spans="1:13">
-      <c r="A60" s="101"/>
-      <c r="B60" s="101"/>
-      <c r="C60" s="100"/>
-      <c r="D60" s="100"/>
-      <c r="E60" s="100"/>
-      <c r="F60" s="105"/>
-      <c r="G60" s="105"/>
+      <c r="A60" s="94"/>
+      <c r="B60" s="94"/>
+      <c r="C60" s="91"/>
+      <c r="D60" s="91"/>
+      <c r="E60" s="91"/>
+      <c r="F60" s="93"/>
+      <c r="G60" s="93"/>
       <c r="H60" s="103"/>
-      <c r="I60" s="100"/>
-      <c r="J60" s="100"/>
-      <c r="K60" s="18"/>
-      <c r="L60" s="29"/>
-      <c r="M60" s="15"/>
+      <c r="I60" s="91"/>
+      <c r="J60" s="91"/>
+      <c r="K60" s="17"/>
+      <c r="L60" s="28"/>
+      <c r="M60" s="14"/>
     </row>
     <row r="61" spans="1:13">
-      <c r="A61" s="19">
+      <c r="A61" s="18">
         <v>1</v>
       </c>
-      <c r="B61" s="71" t="s">
+      <c r="B61" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="C61" s="78" t="s">
+      <c r="C61" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="D61" s="20"/>
-      <c r="E61" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="F61" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="G61" s="69"/>
-      <c r="H61" s="69"/>
-      <c r="I61" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="J61" s="21"/>
-      <c r="K61" s="21"/>
-      <c r="L61" s="28"/>
-      <c r="M61" s="15"/>
+      <c r="D61" s="19"/>
+      <c r="E61" s="19"/>
+      <c r="F61" s="19"/>
+      <c r="G61" s="59"/>
+      <c r="H61" s="59"/>
+      <c r="I61" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="J61" s="20"/>
+      <c r="K61" s="20"/>
+      <c r="L61" s="27"/>
+      <c r="M61" s="14"/>
     </row>
     <row r="62" spans="1:13">
-      <c r="A62" s="19">
+      <c r="A62" s="18">
         <f>A61+1</f>
         <v>2</v>
       </c>
-      <c r="B62" s="71" t="s">
+      <c r="B62" s="61" t="s">
+        <v>49</v>
+      </c>
+      <c r="C62" s="68" t="s">
         <v>50</v>
       </c>
-      <c r="C62" s="78" t="s">
+      <c r="D62" s="19"/>
+      <c r="E62" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="F62" s="19"/>
+      <c r="G62" s="59"/>
+      <c r="H62" s="59"/>
+      <c r="I62" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="D62" s="20"/>
-      <c r="E62" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="F62" s="20"/>
-      <c r="G62" s="69"/>
-      <c r="H62" s="69"/>
-      <c r="I62" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="J62" s="21"/>
-      <c r="K62" s="21"/>
-      <c r="L62" s="28"/>
-      <c r="M62" s="15"/>
+      <c r="J62" s="20"/>
+      <c r="K62" s="20"/>
+      <c r="L62" s="27"/>
+      <c r="M62" s="14"/>
     </row>
     <row r="63" spans="1:13">
-      <c r="A63" s="19">
+      <c r="A63" s="18">
         <f t="shared" ref="A63:A77" si="0">A62+1</f>
         <v>3</v>
       </c>
-      <c r="B63" s="72" t="s">
+      <c r="B63" s="62" t="s">
+        <v>52</v>
+      </c>
+      <c r="C63" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="C63" s="79" t="s">
+      <c r="D63" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="D63" s="20" t="s">
+      <c r="E63" s="19"/>
+      <c r="F63" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G63" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="H63" s="59"/>
+      <c r="I63" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="E63" s="20"/>
-      <c r="F63" s="20"/>
-      <c r="G63" s="69" t="s">
-        <v>14</v>
-      </c>
-      <c r="H63" s="69"/>
-      <c r="I63" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="J63" s="21"/>
-      <c r="K63" s="21"/>
-      <c r="L63" s="22"/>
-      <c r="M63" s="15"/>
+      <c r="J63" s="20"/>
+      <c r="K63" s="20"/>
+      <c r="L63" s="21"/>
+      <c r="M63" s="14"/>
     </row>
     <row r="64" spans="1:13">
-      <c r="A64" s="19">
+      <c r="A64" s="18">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B64" s="73" t="s">
+      <c r="B64" s="63" t="s">
+        <v>58</v>
+      </c>
+      <c r="C64" s="70" t="s">
+        <v>54</v>
+      </c>
+      <c r="D64" s="19"/>
+      <c r="E64" s="19"/>
+      <c r="F64" s="19"/>
+      <c r="G64" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="H64" s="59"/>
+      <c r="I64" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="C64" s="80" t="s">
-        <v>55</v>
-      </c>
-      <c r="D64" s="20"/>
-      <c r="E64" s="20"/>
-      <c r="F64" s="20"/>
-      <c r="G64" s="69" t="s">
-        <v>14</v>
-      </c>
-      <c r="H64" s="69"/>
-      <c r="I64" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="J64" s="21"/>
-      <c r="K64" s="21"/>
-      <c r="L64" s="22"/>
-      <c r="M64" s="15"/>
+      <c r="J64" s="20"/>
+      <c r="K64" s="20"/>
+      <c r="L64" s="21"/>
+      <c r="M64" s="14"/>
     </row>
     <row r="65" spans="1:13">
-      <c r="A65" s="19">
+      <c r="A65" s="18">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B65" s="73" t="s">
+      <c r="B65" s="63" t="s">
+        <v>107</v>
+      </c>
+      <c r="C65" s="70" t="s">
+        <v>48</v>
+      </c>
+      <c r="D65" s="19"/>
+      <c r="E65" s="19"/>
+      <c r="F65" s="19"/>
+      <c r="G65" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="H65" s="59" t="s">
+        <v>107</v>
+      </c>
+      <c r="I65" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="C65" s="80" t="s">
-        <v>48</v>
-      </c>
-      <c r="D65" s="20"/>
-      <c r="E65" s="20"/>
-      <c r="F65" s="20"/>
-      <c r="G65" s="69" t="s">
-        <v>14</v>
-      </c>
-      <c r="H65" s="69" t="s">
-        <v>108</v>
-      </c>
-      <c r="I65" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="J65" s="21"/>
-      <c r="K65" s="21"/>
-      <c r="L65" s="22"/>
-      <c r="M65" s="15"/>
+      <c r="J65" s="20"/>
+      <c r="K65" s="20"/>
+      <c r="L65" s="21"/>
+      <c r="M65" s="14"/>
     </row>
     <row r="66" spans="1:13">
-      <c r="A66" s="19">
+      <c r="A66" s="18">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B66" s="73"/>
-      <c r="C66" s="80"/>
-      <c r="D66" s="74"/>
-      <c r="E66" s="74"/>
-      <c r="F66" s="74"/>
-      <c r="G66" s="75"/>
-      <c r="H66" s="75"/>
-      <c r="I66" s="74"/>
-      <c r="J66" s="76"/>
-      <c r="K66" s="76"/>
-      <c r="L66" s="77"/>
-      <c r="M66" s="15"/>
+      <c r="B66" s="63" t="s">
+        <v>119</v>
+      </c>
+      <c r="C66" s="70" t="s">
+        <v>48</v>
+      </c>
+      <c r="D66" s="64"/>
+      <c r="E66" s="64" t="s">
+        <v>121</v>
+      </c>
+      <c r="F66" s="64"/>
+      <c r="G66" s="65" t="s">
+        <v>14</v>
+      </c>
+      <c r="H66" s="65" t="s">
+        <v>120</v>
+      </c>
+      <c r="I66" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="J66" s="66"/>
+      <c r="K66" s="66"/>
+      <c r="L66" s="67"/>
+      <c r="M66" s="14"/>
     </row>
     <row r="67" spans="1:13">
-      <c r="A67" s="19">
+      <c r="A67" s="18">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B67" s="73"/>
-      <c r="C67" s="80"/>
-      <c r="D67" s="20"/>
-      <c r="E67" s="20"/>
-      <c r="F67" s="20"/>
-      <c r="G67" s="69"/>
-      <c r="H67" s="69"/>
-      <c r="I67" s="20"/>
-      <c r="J67" s="21"/>
-      <c r="K67" s="21"/>
-      <c r="L67" s="22"/>
-      <c r="M67" s="15"/>
+      <c r="B67" s="63"/>
+      <c r="C67" s="70"/>
+      <c r="D67" s="19"/>
+      <c r="E67" s="19"/>
+      <c r="F67" s="19"/>
+      <c r="G67" s="59"/>
+      <c r="H67" s="59"/>
+      <c r="I67" s="19"/>
+      <c r="J67" s="20"/>
+      <c r="K67" s="20"/>
+      <c r="L67" s="21"/>
+      <c r="M67" s="14"/>
     </row>
     <row r="68" spans="1:13">
-      <c r="A68" s="19">
+      <c r="A68" s="18">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B68" s="73"/>
-      <c r="C68" s="80"/>
-      <c r="D68" s="74"/>
-      <c r="E68" s="74"/>
-      <c r="F68" s="74"/>
-      <c r="G68" s="75"/>
-      <c r="H68" s="75"/>
-      <c r="I68" s="74"/>
-      <c r="J68" s="76"/>
-      <c r="K68" s="76"/>
-      <c r="L68" s="77"/>
-      <c r="M68" s="15"/>
+      <c r="B68" s="63"/>
+      <c r="C68" s="70"/>
+      <c r="D68" s="64"/>
+      <c r="E68" s="64"/>
+      <c r="F68" s="64"/>
+      <c r="G68" s="65"/>
+      <c r="H68" s="65"/>
+      <c r="I68" s="64"/>
+      <c r="J68" s="66"/>
+      <c r="K68" s="66"/>
+      <c r="L68" s="67"/>
+      <c r="M68" s="14"/>
     </row>
     <row r="69" spans="1:13">
-      <c r="A69" s="19">
+      <c r="A69" s="18">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B69" s="73"/>
-      <c r="C69" s="80"/>
-      <c r="D69" s="74"/>
-      <c r="E69" s="74"/>
-      <c r="F69" s="74"/>
-      <c r="G69" s="75"/>
-      <c r="H69" s="75"/>
-      <c r="I69" s="74"/>
-      <c r="J69" s="76"/>
-      <c r="K69" s="76"/>
-      <c r="L69" s="77"/>
-      <c r="M69" s="15"/>
+      <c r="B69" s="63"/>
+      <c r="C69" s="70"/>
+      <c r="D69" s="64"/>
+      <c r="E69" s="64"/>
+      <c r="F69" s="64"/>
+      <c r="G69" s="65"/>
+      <c r="H69" s="65"/>
+      <c r="I69" s="64"/>
+      <c r="J69" s="66"/>
+      <c r="K69" s="66"/>
+      <c r="L69" s="67"/>
+      <c r="M69" s="14"/>
     </row>
     <row r="70" spans="1:13">
-      <c r="A70" s="19">
+      <c r="A70" s="18">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B70" s="73"/>
-      <c r="C70" s="80"/>
-      <c r="D70" s="20"/>
-      <c r="E70" s="20"/>
-      <c r="F70" s="20"/>
-      <c r="G70" s="69"/>
-      <c r="H70" s="69"/>
-      <c r="I70" s="20"/>
-      <c r="J70" s="21"/>
-      <c r="K70" s="21"/>
-      <c r="L70" s="22"/>
-      <c r="M70" s="15"/>
+      <c r="B70" s="63"/>
+      <c r="C70" s="70"/>
+      <c r="D70" s="19"/>
+      <c r="E70" s="19"/>
+      <c r="F70" s="19"/>
+      <c r="G70" s="59"/>
+      <c r="H70" s="59"/>
+      <c r="I70" s="19"/>
+      <c r="J70" s="20"/>
+      <c r="K70" s="20"/>
+      <c r="L70" s="21"/>
+      <c r="M70" s="14"/>
     </row>
     <row r="71" spans="1:13">
-      <c r="A71" s="19">
+      <c r="A71" s="18">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B71" s="73"/>
-      <c r="C71" s="80"/>
-      <c r="D71" s="74"/>
-      <c r="E71" s="74"/>
-      <c r="F71" s="74"/>
-      <c r="G71" s="75"/>
-      <c r="H71" s="75"/>
-      <c r="I71" s="74"/>
-      <c r="J71" s="76"/>
-      <c r="K71" s="76"/>
-      <c r="L71" s="77"/>
-      <c r="M71" s="15"/>
+      <c r="B71" s="63"/>
+      <c r="C71" s="70"/>
+      <c r="D71" s="64"/>
+      <c r="E71" s="64"/>
+      <c r="F71" s="64"/>
+      <c r="G71" s="65"/>
+      <c r="H71" s="65"/>
+      <c r="I71" s="64"/>
+      <c r="J71" s="66"/>
+      <c r="K71" s="66"/>
+      <c r="L71" s="67"/>
+      <c r="M71" s="14"/>
     </row>
     <row r="72" spans="1:13">
-      <c r="A72" s="19">
+      <c r="A72" s="18">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B72" s="73"/>
-      <c r="C72" s="80"/>
-      <c r="D72" s="74"/>
-      <c r="E72" s="74"/>
-      <c r="F72" s="74"/>
-      <c r="G72" s="75"/>
-      <c r="H72" s="75"/>
-      <c r="I72" s="74"/>
-      <c r="J72" s="76"/>
-      <c r="K72" s="76"/>
-      <c r="L72" s="77"/>
-      <c r="M72" s="15"/>
+      <c r="B72" s="63"/>
+      <c r="C72" s="70"/>
+      <c r="D72" s="64"/>
+      <c r="E72" s="64"/>
+      <c r="F72" s="64"/>
+      <c r="G72" s="65"/>
+      <c r="H72" s="65"/>
+      <c r="I72" s="64"/>
+      <c r="J72" s="66"/>
+      <c r="K72" s="66"/>
+      <c r="L72" s="67"/>
+      <c r="M72" s="14"/>
     </row>
     <row r="73" spans="1:13">
-      <c r="A73" s="19">
+      <c r="A73" s="18">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B73" s="73"/>
-      <c r="C73" s="80"/>
-      <c r="D73" s="20"/>
-      <c r="E73" s="20"/>
-      <c r="F73" s="20"/>
-      <c r="G73" s="69"/>
-      <c r="H73" s="69"/>
-      <c r="I73" s="20"/>
-      <c r="J73" s="21"/>
-      <c r="K73" s="21"/>
-      <c r="L73" s="22"/>
-      <c r="M73" s="15"/>
+      <c r="B73" s="63"/>
+      <c r="C73" s="70"/>
+      <c r="D73" s="19"/>
+      <c r="E73" s="19"/>
+      <c r="F73" s="19"/>
+      <c r="G73" s="59"/>
+      <c r="H73" s="59"/>
+      <c r="I73" s="19"/>
+      <c r="J73" s="20"/>
+      <c r="K73" s="20"/>
+      <c r="L73" s="21"/>
+      <c r="M73" s="14"/>
     </row>
     <row r="74" spans="1:13">
-      <c r="A74" s="19">
+      <c r="A74" s="18">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B74" s="73"/>
-      <c r="C74" s="80"/>
-      <c r="D74" s="74"/>
-      <c r="E74" s="74"/>
-      <c r="F74" s="74"/>
-      <c r="G74" s="75"/>
-      <c r="H74" s="75"/>
-      <c r="I74" s="74"/>
-      <c r="J74" s="76"/>
-      <c r="K74" s="76"/>
-      <c r="L74" s="77"/>
-      <c r="M74" s="15"/>
+      <c r="B74" s="63"/>
+      <c r="C74" s="70"/>
+      <c r="D74" s="64"/>
+      <c r="E74" s="64"/>
+      <c r="F74" s="64"/>
+      <c r="G74" s="65"/>
+      <c r="H74" s="65"/>
+      <c r="I74" s="64"/>
+      <c r="J74" s="66"/>
+      <c r="K74" s="66"/>
+      <c r="L74" s="67"/>
+      <c r="M74" s="14"/>
     </row>
     <row r="75" spans="1:13">
-      <c r="A75" s="19">
+      <c r="A75" s="18">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B75" s="73"/>
-      <c r="C75" s="80"/>
-      <c r="D75" s="74"/>
-      <c r="E75" s="74"/>
-      <c r="F75" s="74"/>
-      <c r="G75" s="75"/>
-      <c r="H75" s="75"/>
-      <c r="I75" s="74"/>
-      <c r="J75" s="76"/>
-      <c r="K75" s="76"/>
-      <c r="L75" s="77"/>
-      <c r="M75" s="15"/>
+      <c r="B75" s="63"/>
+      <c r="C75" s="70"/>
+      <c r="D75" s="64"/>
+      <c r="E75" s="64"/>
+      <c r="F75" s="64"/>
+      <c r="G75" s="65"/>
+      <c r="H75" s="65"/>
+      <c r="I75" s="64"/>
+      <c r="J75" s="66"/>
+      <c r="K75" s="66"/>
+      <c r="L75" s="67"/>
+      <c r="M75" s="14"/>
     </row>
     <row r="76" spans="1:13">
-      <c r="A76" s="19">
+      <c r="A76" s="18">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B76" s="73"/>
-      <c r="C76" s="80"/>
-      <c r="D76" s="20"/>
-      <c r="E76" s="20"/>
-      <c r="F76" s="20"/>
-      <c r="G76" s="69"/>
-      <c r="H76" s="69"/>
-      <c r="I76" s="20"/>
-      <c r="J76" s="21"/>
-      <c r="K76" s="21"/>
-      <c r="L76" s="22"/>
-      <c r="M76" s="15"/>
+      <c r="B76" s="63"/>
+      <c r="C76" s="70"/>
+      <c r="D76" s="19"/>
+      <c r="E76" s="19"/>
+      <c r="F76" s="19"/>
+      <c r="G76" s="59"/>
+      <c r="H76" s="59"/>
+      <c r="I76" s="19"/>
+      <c r="J76" s="20"/>
+      <c r="K76" s="20"/>
+      <c r="L76" s="21"/>
+      <c r="M76" s="14"/>
     </row>
     <row r="77" spans="1:13">
-      <c r="A77" s="19">
+      <c r="A77" s="18">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B77" s="73"/>
-      <c r="C77" s="80"/>
-      <c r="D77" s="74"/>
-      <c r="E77" s="74"/>
-      <c r="F77" s="74"/>
-      <c r="G77" s="75"/>
-      <c r="H77" s="75"/>
-      <c r="I77" s="74"/>
-      <c r="J77" s="76"/>
-      <c r="K77" s="76"/>
-      <c r="L77" s="77"/>
-      <c r="M77" s="15"/>
+      <c r="B77" s="63"/>
+      <c r="C77" s="70"/>
+      <c r="D77" s="64"/>
+      <c r="E77" s="64"/>
+      <c r="F77" s="64"/>
+      <c r="G77" s="65"/>
+      <c r="H77" s="65"/>
+      <c r="I77" s="64"/>
+      <c r="J77" s="66"/>
+      <c r="K77" s="66"/>
+      <c r="L77" s="67"/>
+      <c r="M77" s="14"/>
     </row>
     <row r="78" spans="1:13">
-      <c r="A78" s="23"/>
-      <c r="B78" s="24"/>
-      <c r="C78" s="25"/>
-      <c r="D78" s="25"/>
-      <c r="E78" s="25"/>
-      <c r="F78" s="25"/>
-      <c r="G78" s="70"/>
-      <c r="H78" s="70"/>
-      <c r="I78" s="25"/>
-      <c r="J78" s="26"/>
-      <c r="K78" s="26"/>
-      <c r="L78" s="27"/>
-      <c r="M78" s="15"/>
+      <c r="A78" s="22"/>
+      <c r="B78" s="23"/>
+      <c r="C78" s="24"/>
+      <c r="D78" s="24"/>
+      <c r="E78" s="24"/>
+      <c r="F78" s="24"/>
+      <c r="G78" s="60"/>
+      <c r="H78" s="60"/>
+      <c r="I78" s="24"/>
+      <c r="J78" s="25"/>
+      <c r="K78" s="25"/>
+      <c r="L78" s="26"/>
+      <c r="M78" s="14"/>
     </row>
     <row r="80" spans="1:13">
-      <c r="A80" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="B80" s="31"/>
-      <c r="C80" s="31"/>
-      <c r="D80" s="31"/>
-      <c r="E80" s="81"/>
-      <c r="F80" s="44" t="s">
+      <c r="A80" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="B80" s="30"/>
+      <c r="C80" s="30"/>
+      <c r="D80" s="30"/>
+      <c r="E80" s="71"/>
+      <c r="F80" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G80" s="44"/>
-      <c r="H80" s="44"/>
-      <c r="I80" s="44"/>
-      <c r="J80" s="43"/>
-      <c r="K80" s="43"/>
-      <c r="L80" s="43"/>
-      <c r="M80" s="43"/>
     </row>
     <row r="81" spans="1:13">
-      <c r="A81" s="47" t="s">
+      <c r="A81" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B81" s="42" t="s">
+      <c r="B81" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C81" s="42"/>
-      <c r="D81" s="42"/>
-      <c r="E81" s="82"/>
-      <c r="F81" s="67"/>
-      <c r="G81" s="67"/>
-      <c r="H81" s="67"/>
-      <c r="I81" s="67"/>
-      <c r="J81" s="44"/>
-      <c r="K81" s="45"/>
-      <c r="L81" s="45"/>
-      <c r="M81" s="35"/>
+      <c r="C81" s="36"/>
+      <c r="D81" s="36"/>
+      <c r="E81" s="72"/>
+      <c r="F81" s="57"/>
+      <c r="G81" s="57"/>
+      <c r="H81" s="57"/>
+      <c r="I81" s="57"/>
+      <c r="K81" s="37"/>
+      <c r="L81" s="37"/>
     </row>
     <row r="82" spans="1:13">
-      <c r="A82" s="51"/>
-      <c r="B82" s="46"/>
-      <c r="C82" s="38"/>
-      <c r="D82" s="38"/>
-      <c r="E82" s="39"/>
-      <c r="F82" s="68"/>
-      <c r="G82" s="68"/>
-      <c r="H82" s="68"/>
-      <c r="I82" s="34"/>
-      <c r="J82" s="36"/>
-      <c r="K82" s="36"/>
-      <c r="L82" s="36"/>
-      <c r="M82" s="35"/>
+      <c r="A82" s="43"/>
+      <c r="B82" s="38"/>
+      <c r="C82" s="32"/>
+      <c r="D82" s="32"/>
+      <c r="E82" s="33"/>
+      <c r="F82" s="58"/>
+      <c r="G82" s="58"/>
+      <c r="H82" s="58"/>
+      <c r="J82"/>
+      <c r="K82"/>
+      <c r="L82"/>
     </row>
     <row r="83" spans="1:13">
-      <c r="A83" s="51"/>
-      <c r="B83" s="46"/>
-      <c r="C83" s="40"/>
-      <c r="D83" s="40"/>
-      <c r="E83" s="41"/>
-      <c r="F83" s="68"/>
-      <c r="G83" s="68"/>
-      <c r="H83" s="68"/>
-      <c r="I83" s="34"/>
-      <c r="J83" s="36"/>
-      <c r="K83" s="36"/>
-      <c r="L83" s="36"/>
-      <c r="M83" s="35"/>
+      <c r="A83" s="43"/>
+      <c r="B83" s="38"/>
+      <c r="C83" s="34"/>
+      <c r="D83" s="34"/>
+      <c r="E83" s="35"/>
+      <c r="F83" s="58"/>
+      <c r="G83" s="58"/>
+      <c r="H83" s="58"/>
+      <c r="J83"/>
+      <c r="K83"/>
+      <c r="L83"/>
     </row>
     <row r="84" spans="1:13">
-      <c r="A84" s="52"/>
-      <c r="B84" s="48"/>
-      <c r="C84" s="49"/>
-      <c r="D84" s="49"/>
-      <c r="E84" s="50"/>
-      <c r="F84" s="68"/>
-      <c r="G84" s="68"/>
-      <c r="H84" s="68"/>
-      <c r="I84" s="34"/>
-      <c r="J84" s="36"/>
-      <c r="K84" s="36"/>
-      <c r="L84" s="36"/>
-      <c r="M84" s="35"/>
+      <c r="A84" s="44"/>
+      <c r="B84" s="40"/>
+      <c r="C84" s="41"/>
+      <c r="D84" s="41"/>
+      <c r="E84" s="42"/>
+      <c r="F84" s="58"/>
+      <c r="G84" s="58"/>
+      <c r="H84" s="58"/>
+      <c r="J84"/>
+      <c r="K84"/>
+      <c r="L84"/>
     </row>
     <row r="85" spans="1:13">
-      <c r="A85" s="13"/>
-      <c r="B85" s="13"/>
-      <c r="C85" s="13"/>
-      <c r="D85" s="13"/>
-      <c r="E85" s="13"/>
-      <c r="F85" s="13"/>
-      <c r="G85" s="13"/>
-      <c r="H85" s="13"/>
-      <c r="I85" s="13"/>
-      <c r="J85" s="13"/>
+      <c r="A85"/>
+      <c r="B85"/>
+      <c r="C85"/>
+      <c r="D85"/>
+      <c r="E85"/>
+      <c r="F85"/>
+      <c r="G85"/>
+      <c r="H85"/>
+      <c r="I85"/>
+      <c r="J85"/>
     </row>
     <row r="86" spans="1:13">
-      <c r="A86" s="13"/>
-      <c r="B86" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="C86" s="13"/>
-      <c r="D86" s="13"/>
-      <c r="E86" s="13"/>
-      <c r="F86" s="13"/>
-      <c r="G86" s="13"/>
-      <c r="H86" s="13"/>
-      <c r="I86" s="13"/>
-      <c r="J86" s="13"/>
+      <c r="A86"/>
+      <c r="B86" t="s">
+        <v>85</v>
+      </c>
+      <c r="C86"/>
+      <c r="D86"/>
+      <c r="E86"/>
+      <c r="F86"/>
+      <c r="G86"/>
+      <c r="H86"/>
+      <c r="I86"/>
+      <c r="J86"/>
     </row>
     <row r="87" spans="1:13">
       <c r="A87" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B87" s="13"/>
+      <c r="C87" s="13"/>
+      <c r="D87" s="13"/>
+      <c r="E87" s="13"/>
+      <c r="F87" s="13"/>
+      <c r="G87" s="13"/>
+      <c r="H87" s="13"/>
+      <c r="I87" s="13"/>
+      <c r="J87" s="13"/>
+      <c r="K87" s="13"/>
+      <c r="L87" s="6"/>
+      <c r="M87" s="14"/>
+    </row>
+    <row r="88" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A88" s="94" t="s">
+        <v>7</v>
+      </c>
+      <c r="B88" s="94" t="s">
         <v>84</v>
       </c>
-      <c r="B87" s="14"/>
-      <c r="C87" s="14"/>
-      <c r="D87" s="14"/>
-      <c r="E87" s="14"/>
-      <c r="F87" s="14"/>
-      <c r="G87" s="14"/>
-      <c r="H87" s="14"/>
-      <c r="I87" s="14"/>
-      <c r="J87" s="14"/>
-      <c r="K87" s="14"/>
-      <c r="L87" s="6"/>
-      <c r="M87" s="15"/>
-    </row>
-    <row r="88" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A88" s="101" t="s">
-        <v>7</v>
-      </c>
-      <c r="B88" s="101" t="s">
-        <v>85</v>
-      </c>
-      <c r="C88" s="100" t="s">
+      <c r="C88" s="91" t="s">
+        <v>86</v>
+      </c>
+      <c r="D88" s="91" t="s">
         <v>87</v>
       </c>
-      <c r="D88" s="100" t="s">
+      <c r="E88" s="91" t="s">
+        <v>81</v>
+      </c>
+      <c r="F88" s="88"/>
+      <c r="G88" s="88"/>
+      <c r="H88" s="88"/>
+      <c r="I88" s="90"/>
+      <c r="J88" s="91"/>
+      <c r="K88" s="15"/>
+      <c r="L88" s="16"/>
+      <c r="M88" s="9"/>
+    </row>
+    <row r="89" spans="1:13">
+      <c r="A89" s="94"/>
+      <c r="B89" s="94"/>
+      <c r="C89" s="91"/>
+      <c r="D89" s="91"/>
+      <c r="E89" s="91"/>
+      <c r="F89" s="89"/>
+      <c r="G89" s="89"/>
+      <c r="H89" s="89"/>
+      <c r="I89" s="90"/>
+      <c r="J89" s="91"/>
+      <c r="K89" s="17"/>
+      <c r="L89" s="28"/>
+      <c r="M89" s="14"/>
+    </row>
+    <row r="90" spans="1:13">
+      <c r="A90" s="18">
+        <v>1</v>
+      </c>
+      <c r="B90" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="E88" s="100" t="s">
-        <v>82</v>
-      </c>
-      <c r="F88" s="111"/>
-      <c r="G88" s="111"/>
-      <c r="H88" s="111"/>
-      <c r="I88" s="113"/>
-      <c r="J88" s="100"/>
-      <c r="K88" s="16"/>
-      <c r="L88" s="17"/>
-      <c r="M88" s="9"/>
-    </row>
-    <row r="89" spans="1:13">
-      <c r="A89" s="101"/>
-      <c r="B89" s="101"/>
-      <c r="C89" s="100"/>
-      <c r="D89" s="100"/>
-      <c r="E89" s="100"/>
-      <c r="F89" s="112"/>
-      <c r="G89" s="112"/>
-      <c r="H89" s="112"/>
-      <c r="I89" s="113"/>
-      <c r="J89" s="100"/>
-      <c r="K89" s="18"/>
-      <c r="L89" s="29"/>
-      <c r="M89" s="15"/>
-    </row>
-    <row r="90" spans="1:13">
-      <c r="A90" s="19">
-        <v>1</v>
-      </c>
-      <c r="B90" s="71" t="s">
-        <v>89</v>
-      </c>
-      <c r="C90" s="78" t="s">
+      <c r="C90" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="D90" s="20"/>
-      <c r="E90" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="F90" s="87"/>
-      <c r="G90" s="89"/>
-      <c r="H90" s="89"/>
-      <c r="I90" s="87"/>
-      <c r="J90" s="21"/>
-      <c r="K90" s="21"/>
-      <c r="L90" s="28"/>
-      <c r="M90" s="15"/>
+      <c r="D90" s="19"/>
+      <c r="E90" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="F90" s="77"/>
+      <c r="G90" s="79"/>
+      <c r="H90" s="79"/>
+      <c r="I90" s="77"/>
+      <c r="J90" s="20"/>
+      <c r="K90" s="20"/>
+      <c r="L90" s="27"/>
+      <c r="M90" s="14"/>
     </row>
     <row r="91" spans="1:13">
-      <c r="A91" s="19">
+      <c r="A91" s="18">
         <f>A90+1</f>
         <v>2</v>
       </c>
-      <c r="B91" s="71" t="s">
+      <c r="B91" s="61" t="s">
+        <v>89</v>
+      </c>
+      <c r="C91" s="68" t="s">
         <v>90</v>
       </c>
-      <c r="C91" s="78" t="s">
-        <v>91</v>
-      </c>
-      <c r="D91" s="20"/>
-      <c r="E91" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="F91" s="87"/>
-      <c r="G91" s="89"/>
-      <c r="H91" s="89"/>
-      <c r="I91" s="87"/>
-      <c r="J91" s="21"/>
-      <c r="K91" s="21"/>
-      <c r="L91" s="28"/>
-      <c r="M91" s="15"/>
+      <c r="D91" s="19"/>
+      <c r="E91" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="F91" s="77"/>
+      <c r="G91" s="79"/>
+      <c r="H91" s="79"/>
+      <c r="I91" s="77"/>
+      <c r="J91" s="20"/>
+      <c r="K91" s="20"/>
+      <c r="L91" s="27"/>
+      <c r="M91" s="14"/>
     </row>
     <row r="92" spans="1:13">
-      <c r="A92" s="19">
+      <c r="A92" s="18">
         <f t="shared" ref="A92:A96" si="1">A91+1</f>
         <v>3</v>
       </c>
-      <c r="B92" s="72" t="s">
+      <c r="B92" s="62" t="s">
+        <v>101</v>
+      </c>
+      <c r="C92" s="69" t="s">
+        <v>53</v>
+      </c>
+      <c r="D92" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E92" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C92" s="79" t="s">
-        <v>54</v>
-      </c>
-      <c r="D92" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="E92" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="F92" s="87"/>
-      <c r="G92" s="89"/>
-      <c r="H92" s="89"/>
-      <c r="I92" s="87"/>
-      <c r="J92" s="21"/>
-      <c r="K92" s="21"/>
-      <c r="L92" s="22"/>
-      <c r="M92" s="15"/>
+      <c r="F92" s="77"/>
+      <c r="G92" s="79"/>
+      <c r="H92" s="79"/>
+      <c r="I92" s="77"/>
+      <c r="J92" s="20"/>
+      <c r="K92" s="20"/>
+      <c r="L92" s="21"/>
+      <c r="M92" s="14"/>
     </row>
     <row r="93" spans="1:13">
-      <c r="A93" s="19">
+      <c r="A93" s="18">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B93" s="73"/>
-      <c r="C93" s="80"/>
-      <c r="D93" s="20"/>
-      <c r="E93" s="20"/>
-      <c r="F93" s="87"/>
-      <c r="G93" s="89"/>
-      <c r="H93" s="89"/>
-      <c r="I93" s="87"/>
-      <c r="J93" s="21"/>
-      <c r="K93" s="21"/>
-      <c r="L93" s="22"/>
-      <c r="M93" s="15"/>
+      <c r="B93" s="63"/>
+      <c r="C93" s="70"/>
+      <c r="D93" s="19"/>
+      <c r="E93" s="19"/>
+      <c r="F93" s="77"/>
+      <c r="G93" s="79"/>
+      <c r="H93" s="79"/>
+      <c r="I93" s="77"/>
+      <c r="J93" s="20"/>
+      <c r="K93" s="20"/>
+      <c r="L93" s="21"/>
+      <c r="M93" s="14"/>
     </row>
     <row r="94" spans="1:13">
-      <c r="A94" s="19">
+      <c r="A94" s="18">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B94" s="73"/>
-      <c r="C94" s="80"/>
-      <c r="D94" s="20"/>
-      <c r="E94" s="20"/>
-      <c r="F94" s="87"/>
-      <c r="G94" s="89"/>
-      <c r="H94" s="89"/>
-      <c r="I94" s="87"/>
-      <c r="J94" s="21"/>
-      <c r="K94" s="21"/>
-      <c r="L94" s="22"/>
-      <c r="M94" s="15"/>
+      <c r="B94" s="63"/>
+      <c r="C94" s="70"/>
+      <c r="D94" s="19"/>
+      <c r="E94" s="19"/>
+      <c r="F94" s="77"/>
+      <c r="G94" s="79"/>
+      <c r="H94" s="79"/>
+      <c r="I94" s="77"/>
+      <c r="J94" s="20"/>
+      <c r="K94" s="20"/>
+      <c r="L94" s="21"/>
+      <c r="M94" s="14"/>
     </row>
     <row r="95" spans="1:13">
-      <c r="A95" s="19">
+      <c r="A95" s="18">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B95" s="73"/>
-      <c r="C95" s="80"/>
-      <c r="D95" s="74"/>
-      <c r="E95" s="74"/>
-      <c r="F95" s="88"/>
-      <c r="G95" s="90"/>
-      <c r="H95" s="90"/>
-      <c r="I95" s="88"/>
-      <c r="J95" s="76"/>
-      <c r="K95" s="76"/>
-      <c r="L95" s="77"/>
-      <c r="M95" s="15"/>
+      <c r="B95" s="63"/>
+      <c r="C95" s="70"/>
+      <c r="D95" s="64"/>
+      <c r="E95" s="64"/>
+      <c r="F95" s="78"/>
+      <c r="G95" s="80"/>
+      <c r="H95" s="80"/>
+      <c r="I95" s="78"/>
+      <c r="J95" s="66"/>
+      <c r="K95" s="66"/>
+      <c r="L95" s="67"/>
+      <c r="M95" s="14"/>
     </row>
     <row r="96" spans="1:13">
-      <c r="A96" s="19">
+      <c r="A96" s="18">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B96" s="73"/>
-      <c r="C96" s="80"/>
-      <c r="D96" s="20"/>
-      <c r="E96" s="20"/>
-      <c r="F96" s="87"/>
-      <c r="G96" s="89"/>
-      <c r="H96" s="89"/>
-      <c r="I96" s="87"/>
-      <c r="J96" s="21"/>
-      <c r="K96" s="21"/>
-      <c r="L96" s="22"/>
-      <c r="M96" s="15"/>
+      <c r="B96" s="63"/>
+      <c r="C96" s="70"/>
+      <c r="D96" s="19"/>
+      <c r="E96" s="19"/>
+      <c r="F96" s="77"/>
+      <c r="G96" s="79"/>
+      <c r="H96" s="79"/>
+      <c r="I96" s="77"/>
+      <c r="J96" s="20"/>
+      <c r="K96" s="20"/>
+      <c r="L96" s="21"/>
+      <c r="M96" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="F88:F89"/>
-    <mergeCell ref="H88:H89"/>
-    <mergeCell ref="I88:J89"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="G88:G89"/>
-    <mergeCell ref="A88:A89"/>
-    <mergeCell ref="B88:B89"/>
-    <mergeCell ref="C88:C89"/>
-    <mergeCell ref="D88:D89"/>
-    <mergeCell ref="E88:E89"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C14:E14"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="I59:J60"/>
@@ -4010,6 +3863,21 @@
     <mergeCell ref="H59:H60"/>
     <mergeCell ref="F59:F60"/>
     <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="A88:A89"/>
+    <mergeCell ref="B88:B89"/>
+    <mergeCell ref="C88:C89"/>
+    <mergeCell ref="D88:D89"/>
+    <mergeCell ref="E88:E89"/>
+    <mergeCell ref="F88:F89"/>
+    <mergeCell ref="H88:H89"/>
+    <mergeCell ref="I88:J89"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="G88:G89"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="6">
@@ -4054,102 +3922,102 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="3" width="8.83203125" style="55" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" style="55" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="55" customWidth="1"/>
-    <col min="6" max="6" width="18.5" style="55" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="55" customWidth="1"/>
-    <col min="8" max="8" width="18.5" style="55" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="55" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" style="55" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.83203125" style="55" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" style="55" bestFit="1" customWidth="1"/>
-    <col min="13" max="253" width="8.83203125" style="55" customWidth="1"/>
-    <col min="254" max="16384" width="10.83203125" style="55"/>
+    <col min="1" max="3" width="8.83203125" style="47" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" style="47" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="47" customWidth="1"/>
+    <col min="6" max="6" width="18.5" style="47" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="47" customWidth="1"/>
+    <col min="8" max="8" width="18.5" style="47" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="47" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" style="47" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="13" max="253" width="8.83203125" style="47" customWidth="1"/>
+    <col min="254" max="16384" width="10.83203125" style="47"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="54" t="s">
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="46" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="56" t="s">
+      <c r="F3" s="48" t="s">
+        <v>110</v>
+      </c>
+      <c r="H3" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="48" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="B4" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="81"/>
+      <c r="H4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="L4" s="50"/>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="B5" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="52"/>
+      <c r="F5" s="82" t="s">
         <v>111</v>
       </c>
-      <c r="H3" s="56" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="56" t="s">
-        <v>11</v>
-      </c>
-      <c r="L3" s="56" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="B4" s="57" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="60" t="s">
+      <c r="H5" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="91"/>
-      <c r="H4" s="58"/>
-      <c r="J4" s="58"/>
-      <c r="L4" s="58"/>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="B5" s="59" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="60"/>
-      <c r="F5" s="92" t="s">
+      <c r="J5" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="52" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="B6" s="53"/>
+      <c r="F6" s="82" t="s">
         <v>112</v>
       </c>
-      <c r="H5" s="60" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="60" t="s">
-        <v>13</v>
-      </c>
-      <c r="L5" s="60" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="B6" s="61"/>
-      <c r="F6" s="92" t="s">
+    </row>
+    <row r="7" spans="1:12">
+      <c r="F7" s="83" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
-      <c r="F7" s="93" t="s">
+    <row r="8" spans="1:12">
+      <c r="F8" s="84" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="F8" s="94" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Generate routeRecordMap mainly using for bread crumbs.
</commit_message>
<xml_diff>
--- a/meta/components/PlainBoxSample.xlsx
+++ b/meta/components/PlainBoxSample.xlsx
@@ -1,41 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoVueComponent/meta/components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B4C9076-C8FA-4A4C-AAB1-529FC62BEB62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BFEF66-DEBE-254E-B8A0-7FEFD3F8A9FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="2260" windowWidth="25200" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9860" yWindow="7560" windowWidth="25200" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VueComponent" sheetId="1" r:id="rId1"/>
     <sheet name="config" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="adjustDefaultValue">config!$L$4:$L$5</definedName>
-    <definedName name="adjustFieldName">config!$J$4:$J$5</definedName>
-    <definedName name="adjustFiledName">config!$J$4:$J$5</definedName>
+    <definedName name="adjustDefaultValue">config!$J$4:$J$5</definedName>
+    <definedName name="adjustFieldName">config!$H$4:$H$5</definedName>
     <definedName name="componentKind">config!$B$4:$B$5</definedName>
-    <definedName name="createToString">config!$H$4:$H$5</definedName>
-    <definedName name="httpdMethod">config!$F$4:$F$8</definedName>
+    <definedName name="createToString">config!$F$4:$F$5</definedName>
+    <definedName name="layoutType">config!$L$3:$L$7</definedName>
     <definedName name="yesNo">config!$D$4:$D$5</definedName>
-    <definedName name="チェック種別" localSheetId="1">#REF!</definedName>
-    <definedName name="チェック種別">#REF!</definedName>
-    <definedName name="デリミタ" localSheetId="1">#REF!</definedName>
-    <definedName name="デリミタ">#REF!</definedName>
-    <definedName name="デリミタ選択肢" localSheetId="1">#REF!</definedName>
-    <definedName name="デリミタ選択肢">#REF!</definedName>
-    <definedName name="型" localSheetId="1">#REF!</definedName>
-    <definedName name="型">#REF!</definedName>
-    <definedName name="項目型" localSheetId="1">#REF!</definedName>
-    <definedName name="項目型">#REF!</definedName>
-    <definedName name="必須" localSheetId="1">#REF!</definedName>
-    <definedName name="必須">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -58,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="130">
   <si>
     <t>パッケージ</t>
   </si>
@@ -957,51 +944,96 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>HTTPメソッド</t>
+    <t>PlainBoxSample</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>sample.pages.plainBoxSample</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>/plainbox</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>plainbox</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>fuga</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>fur</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>"ふが"</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>レイアウト</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>single</t>
+  </si>
+  <si>
+    <t>/* 画面レイアウト識別子 */</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>レイアウト</t>
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>POST</t>
+    <t>single</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>list</t>
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>GET</t>
+    <t>detail</t>
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>PUT</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>DELETE</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>PlainBoxSample</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>sample.pages.plainBoxSample</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>/plainbox</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>plainbox</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>fuga</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>fur</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>"ふが"</t>
+    <t>Vueコンポーネント定義・パンくずリスト</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>/* この画面のパンくずリストを記述します。（自分自身は書かない） */</t>
+    <rPh sb="5" eb="7">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>キジュツ</t>
+    </rPh>
+    <rPh sb="23" eb="27">
+      <t>ジブンジシン</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>カ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>コンポーネント別名</t>
+    <rPh sb="7" eb="9">
+      <t>ベツメイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>HOME</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ボックスサンプルプレイン</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1061,7 +1093,7 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1098,8 +1130,32 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="48">
+  <borders count="60">
     <border>
       <left/>
       <right/>
@@ -1651,46 +1707,194 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dashed">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
-      <top style="dashed">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dashed">
-        <color indexed="64"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
-      <top style="dashed">
-        <color indexed="64"/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1699,7 +1903,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1851,21 +2055,102 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="46" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="46" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="47" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="46" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="47" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="48" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="47" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1874,45 +2159,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2325,10 +2571,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M96"/>
+  <dimension ref="A1:M103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2377,7 +2623,7 @@
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="8"/>
@@ -2405,7 +2651,7 @@
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="7" t="s">
-        <v>62</v>
+        <v>129</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="8"/>
@@ -2419,7 +2665,7 @@
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="10" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D9" s="31"/>
       <c r="E9" s="11"/>
@@ -2428,12 +2674,12 @@
       </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="95" t="s">
+      <c r="A10" s="118" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="96"/>
+      <c r="B10" s="119"/>
       <c r="C10" s="10" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D10" s="31"/>
       <c r="E10" s="11"/>
@@ -2442,12 +2688,12 @@
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="95" t="s">
+      <c r="A11" s="118" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="96"/>
+      <c r="B11" s="119"/>
       <c r="C11" s="10" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D11" s="31"/>
       <c r="E11" s="11"/>
@@ -2456,10 +2702,10 @@
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="95" t="s">
+      <c r="A12" s="118" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="96"/>
+      <c r="B12" s="119"/>
       <c r="C12" s="10" t="s">
         <v>21</v>
       </c>
@@ -2470,10 +2716,10 @@
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="95" t="s">
+      <c r="A13" s="118" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="96"/>
+      <c r="B13" s="119"/>
       <c r="C13" s="76" t="s">
         <v>63</v>
       </c>
@@ -2488,11 +2734,11 @@
         <v>1</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="97" t="s">
+      <c r="C14" s="120" t="s">
         <v>71</v>
       </c>
-      <c r="D14" s="98"/>
-      <c r="E14" s="99"/>
+      <c r="D14" s="121"/>
+      <c r="E14" s="122"/>
       <c r="F14" s="56"/>
       <c r="G14" s="56"/>
       <c r="H14" s="56"/>
@@ -2543,30 +2789,27 @@
       <c r="I17"/>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="55"/>
+      <c r="A18" s="84" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18" s="85"/>
+      <c r="C18" s="86" t="s">
+        <v>118</v>
+      </c>
       <c r="D18" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18"/>
-      <c r="F18"/>
+        <v>119</v>
+      </c>
       <c r="G18"/>
       <c r="H18"/>
-      <c r="I18"/>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="54" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B19" s="13"/>
-      <c r="C19" s="55" t="s">
-        <v>14</v>
-      </c>
+      <c r="C19" s="55"/>
       <c r="D19" t="s">
-        <v>73</v>
+        <v>36</v>
       </c>
       <c r="E19"/>
       <c r="F19"/>
@@ -2576,14 +2819,14 @@
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="54" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="B20" s="13"/>
       <c r="C20" s="55" t="s">
         <v>14</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="E20"/>
       <c r="F20"/>
@@ -2593,14 +2836,14 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="54" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="B21" s="13"/>
       <c r="C21" s="55" t="s">
         <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>74</v>
+        <v>30</v>
       </c>
       <c r="E21"/>
       <c r="F21"/>
@@ -2609,15 +2852,15 @@
       <c r="I21"/>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="100" t="s">
-        <v>77</v>
-      </c>
-      <c r="B22" s="101"/>
+      <c r="A22" s="54" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="13"/>
       <c r="C22" s="55" t="s">
         <v>14</v>
       </c>
       <c r="D22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E22"/>
       <c r="F22"/>
@@ -2626,14 +2869,16 @@
       <c r="I22"/>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="13"/>
+      <c r="A23" s="110" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="111"/>
       <c r="C23" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="D23"/>
+      <c r="D23" t="s">
+        <v>75</v>
+      </c>
       <c r="E23"/>
       <c r="F23"/>
       <c r="G23"/>
@@ -2641,16 +2886,14 @@
       <c r="I23"/>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="100" t="s">
-        <v>18</v>
-      </c>
-      <c r="B24" s="101"/>
+      <c r="A24" s="54" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="13"/>
       <c r="C24" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="D24" t="s">
-        <v>19</v>
-      </c>
+      <c r="D24"/>
       <c r="E24"/>
       <c r="F24"/>
       <c r="G24"/>
@@ -2658,14 +2901,16 @@
       <c r="I24"/>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="100" t="s">
-        <v>64</v>
-      </c>
-      <c r="B25" s="101"/>
+      <c r="A25" s="110" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="111"/>
       <c r="C25" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="D25"/>
+      <c r="D25" t="s">
+        <v>19</v>
+      </c>
       <c r="E25"/>
       <c r="F25"/>
       <c r="G25"/>
@@ -2673,64 +2918,62 @@
       <c r="I25"/>
     </row>
     <row r="26" spans="1:12">
-      <c r="B26"/>
+      <c r="A26" s="110" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="111"/>
+      <c r="C26" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="F26"/>
+      <c r="G26"/>
+      <c r="H26"/>
+      <c r="I26"/>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="71"/>
-      <c r="F27" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="B27"/>
     </row>
     <row r="28" spans="1:12">
-      <c r="A28" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="72"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="57"/>
-      <c r="H28" s="57"/>
-      <c r="I28" s="57"/>
-      <c r="K28" s="37"/>
-      <c r="L28" s="37"/>
+      <c r="A28" s="90" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28" s="91"/>
+      <c r="C28" s="91"/>
+      <c r="D28" s="91"/>
+      <c r="E28" s="92"/>
+      <c r="F28" s="1" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="29" spans="1:12">
-      <c r="A29" s="43">
+      <c r="A29" s="93" t="s">
+        <v>126</v>
+      </c>
+      <c r="B29" s="94" t="s">
+        <v>127</v>
+      </c>
+      <c r="C29" s="94"/>
+      <c r="D29" s="94"/>
+      <c r="E29" s="95"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="57"/>
+      <c r="I29" s="57"/>
+      <c r="K29" s="37"/>
+      <c r="L29" s="37"/>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="96">
         <v>1</v>
       </c>
-      <c r="B29" s="38" t="s">
-        <v>104</v>
-      </c>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="58"/>
-      <c r="G29" s="58"/>
-      <c r="H29" s="58"/>
-      <c r="J29"/>
-      <c r="K29"/>
-      <c r="L29"/>
-    </row>
-    <row r="30" spans="1:12">
-      <c r="A30" s="43">
-        <v>2</v>
-      </c>
-      <c r="B30" s="38" t="s">
-        <v>105</v>
-      </c>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="35"/>
+      <c r="B30" s="97" t="s">
+        <v>128</v>
+      </c>
+      <c r="C30" s="98"/>
+      <c r="D30" s="98"/>
+      <c r="E30" s="99"/>
       <c r="F30" s="58"/>
       <c r="G30" s="58"/>
       <c r="H30" s="58"/>
@@ -2739,11 +2982,11 @@
       <c r="L30"/>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="44"/>
-      <c r="B31" s="40"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="42"/>
+      <c r="A31" s="96"/>
+      <c r="B31" s="97"/>
+      <c r="C31" s="100"/>
+      <c r="D31" s="100"/>
+      <c r="E31" s="101"/>
       <c r="F31" s="58"/>
       <c r="G31" s="58"/>
       <c r="H31" s="58"/>
@@ -2752,73 +2995,64 @@
       <c r="L31"/>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32"/>
-      <c r="B32"/>
-      <c r="C32"/>
-      <c r="D32"/>
-      <c r="E32"/>
-      <c r="F32"/>
-      <c r="G32"/>
-      <c r="H32"/>
-      <c r="I32"/>
+      <c r="A32" s="102"/>
+      <c r="B32" s="103"/>
+      <c r="C32" s="104"/>
+      <c r="D32" s="104"/>
+      <c r="E32" s="105"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="58"/>
+      <c r="H32" s="58"/>
       <c r="J32"/>
-    </row>
-    <row r="33" spans="1:12">
-      <c r="A33" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="B33" s="30"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="71"/>
-      <c r="F33" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="K32"/>
+      <c r="L32"/>
+    </row>
+    <row r="33" spans="1:12" s="108" customFormat="1">
+      <c r="A33" s="106"/>
+      <c r="B33" s="106"/>
+      <c r="C33" s="107"/>
+      <c r="G33" s="109"/>
+      <c r="H33" s="109"/>
     </row>
     <row r="34" spans="1:12">
-      <c r="A34" s="39" t="s">
+      <c r="A34" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="71"/>
+      <c r="F34" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="C34" s="36"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="72"/>
-      <c r="F34" s="57"/>
-      <c r="G34" s="57"/>
-      <c r="H34" s="57"/>
-      <c r="I34" s="57"/>
-      <c r="K34" s="37"/>
-      <c r="L34" s="37"/>
-    </row>
-    <row r="35" spans="1:12">
-      <c r="A35" s="43">
-        <v>1</v>
-      </c>
-      <c r="B35" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="58"/>
-      <c r="G35" s="58"/>
-      <c r="H35" s="58"/>
-      <c r="J35"/>
-      <c r="K35"/>
-      <c r="L35"/>
+      <c r="B35" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="36"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="72"/>
+      <c r="F35" s="57"/>
+      <c r="G35" s="57"/>
+      <c r="H35" s="57"/>
+      <c r="I35" s="57"/>
+      <c r="K35" s="37"/>
+      <c r="L35" s="37"/>
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B36" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="C36" s="34"/>
-      <c r="D36" s="34"/>
-      <c r="E36" s="35"/>
+        <v>104</v>
+      </c>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="33"/>
       <c r="F36" s="58"/>
       <c r="G36" s="58"/>
       <c r="H36" s="58"/>
@@ -2827,11 +3061,15 @@
       <c r="L36"/>
     </row>
     <row r="37" spans="1:12">
-      <c r="A37" s="44"/>
-      <c r="B37" s="40"/>
-      <c r="C37" s="41"/>
-      <c r="D37" s="41"/>
-      <c r="E37" s="42"/>
+      <c r="A37" s="43">
+        <v>2</v>
+      </c>
+      <c r="B37" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="C37" s="34"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="35"/>
       <c r="F37" s="58"/>
       <c r="G37" s="58"/>
       <c r="H37" s="58"/>
@@ -2840,11 +3078,11 @@
       <c r="L37"/>
     </row>
     <row r="38" spans="1:12">
-      <c r="A38" s="73"/>
-      <c r="B38" s="74"/>
-      <c r="C38" s="75"/>
-      <c r="D38" s="75"/>
-      <c r="E38" s="75"/>
+      <c r="A38" s="44"/>
+      <c r="B38" s="40"/>
+      <c r="C38" s="41"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="42"/>
       <c r="F38" s="58"/>
       <c r="G38" s="58"/>
       <c r="H38" s="58"/>
@@ -2853,53 +3091,56 @@
       <c r="L38"/>
     </row>
     <row r="39" spans="1:12">
-      <c r="A39" s="29" t="s">
-        <v>93</v>
-      </c>
-      <c r="B39" s="30"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="71"/>
-      <c r="F39" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="A39"/>
+      <c r="B39"/>
+      <c r="C39"/>
+      <c r="D39"/>
+      <c r="E39"/>
+      <c r="F39"/>
+      <c r="G39"/>
+      <c r="H39"/>
+      <c r="I39"/>
+      <c r="J39"/>
     </row>
     <row r="40" spans="1:12">
-      <c r="A40" s="39" t="s">
+      <c r="A40" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40" s="30"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="71"/>
+      <c r="F40" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="72"/>
-      <c r="F40" s="57"/>
-      <c r="G40" s="57"/>
-      <c r="H40" s="57"/>
-      <c r="I40" s="57"/>
-      <c r="K40" s="37"/>
-      <c r="L40" s="37"/>
-    </row>
-    <row r="41" spans="1:12">
-      <c r="A41" s="43"/>
-      <c r="B41" s="38"/>
-      <c r="C41" s="32"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="33"/>
-      <c r="F41" s="58"/>
-      <c r="G41" s="58"/>
-      <c r="H41" s="58"/>
-      <c r="J41"/>
-      <c r="K41"/>
-      <c r="L41"/>
+      <c r="B41" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="C41" s="36"/>
+      <c r="D41" s="36"/>
+      <c r="E41" s="72"/>
+      <c r="F41" s="57"/>
+      <c r="G41" s="57"/>
+      <c r="H41" s="57"/>
+      <c r="I41" s="57"/>
+      <c r="K41" s="37"/>
+      <c r="L41" s="37"/>
     </row>
     <row r="42" spans="1:12">
-      <c r="A42" s="43"/>
-      <c r="B42" s="38"/>
-      <c r="C42" s="34"/>
-      <c r="D42" s="34"/>
-      <c r="E42" s="35"/>
+      <c r="A42" s="43">
+        <v>1</v>
+      </c>
+      <c r="B42" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" s="32"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="33"/>
       <c r="F42" s="58"/>
       <c r="G42" s="58"/>
       <c r="H42" s="58"/>
@@ -2908,11 +3149,15 @@
       <c r="L42"/>
     </row>
     <row r="43" spans="1:12">
-      <c r="A43" s="44"/>
-      <c r="B43" s="40"/>
-      <c r="C43" s="41"/>
-      <c r="D43" s="41"/>
-      <c r="E43" s="42"/>
+      <c r="A43" s="43">
+        <v>2</v>
+      </c>
+      <c r="B43" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" s="34"/>
+      <c r="D43" s="34"/>
+      <c r="E43" s="35"/>
       <c r="F43" s="58"/>
       <c r="G43" s="58"/>
       <c r="H43" s="58"/>
@@ -2921,69 +3166,66 @@
       <c r="L43"/>
     </row>
     <row r="44" spans="1:12">
-      <c r="A44"/>
-      <c r="B44"/>
-      <c r="C44"/>
-      <c r="D44"/>
-      <c r="E44"/>
-      <c r="F44"/>
-      <c r="G44"/>
-      <c r="H44"/>
-      <c r="I44"/>
+      <c r="A44" s="44"/>
+      <c r="B44" s="40"/>
+      <c r="C44" s="41"/>
+      <c r="D44" s="41"/>
+      <c r="E44" s="42"/>
+      <c r="F44" s="58"/>
+      <c r="G44" s="58"/>
+      <c r="H44" s="58"/>
       <c r="J44"/>
+      <c r="K44"/>
+      <c r="L44"/>
     </row>
     <row r="45" spans="1:12">
-      <c r="A45" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="B45" s="30"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="30"/>
-      <c r="E45" s="71"/>
-      <c r="F45" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="A45" s="73"/>
+      <c r="B45" s="74"/>
+      <c r="C45" s="75"/>
+      <c r="D45" s="75"/>
+      <c r="E45" s="75"/>
+      <c r="F45" s="58"/>
+      <c r="G45" s="58"/>
+      <c r="H45" s="58"/>
+      <c r="J45"/>
+      <c r="K45"/>
+      <c r="L45"/>
     </row>
     <row r="46" spans="1:12">
-      <c r="A46" s="39" t="s">
+      <c r="A46" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="B46" s="30"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="71"/>
+      <c r="F46" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B46" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="C46" s="39" t="s">
-        <v>109</v>
-      </c>
-      <c r="D46" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="E46" s="72"/>
-      <c r="F46" s="57"/>
-      <c r="G46" s="57"/>
-      <c r="H46" s="57"/>
-      <c r="I46" s="57"/>
-      <c r="K46" s="37"/>
-      <c r="L46" s="37"/>
-    </row>
-    <row r="47" spans="1:12">
-      <c r="A47" s="43"/>
-      <c r="B47" s="38"/>
-      <c r="C47" s="85"/>
-      <c r="D47" s="32"/>
-      <c r="E47" s="33"/>
-      <c r="F47" s="58"/>
-      <c r="G47" s="58"/>
-      <c r="H47" s="58"/>
-      <c r="J47"/>
-      <c r="K47"/>
-      <c r="L47"/>
+      <c r="B47" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47" s="36"/>
+      <c r="D47" s="36"/>
+      <c r="E47" s="72"/>
+      <c r="F47" s="57"/>
+      <c r="G47" s="57"/>
+      <c r="H47" s="57"/>
+      <c r="I47" s="57"/>
+      <c r="K47" s="37"/>
+      <c r="L47" s="37"/>
     </row>
     <row r="48" spans="1:12">
       <c r="A48" s="43"/>
       <c r="B48" s="38"/>
-      <c r="C48" s="86"/>
-      <c r="D48" s="34"/>
-      <c r="E48" s="35"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="32"/>
+      <c r="E48" s="33"/>
       <c r="F48" s="58"/>
       <c r="G48" s="58"/>
       <c r="H48" s="58"/>
@@ -2991,12 +3233,12 @@
       <c r="K48"/>
       <c r="L48"/>
     </row>
-    <row r="49" spans="1:13">
-      <c r="A49" s="44"/>
-      <c r="B49" s="40"/>
-      <c r="C49" s="87"/>
-      <c r="D49" s="41"/>
-      <c r="E49" s="42"/>
+    <row r="49" spans="1:12">
+      <c r="A49" s="43"/>
+      <c r="B49" s="38"/>
+      <c r="C49" s="34"/>
+      <c r="D49" s="34"/>
+      <c r="E49" s="35"/>
       <c r="F49" s="58"/>
       <c r="G49" s="58"/>
       <c r="H49" s="58"/>
@@ -3004,12 +3246,12 @@
       <c r="K49"/>
       <c r="L49"/>
     </row>
-    <row r="50" spans="1:13">
-      <c r="A50" s="73"/>
-      <c r="B50" s="74"/>
-      <c r="C50" s="75"/>
-      <c r="D50" s="75"/>
-      <c r="E50" s="75"/>
+    <row r="50" spans="1:12">
+      <c r="A50" s="44"/>
+      <c r="B50" s="40"/>
+      <c r="C50" s="41"/>
+      <c r="D50" s="41"/>
+      <c r="E50" s="42"/>
       <c r="F50" s="58"/>
       <c r="G50" s="58"/>
       <c r="H50" s="58"/>
@@ -3017,56 +3259,57 @@
       <c r="K50"/>
       <c r="L50"/>
     </row>
-    <row r="51" spans="1:13">
-      <c r="A51" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="B51" s="30"/>
-      <c r="C51" s="30"/>
-      <c r="D51" s="30"/>
-      <c r="E51" s="71"/>
-      <c r="F51" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13">
-      <c r="A52" s="39" t="s">
+    <row r="51" spans="1:12">
+      <c r="A51"/>
+      <c r="B51"/>
+      <c r="C51"/>
+      <c r="D51"/>
+      <c r="E51"/>
+      <c r="F51"/>
+      <c r="G51"/>
+      <c r="H51"/>
+      <c r="I51"/>
+      <c r="J51"/>
+    </row>
+    <row r="52" spans="1:12">
+      <c r="A52" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B52" s="30"/>
+      <c r="C52" s="30"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="71"/>
+      <c r="F52" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
+      <c r="A53" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B52" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="C52" s="36"/>
-      <c r="D52" s="36"/>
-      <c r="E52" s="72"/>
-      <c r="F52" s="57" t="s">
-        <v>103</v>
-      </c>
-      <c r="G52" s="57"/>
-      <c r="H52" s="57"/>
-      <c r="I52" s="57"/>
-      <c r="K52" s="37"/>
-      <c r="L52" s="37"/>
-    </row>
-    <row r="53" spans="1:13">
-      <c r="A53" s="43"/>
-      <c r="B53" s="38"/>
-      <c r="C53" s="32"/>
-      <c r="D53" s="32"/>
-      <c r="E53" s="33"/>
-      <c r="F53" s="58"/>
-      <c r="G53" s="58"/>
-      <c r="H53" s="58"/>
-      <c r="J53"/>
-      <c r="K53"/>
-      <c r="L53"/>
-    </row>
-    <row r="54" spans="1:13">
+      <c r="B53" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="C53" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="D53" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="E53" s="72"/>
+      <c r="F53" s="57"/>
+      <c r="G53" s="57"/>
+      <c r="H53" s="57"/>
+      <c r="I53" s="57"/>
+      <c r="K53" s="37"/>
+      <c r="L53" s="37"/>
+    </row>
+    <row r="54" spans="1:12">
       <c r="A54" s="43"/>
       <c r="B54" s="38"/>
-      <c r="C54" s="34"/>
-      <c r="D54" s="34"/>
-      <c r="E54" s="35"/>
+      <c r="C54" s="81"/>
+      <c r="D54" s="32"/>
+      <c r="E54" s="33"/>
       <c r="F54" s="58"/>
       <c r="G54" s="58"/>
       <c r="H54" s="58"/>
@@ -3074,12 +3317,12 @@
       <c r="K54"/>
       <c r="L54"/>
     </row>
-    <row r="55" spans="1:13">
-      <c r="A55" s="44"/>
-      <c r="B55" s="40"/>
-      <c r="C55" s="41"/>
-      <c r="D55" s="41"/>
-      <c r="E55" s="42"/>
+    <row r="55" spans="1:12">
+      <c r="A55" s="43"/>
+      <c r="B55" s="38"/>
+      <c r="C55" s="82"/>
+      <c r="D55" s="34"/>
+      <c r="E55" s="35"/>
       <c r="F55" s="58"/>
       <c r="G55" s="58"/>
       <c r="H55" s="58"/>
@@ -3087,327 +3330,267 @@
       <c r="K55"/>
       <c r="L55"/>
     </row>
-    <row r="56" spans="1:13">
-      <c r="A56"/>
-      <c r="B56"/>
-      <c r="C56"/>
-      <c r="D56"/>
-      <c r="E56"/>
-      <c r="F56"/>
-      <c r="G56"/>
-      <c r="H56"/>
-      <c r="I56"/>
+    <row r="56" spans="1:12">
+      <c r="A56" s="44"/>
+      <c r="B56" s="40"/>
+      <c r="C56" s="83"/>
+      <c r="D56" s="41"/>
+      <c r="E56" s="42"/>
+      <c r="F56" s="58"/>
+      <c r="G56" s="58"/>
+      <c r="H56" s="58"/>
       <c r="J56"/>
-    </row>
-    <row r="57" spans="1:13">
-      <c r="A57"/>
-      <c r="B57" t="s">
+      <c r="K56"/>
+      <c r="L56"/>
+    </row>
+    <row r="57" spans="1:12">
+      <c r="A57" s="73"/>
+      <c r="B57" s="74"/>
+      <c r="C57" s="75"/>
+      <c r="D57" s="75"/>
+      <c r="E57" s="75"/>
+      <c r="F57" s="58"/>
+      <c r="G57" s="58"/>
+      <c r="H57" s="58"/>
+      <c r="J57"/>
+      <c r="K57"/>
+      <c r="L57"/>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="A58" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="B58" s="30"/>
+      <c r="C58" s="30"/>
+      <c r="D58" s="30"/>
+      <c r="E58" s="71"/>
+      <c r="F58" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
+      <c r="A59" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C59" s="36"/>
+      <c r="D59" s="36"/>
+      <c r="E59" s="72"/>
+      <c r="F59" s="57" t="s">
+        <v>103</v>
+      </c>
+      <c r="G59" s="57"/>
+      <c r="H59" s="57"/>
+      <c r="I59" s="57"/>
+      <c r="K59" s="37"/>
+      <c r="L59" s="37"/>
+    </row>
+    <row r="60" spans="1:12">
+      <c r="A60" s="43"/>
+      <c r="B60" s="38"/>
+      <c r="C60" s="32"/>
+      <c r="D60" s="32"/>
+      <c r="E60" s="33"/>
+      <c r="F60" s="58"/>
+      <c r="G60" s="58"/>
+      <c r="H60" s="58"/>
+      <c r="J60"/>
+      <c r="K60"/>
+      <c r="L60"/>
+    </row>
+    <row r="61" spans="1:12">
+      <c r="A61" s="43"/>
+      <c r="B61" s="38"/>
+      <c r="C61" s="34"/>
+      <c r="D61" s="34"/>
+      <c r="E61" s="35"/>
+      <c r="F61" s="58"/>
+      <c r="G61" s="58"/>
+      <c r="H61" s="58"/>
+      <c r="J61"/>
+      <c r="K61"/>
+      <c r="L61"/>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="A62" s="44"/>
+      <c r="B62" s="40"/>
+      <c r="C62" s="41"/>
+      <c r="D62" s="41"/>
+      <c r="E62" s="42"/>
+      <c r="F62" s="58"/>
+      <c r="G62" s="58"/>
+      <c r="H62" s="58"/>
+      <c r="J62"/>
+      <c r="K62"/>
+      <c r="L62"/>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="A63"/>
+      <c r="B63"/>
+      <c r="C63"/>
+      <c r="D63"/>
+      <c r="E63"/>
+      <c r="F63"/>
+      <c r="G63"/>
+      <c r="H63"/>
+      <c r="I63"/>
+      <c r="J63"/>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="A64"/>
+      <c r="B64" t="s">
         <v>78</v>
       </c>
-      <c r="C57"/>
-      <c r="D57"/>
-      <c r="E57"/>
-      <c r="F57"/>
-      <c r="G57"/>
-      <c r="H57"/>
-      <c r="I57"/>
-      <c r="J57"/>
-    </row>
-    <row r="58" spans="1:13">
-      <c r="A58" s="3" t="s">
+      <c r="C64"/>
+      <c r="D64"/>
+      <c r="E64"/>
+      <c r="F64"/>
+      <c r="G64"/>
+      <c r="H64"/>
+      <c r="I64"/>
+      <c r="J64"/>
+    </row>
+    <row r="65" spans="1:13">
+      <c r="A65" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B58" s="13"/>
-      <c r="C58" s="13"/>
-      <c r="D58" s="13"/>
-      <c r="E58" s="13"/>
-      <c r="F58" s="13"/>
-      <c r="G58" s="13"/>
-      <c r="H58" s="13"/>
-      <c r="I58" s="13"/>
-      <c r="J58" s="13"/>
-      <c r="K58" s="13"/>
-      <c r="L58" s="6"/>
-      <c r="M58" s="14"/>
-    </row>
-    <row r="59" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A59" s="94" t="s">
+      <c r="B65" s="13"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="13"/>
+      <c r="E65" s="13"/>
+      <c r="F65" s="13"/>
+      <c r="G65" s="13"/>
+      <c r="H65" s="13"/>
+      <c r="I65" s="13"/>
+      <c r="J65" s="13"/>
+      <c r="K65" s="13"/>
+      <c r="L65" s="6"/>
+      <c r="M65" s="14"/>
+    </row>
+    <row r="66" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A66" s="113" t="s">
         <v>7</v>
       </c>
-      <c r="B59" s="94" t="s">
+      <c r="B66" s="113" t="s">
         <v>3</v>
       </c>
-      <c r="C59" s="91" t="s">
+      <c r="C66" s="112" t="s">
         <v>4</v>
       </c>
-      <c r="D59" s="91" t="s">
+      <c r="D66" s="112" t="s">
         <v>6</v>
       </c>
-      <c r="E59" s="91" t="s">
+      <c r="E66" s="112" t="s">
         <v>5</v>
       </c>
-      <c r="F59" s="92" t="s">
+      <c r="F66" s="116" t="s">
         <v>33</v>
       </c>
-      <c r="G59" s="92" t="s">
+      <c r="G66" s="116" t="s">
         <v>16</v>
       </c>
-      <c r="H59" s="102" t="s">
+      <c r="H66" s="114" t="s">
         <v>106</v>
       </c>
-      <c r="I59" s="91" t="s">
+      <c r="I66" s="112" t="s">
         <v>1</v>
       </c>
-      <c r="J59" s="91"/>
-      <c r="K59" s="15"/>
-      <c r="L59" s="16"/>
-      <c r="M59" s="9"/>
-    </row>
-    <row r="60" spans="1:13">
-      <c r="A60" s="94"/>
-      <c r="B60" s="94"/>
-      <c r="C60" s="91"/>
-      <c r="D60" s="91"/>
-      <c r="E60" s="91"/>
-      <c r="F60" s="93"/>
-      <c r="G60" s="93"/>
-      <c r="H60" s="103"/>
-      <c r="I60" s="91"/>
-      <c r="J60" s="91"/>
-      <c r="K60" s="17"/>
-      <c r="L60" s="28"/>
-      <c r="M60" s="14"/>
-    </row>
-    <row r="61" spans="1:13">
-      <c r="A61" s="18">
-        <v>1</v>
-      </c>
-      <c r="B61" s="61" t="s">
-        <v>47</v>
-      </c>
-      <c r="C61" s="68" t="s">
-        <v>48</v>
-      </c>
-      <c r="D61" s="19"/>
-      <c r="E61" s="19"/>
-      <c r="F61" s="19"/>
-      <c r="G61" s="59"/>
-      <c r="H61" s="59"/>
-      <c r="I61" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="J61" s="20"/>
-      <c r="K61" s="20"/>
-      <c r="L61" s="27"/>
-      <c r="M61" s="14"/>
-    </row>
-    <row r="62" spans="1:13">
-      <c r="A62" s="18">
-        <f>A61+1</f>
-        <v>2</v>
-      </c>
-      <c r="B62" s="61" t="s">
-        <v>49</v>
-      </c>
-      <c r="C62" s="68" t="s">
-        <v>50</v>
-      </c>
-      <c r="D62" s="19"/>
-      <c r="E62" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="F62" s="19"/>
-      <c r="G62" s="59"/>
-      <c r="H62" s="59"/>
-      <c r="I62" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="J62" s="20"/>
-      <c r="K62" s="20"/>
-      <c r="L62" s="27"/>
-      <c r="M62" s="14"/>
-    </row>
-    <row r="63" spans="1:13">
-      <c r="A63" s="18">
-        <f t="shared" ref="A63:A77" si="0">A62+1</f>
-        <v>3</v>
-      </c>
-      <c r="B63" s="62" t="s">
-        <v>52</v>
-      </c>
-      <c r="C63" s="69" t="s">
-        <v>53</v>
-      </c>
-      <c r="D63" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="E63" s="19"/>
-      <c r="F63" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G63" s="59" t="s">
-        <v>14</v>
-      </c>
-      <c r="H63" s="59"/>
-      <c r="I63" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="J63" s="20"/>
-      <c r="K63" s="20"/>
-      <c r="L63" s="21"/>
-      <c r="M63" s="14"/>
-    </row>
-    <row r="64" spans="1:13">
-      <c r="A64" s="18">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B64" s="63" t="s">
-        <v>58</v>
-      </c>
-      <c r="C64" s="70" t="s">
-        <v>54</v>
-      </c>
-      <c r="D64" s="19"/>
-      <c r="E64" s="19"/>
-      <c r="F64" s="19"/>
-      <c r="G64" s="59" t="s">
-        <v>14</v>
-      </c>
-      <c r="H64" s="59"/>
-      <c r="I64" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="J64" s="20"/>
-      <c r="K64" s="20"/>
-      <c r="L64" s="21"/>
-      <c r="M64" s="14"/>
-    </row>
-    <row r="65" spans="1:13">
-      <c r="A65" s="18">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B65" s="63" t="s">
-        <v>107</v>
-      </c>
-      <c r="C65" s="70" t="s">
-        <v>48</v>
-      </c>
-      <c r="D65" s="19"/>
-      <c r="E65" s="19"/>
-      <c r="F65" s="19"/>
-      <c r="G65" s="59" t="s">
-        <v>14</v>
-      </c>
-      <c r="H65" s="59" t="s">
-        <v>107</v>
-      </c>
-      <c r="I65" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="J65" s="20"/>
-      <c r="K65" s="20"/>
-      <c r="L65" s="21"/>
-      <c r="M65" s="14"/>
-    </row>
-    <row r="66" spans="1:13">
-      <c r="A66" s="18">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B66" s="63" t="s">
-        <v>119</v>
-      </c>
-      <c r="C66" s="70" t="s">
-        <v>48</v>
-      </c>
-      <c r="D66" s="64"/>
-      <c r="E66" s="64" t="s">
-        <v>121</v>
-      </c>
-      <c r="F66" s="64"/>
-      <c r="G66" s="65" t="s">
-        <v>14</v>
-      </c>
-      <c r="H66" s="65" t="s">
-        <v>120</v>
-      </c>
-      <c r="I66" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="J66" s="66"/>
-      <c r="K66" s="66"/>
-      <c r="L66" s="67"/>
-      <c r="M66" s="14"/>
+      <c r="J66" s="112"/>
+      <c r="K66" s="15"/>
+      <c r="L66" s="16"/>
+      <c r="M66" s="9"/>
     </row>
     <row r="67" spans="1:13">
-      <c r="A67" s="18">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B67" s="63"/>
-      <c r="C67" s="70"/>
-      <c r="D67" s="19"/>
-      <c r="E67" s="19"/>
-      <c r="F67" s="19"/>
-      <c r="G67" s="59"/>
-      <c r="H67" s="59"/>
-      <c r="I67" s="19"/>
-      <c r="J67" s="20"/>
-      <c r="K67" s="20"/>
-      <c r="L67" s="21"/>
+      <c r="A67" s="113"/>
+      <c r="B67" s="113"/>
+      <c r="C67" s="112"/>
+      <c r="D67" s="112"/>
+      <c r="E67" s="112"/>
+      <c r="F67" s="117"/>
+      <c r="G67" s="117"/>
+      <c r="H67" s="115"/>
+      <c r="I67" s="112"/>
+      <c r="J67" s="112"/>
+      <c r="K67" s="17"/>
+      <c r="L67" s="28"/>
       <c r="M67" s="14"/>
     </row>
     <row r="68" spans="1:13">
       <c r="A68" s="18">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B68" s="63"/>
-      <c r="C68" s="70"/>
-      <c r="D68" s="64"/>
-      <c r="E68" s="64"/>
-      <c r="F68" s="64"/>
-      <c r="G68" s="65"/>
-      <c r="H68" s="65"/>
-      <c r="I68" s="64"/>
-      <c r="J68" s="66"/>
-      <c r="K68" s="66"/>
-      <c r="L68" s="67"/>
+        <v>1</v>
+      </c>
+      <c r="B68" s="61" t="s">
+        <v>47</v>
+      </c>
+      <c r="C68" s="68" t="s">
+        <v>48</v>
+      </c>
+      <c r="D68" s="19"/>
+      <c r="E68" s="19"/>
+      <c r="F68" s="19"/>
+      <c r="G68" s="59"/>
+      <c r="H68" s="59"/>
+      <c r="I68" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="J68" s="20"/>
+      <c r="K68" s="20"/>
+      <c r="L68" s="27"/>
       <c r="M68" s="14"/>
     </row>
     <row r="69" spans="1:13">
       <c r="A69" s="18">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B69" s="63"/>
-      <c r="C69" s="70"/>
-      <c r="D69" s="64"/>
-      <c r="E69" s="64"/>
-      <c r="F69" s="64"/>
-      <c r="G69" s="65"/>
-      <c r="H69" s="65"/>
-      <c r="I69" s="64"/>
-      <c r="J69" s="66"/>
-      <c r="K69" s="66"/>
-      <c r="L69" s="67"/>
+        <f>A68+1</f>
+        <v>2</v>
+      </c>
+      <c r="B69" s="61" t="s">
+        <v>49</v>
+      </c>
+      <c r="C69" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="D69" s="19"/>
+      <c r="E69" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="F69" s="19"/>
+      <c r="G69" s="59"/>
+      <c r="H69" s="59"/>
+      <c r="I69" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="J69" s="20"/>
+      <c r="K69" s="20"/>
+      <c r="L69" s="27"/>
       <c r="M69" s="14"/>
     </row>
     <row r="70" spans="1:13">
       <c r="A70" s="18">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B70" s="63"/>
-      <c r="C70" s="70"/>
-      <c r="D70" s="19"/>
+        <f t="shared" ref="A70:A84" si="0">A69+1</f>
+        <v>3</v>
+      </c>
+      <c r="B70" s="62" t="s">
+        <v>52</v>
+      </c>
+      <c r="C70" s="69" t="s">
+        <v>53</v>
+      </c>
+      <c r="D70" s="19" t="s">
+        <v>54</v>
+      </c>
       <c r="E70" s="19"/>
-      <c r="F70" s="19"/>
-      <c r="G70" s="59"/>
+      <c r="F70" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G70" s="59" t="s">
+        <v>14</v>
+      </c>
       <c r="H70" s="59"/>
-      <c r="I70" s="19"/>
+      <c r="I70" s="19" t="s">
+        <v>55</v>
+      </c>
       <c r="J70" s="20"/>
       <c r="K70" s="20"/>
       <c r="L70" s="21"/>
@@ -3416,79 +3599,109 @@
     <row r="71" spans="1:13">
       <c r="A71" s="18">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B71" s="63"/>
-      <c r="C71" s="70"/>
-      <c r="D71" s="64"/>
-      <c r="E71" s="64"/>
-      <c r="F71" s="64"/>
-      <c r="G71" s="65"/>
-      <c r="H71" s="65"/>
-      <c r="I71" s="64"/>
-      <c r="J71" s="66"/>
-      <c r="K71" s="66"/>
-      <c r="L71" s="67"/>
+        <v>4</v>
+      </c>
+      <c r="B71" s="63" t="s">
+        <v>58</v>
+      </c>
+      <c r="C71" s="70" t="s">
+        <v>54</v>
+      </c>
+      <c r="D71" s="19"/>
+      <c r="E71" s="19"/>
+      <c r="F71" s="19"/>
+      <c r="G71" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="H71" s="59"/>
+      <c r="I71" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="J71" s="20"/>
+      <c r="K71" s="20"/>
+      <c r="L71" s="21"/>
       <c r="M71" s="14"/>
     </row>
     <row r="72" spans="1:13">
       <c r="A72" s="18">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B72" s="63"/>
-      <c r="C72" s="70"/>
-      <c r="D72" s="64"/>
-      <c r="E72" s="64"/>
-      <c r="F72" s="64"/>
-      <c r="G72" s="65"/>
-      <c r="H72" s="65"/>
-      <c r="I72" s="64"/>
-      <c r="J72" s="66"/>
-      <c r="K72" s="66"/>
-      <c r="L72" s="67"/>
+        <v>5</v>
+      </c>
+      <c r="B72" s="63" t="s">
+        <v>107</v>
+      </c>
+      <c r="C72" s="70" t="s">
+        <v>48</v>
+      </c>
+      <c r="D72" s="19"/>
+      <c r="E72" s="19"/>
+      <c r="F72" s="19"/>
+      <c r="G72" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="H72" s="59" t="s">
+        <v>107</v>
+      </c>
+      <c r="I72" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="J72" s="20"/>
+      <c r="K72" s="20"/>
+      <c r="L72" s="21"/>
       <c r="M72" s="14"/>
     </row>
     <row r="73" spans="1:13">
       <c r="A73" s="18">
         <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B73" s="63"/>
-      <c r="C73" s="70"/>
-      <c r="D73" s="19"/>
-      <c r="E73" s="19"/>
-      <c r="F73" s="19"/>
-      <c r="G73" s="59"/>
-      <c r="H73" s="59"/>
-      <c r="I73" s="19"/>
-      <c r="J73" s="20"/>
-      <c r="K73" s="20"/>
-      <c r="L73" s="21"/>
+        <v>6</v>
+      </c>
+      <c r="B73" s="63" t="s">
+        <v>114</v>
+      </c>
+      <c r="C73" s="70" t="s">
+        <v>48</v>
+      </c>
+      <c r="D73" s="64"/>
+      <c r="E73" s="64" t="s">
+        <v>116</v>
+      </c>
+      <c r="F73" s="64"/>
+      <c r="G73" s="65" t="s">
+        <v>14</v>
+      </c>
+      <c r="H73" s="65" t="s">
+        <v>115</v>
+      </c>
+      <c r="I73" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="J73" s="66"/>
+      <c r="K73" s="66"/>
+      <c r="L73" s="67"/>
       <c r="M73" s="14"/>
     </row>
     <row r="74" spans="1:13">
       <c r="A74" s="18">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B74" s="63"/>
       <c r="C74" s="70"/>
-      <c r="D74" s="64"/>
-      <c r="E74" s="64"/>
-      <c r="F74" s="64"/>
-      <c r="G74" s="65"/>
-      <c r="H74" s="65"/>
-      <c r="I74" s="64"/>
-      <c r="J74" s="66"/>
-      <c r="K74" s="66"/>
-      <c r="L74" s="67"/>
+      <c r="D74" s="19"/>
+      <c r="E74" s="19"/>
+      <c r="F74" s="19"/>
+      <c r="G74" s="59"/>
+      <c r="H74" s="59"/>
+      <c r="I74" s="19"/>
+      <c r="J74" s="20"/>
+      <c r="K74" s="20"/>
+      <c r="L74" s="21"/>
       <c r="M74" s="14"/>
     </row>
     <row r="75" spans="1:13">
       <c r="A75" s="18">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B75" s="63"/>
       <c r="C75" s="70"/>
@@ -3506,399 +3719,532 @@
     <row r="76" spans="1:13">
       <c r="A76" s="18">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B76" s="63"/>
       <c r="C76" s="70"/>
-      <c r="D76" s="19"/>
-      <c r="E76" s="19"/>
-      <c r="F76" s="19"/>
-      <c r="G76" s="59"/>
-      <c r="H76" s="59"/>
-      <c r="I76" s="19"/>
-      <c r="J76" s="20"/>
-      <c r="K76" s="20"/>
-      <c r="L76" s="21"/>
+      <c r="D76" s="64"/>
+      <c r="E76" s="64"/>
+      <c r="F76" s="64"/>
+      <c r="G76" s="65"/>
+      <c r="H76" s="65"/>
+      <c r="I76" s="64"/>
+      <c r="J76" s="66"/>
+      <c r="K76" s="66"/>
+      <c r="L76" s="67"/>
       <c r="M76" s="14"/>
     </row>
     <row r="77" spans="1:13">
       <c r="A77" s="18">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B77" s="63"/>
       <c r="C77" s="70"/>
-      <c r="D77" s="64"/>
-      <c r="E77" s="64"/>
-      <c r="F77" s="64"/>
-      <c r="G77" s="65"/>
-      <c r="H77" s="65"/>
-      <c r="I77" s="64"/>
-      <c r="J77" s="66"/>
-      <c r="K77" s="66"/>
-      <c r="L77" s="67"/>
+      <c r="D77" s="19"/>
+      <c r="E77" s="19"/>
+      <c r="F77" s="19"/>
+      <c r="G77" s="59"/>
+      <c r="H77" s="59"/>
+      <c r="I77" s="19"/>
+      <c r="J77" s="20"/>
+      <c r="K77" s="20"/>
+      <c r="L77" s="21"/>
       <c r="M77" s="14"/>
     </row>
     <row r="78" spans="1:13">
-      <c r="A78" s="22"/>
-      <c r="B78" s="23"/>
-      <c r="C78" s="24"/>
-      <c r="D78" s="24"/>
-      <c r="E78" s="24"/>
-      <c r="F78" s="24"/>
-      <c r="G78" s="60"/>
-      <c r="H78" s="60"/>
-      <c r="I78" s="24"/>
-      <c r="J78" s="25"/>
-      <c r="K78" s="25"/>
-      <c r="L78" s="26"/>
+      <c r="A78" s="18">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B78" s="63"/>
+      <c r="C78" s="70"/>
+      <c r="D78" s="64"/>
+      <c r="E78" s="64"/>
+      <c r="F78" s="64"/>
+      <c r="G78" s="65"/>
+      <c r="H78" s="65"/>
+      <c r="I78" s="64"/>
+      <c r="J78" s="66"/>
+      <c r="K78" s="66"/>
+      <c r="L78" s="67"/>
       <c r="M78" s="14"/>
     </row>
+    <row r="79" spans="1:13">
+      <c r="A79" s="18">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B79" s="63"/>
+      <c r="C79" s="70"/>
+      <c r="D79" s="64"/>
+      <c r="E79" s="64"/>
+      <c r="F79" s="64"/>
+      <c r="G79" s="65"/>
+      <c r="H79" s="65"/>
+      <c r="I79" s="64"/>
+      <c r="J79" s="66"/>
+      <c r="K79" s="66"/>
+      <c r="L79" s="67"/>
+      <c r="M79" s="14"/>
+    </row>
     <row r="80" spans="1:13">
-      <c r="A80" s="29" t="s">
+      <c r="A80" s="18">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B80" s="63"/>
+      <c r="C80" s="70"/>
+      <c r="D80" s="19"/>
+      <c r="E80" s="19"/>
+      <c r="F80" s="19"/>
+      <c r="G80" s="59"/>
+      <c r="H80" s="59"/>
+      <c r="I80" s="19"/>
+      <c r="J80" s="20"/>
+      <c r="K80" s="20"/>
+      <c r="L80" s="21"/>
+      <c r="M80" s="14"/>
+    </row>
+    <row r="81" spans="1:13">
+      <c r="A81" s="18">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B81" s="63"/>
+      <c r="C81" s="70"/>
+      <c r="D81" s="64"/>
+      <c r="E81" s="64"/>
+      <c r="F81" s="64"/>
+      <c r="G81" s="65"/>
+      <c r="H81" s="65"/>
+      <c r="I81" s="64"/>
+      <c r="J81" s="66"/>
+      <c r="K81" s="66"/>
+      <c r="L81" s="67"/>
+      <c r="M81" s="14"/>
+    </row>
+    <row r="82" spans="1:13">
+      <c r="A82" s="18">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B82" s="63"/>
+      <c r="C82" s="70"/>
+      <c r="D82" s="64"/>
+      <c r="E82" s="64"/>
+      <c r="F82" s="64"/>
+      <c r="G82" s="65"/>
+      <c r="H82" s="65"/>
+      <c r="I82" s="64"/>
+      <c r="J82" s="66"/>
+      <c r="K82" s="66"/>
+      <c r="L82" s="67"/>
+      <c r="M82" s="14"/>
+    </row>
+    <row r="83" spans="1:13">
+      <c r="A83" s="18">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B83" s="63"/>
+      <c r="C83" s="70"/>
+      <c r="D83" s="19"/>
+      <c r="E83" s="19"/>
+      <c r="F83" s="19"/>
+      <c r="G83" s="59"/>
+      <c r="H83" s="59"/>
+      <c r="I83" s="19"/>
+      <c r="J83" s="20"/>
+      <c r="K83" s="20"/>
+      <c r="L83" s="21"/>
+      <c r="M83" s="14"/>
+    </row>
+    <row r="84" spans="1:13">
+      <c r="A84" s="18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B84" s="63"/>
+      <c r="C84" s="70"/>
+      <c r="D84" s="64"/>
+      <c r="E84" s="64"/>
+      <c r="F84" s="64"/>
+      <c r="G84" s="65"/>
+      <c r="H84" s="65"/>
+      <c r="I84" s="64"/>
+      <c r="J84" s="66"/>
+      <c r="K84" s="66"/>
+      <c r="L84" s="67"/>
+      <c r="M84" s="14"/>
+    </row>
+    <row r="85" spans="1:13">
+      <c r="A85" s="22"/>
+      <c r="B85" s="23"/>
+      <c r="C85" s="24"/>
+      <c r="D85" s="24"/>
+      <c r="E85" s="24"/>
+      <c r="F85" s="24"/>
+      <c r="G85" s="60"/>
+      <c r="H85" s="60"/>
+      <c r="I85" s="24"/>
+      <c r="J85" s="25"/>
+      <c r="K85" s="25"/>
+      <c r="L85" s="26"/>
+      <c r="M85" s="14"/>
+    </row>
+    <row r="87" spans="1:13">
+      <c r="A87" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="B80" s="30"/>
-      <c r="C80" s="30"/>
-      <c r="D80" s="30"/>
-      <c r="E80" s="71"/>
-      <c r="F80" s="1" t="s">
+      <c r="B87" s="30"/>
+      <c r="C87" s="30"/>
+      <c r="D87" s="30"/>
+      <c r="E87" s="71"/>
+      <c r="F87" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="81" spans="1:13">
-      <c r="A81" s="39" t="s">
+    <row r="88" spans="1:13">
+      <c r="A88" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B81" s="36" t="s">
+      <c r="B88" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C81" s="36"/>
-      <c r="D81" s="36"/>
-      <c r="E81" s="72"/>
-      <c r="F81" s="57"/>
-      <c r="G81" s="57"/>
-      <c r="H81" s="57"/>
-      <c r="I81" s="57"/>
-      <c r="K81" s="37"/>
-      <c r="L81" s="37"/>
-    </row>
-    <row r="82" spans="1:13">
-      <c r="A82" s="43"/>
-      <c r="B82" s="38"/>
-      <c r="C82" s="32"/>
-      <c r="D82" s="32"/>
-      <c r="E82" s="33"/>
-      <c r="F82" s="58"/>
-      <c r="G82" s="58"/>
-      <c r="H82" s="58"/>
-      <c r="J82"/>
-      <c r="K82"/>
-      <c r="L82"/>
-    </row>
-    <row r="83" spans="1:13">
-      <c r="A83" s="43"/>
-      <c r="B83" s="38"/>
-      <c r="C83" s="34"/>
-      <c r="D83" s="34"/>
-      <c r="E83" s="35"/>
-      <c r="F83" s="58"/>
-      <c r="G83" s="58"/>
-      <c r="H83" s="58"/>
-      <c r="J83"/>
-      <c r="K83"/>
-      <c r="L83"/>
-    </row>
-    <row r="84" spans="1:13">
-      <c r="A84" s="44"/>
-      <c r="B84" s="40"/>
-      <c r="C84" s="41"/>
-      <c r="D84" s="41"/>
-      <c r="E84" s="42"/>
-      <c r="F84" s="58"/>
-      <c r="G84" s="58"/>
-      <c r="H84" s="58"/>
-      <c r="J84"/>
-      <c r="K84"/>
-      <c r="L84"/>
-    </row>
-    <row r="85" spans="1:13">
-      <c r="A85"/>
-      <c r="B85"/>
-      <c r="C85"/>
-      <c r="D85"/>
-      <c r="E85"/>
-      <c r="F85"/>
-      <c r="G85"/>
-      <c r="H85"/>
-      <c r="I85"/>
-      <c r="J85"/>
-    </row>
-    <row r="86" spans="1:13">
-      <c r="A86"/>
-      <c r="B86" t="s">
+      <c r="C88" s="36"/>
+      <c r="D88" s="36"/>
+      <c r="E88" s="72"/>
+      <c r="F88" s="57"/>
+      <c r="G88" s="57"/>
+      <c r="H88" s="57"/>
+      <c r="I88" s="57"/>
+      <c r="K88" s="37"/>
+      <c r="L88" s="37"/>
+    </row>
+    <row r="89" spans="1:13">
+      <c r="A89" s="43"/>
+      <c r="B89" s="38"/>
+      <c r="C89" s="32"/>
+      <c r="D89" s="32"/>
+      <c r="E89" s="33"/>
+      <c r="F89" s="58"/>
+      <c r="G89" s="58"/>
+      <c r="H89" s="58"/>
+      <c r="J89"/>
+      <c r="K89"/>
+      <c r="L89"/>
+    </row>
+    <row r="90" spans="1:13">
+      <c r="A90" s="43"/>
+      <c r="B90" s="38"/>
+      <c r="C90" s="34"/>
+      <c r="D90" s="34"/>
+      <c r="E90" s="35"/>
+      <c r="F90" s="58"/>
+      <c r="G90" s="58"/>
+      <c r="H90" s="58"/>
+      <c r="J90"/>
+      <c r="K90"/>
+      <c r="L90"/>
+    </row>
+    <row r="91" spans="1:13">
+      <c r="A91" s="44"/>
+      <c r="B91" s="40"/>
+      <c r="C91" s="41"/>
+      <c r="D91" s="41"/>
+      <c r="E91" s="42"/>
+      <c r="F91" s="58"/>
+      <c r="G91" s="58"/>
+      <c r="H91" s="58"/>
+      <c r="J91"/>
+      <c r="K91"/>
+      <c r="L91"/>
+    </row>
+    <row r="92" spans="1:13">
+      <c r="A92"/>
+      <c r="B92"/>
+      <c r="C92"/>
+      <c r="D92"/>
+      <c r="E92"/>
+      <c r="F92"/>
+      <c r="G92"/>
+      <c r="H92"/>
+      <c r="I92"/>
+      <c r="J92"/>
+    </row>
+    <row r="93" spans="1:13">
+      <c r="A93"/>
+      <c r="B93" t="s">
         <v>85</v>
       </c>
-      <c r="C86"/>
-      <c r="D86"/>
-      <c r="E86"/>
-      <c r="F86"/>
-      <c r="G86"/>
-      <c r="H86"/>
-      <c r="I86"/>
-      <c r="J86"/>
-    </row>
-    <row r="87" spans="1:13">
-      <c r="A87" s="3" t="s">
+      <c r="C93"/>
+      <c r="D93"/>
+      <c r="E93"/>
+      <c r="F93"/>
+      <c r="G93"/>
+      <c r="H93"/>
+      <c r="I93"/>
+      <c r="J93"/>
+    </row>
+    <row r="94" spans="1:13">
+      <c r="A94" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B87" s="13"/>
-      <c r="C87" s="13"/>
-      <c r="D87" s="13"/>
-      <c r="E87" s="13"/>
-      <c r="F87" s="13"/>
-      <c r="G87" s="13"/>
-      <c r="H87" s="13"/>
-      <c r="I87" s="13"/>
-      <c r="J87" s="13"/>
-      <c r="K87" s="13"/>
-      <c r="L87" s="6"/>
-      <c r="M87" s="14"/>
-    </row>
-    <row r="88" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A88" s="94" t="s">
+      <c r="B94" s="13"/>
+      <c r="C94" s="13"/>
+      <c r="D94" s="13"/>
+      <c r="E94" s="13"/>
+      <c r="F94" s="13"/>
+      <c r="G94" s="13"/>
+      <c r="H94" s="13"/>
+      <c r="I94" s="13"/>
+      <c r="J94" s="13"/>
+      <c r="K94" s="13"/>
+      <c r="L94" s="6"/>
+      <c r="M94" s="14"/>
+    </row>
+    <row r="95" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A95" s="113" t="s">
         <v>7</v>
       </c>
-      <c r="B88" s="94" t="s">
+      <c r="B95" s="113" t="s">
         <v>84</v>
       </c>
-      <c r="C88" s="91" t="s">
+      <c r="C95" s="112" t="s">
         <v>86</v>
       </c>
-      <c r="D88" s="91" t="s">
+      <c r="D95" s="112" t="s">
         <v>87</v>
       </c>
-      <c r="E88" s="91" t="s">
+      <c r="E95" s="112" t="s">
         <v>81</v>
       </c>
-      <c r="F88" s="88"/>
-      <c r="G88" s="88"/>
-      <c r="H88" s="88"/>
-      <c r="I88" s="90"/>
-      <c r="J88" s="91"/>
-      <c r="K88" s="15"/>
-      <c r="L88" s="16"/>
-      <c r="M88" s="9"/>
-    </row>
-    <row r="89" spans="1:13">
-      <c r="A89" s="94"/>
-      <c r="B89" s="94"/>
-      <c r="C89" s="91"/>
-      <c r="D89" s="91"/>
-      <c r="E89" s="91"/>
-      <c r="F89" s="89"/>
-      <c r="G89" s="89"/>
-      <c r="H89" s="89"/>
-      <c r="I89" s="90"/>
-      <c r="J89" s="91"/>
-      <c r="K89" s="17"/>
-      <c r="L89" s="28"/>
-      <c r="M89" s="14"/>
-    </row>
-    <row r="90" spans="1:13">
-      <c r="A90" s="18">
+      <c r="F95" s="123"/>
+      <c r="G95" s="123"/>
+      <c r="H95" s="123"/>
+      <c r="I95" s="125"/>
+      <c r="J95" s="112"/>
+      <c r="K95" s="15"/>
+      <c r="L95" s="16"/>
+      <c r="M95" s="9"/>
+    </row>
+    <row r="96" spans="1:13">
+      <c r="A96" s="113"/>
+      <c r="B96" s="113"/>
+      <c r="C96" s="112"/>
+      <c r="D96" s="112"/>
+      <c r="E96" s="112"/>
+      <c r="F96" s="124"/>
+      <c r="G96" s="124"/>
+      <c r="H96" s="124"/>
+      <c r="I96" s="125"/>
+      <c r="J96" s="112"/>
+      <c r="K96" s="17"/>
+      <c r="L96" s="28"/>
+      <c r="M96" s="14"/>
+    </row>
+    <row r="97" spans="1:13">
+      <c r="A97" s="18">
         <v>1</v>
       </c>
-      <c r="B90" s="61" t="s">
+      <c r="B97" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="C90" s="68" t="s">
+      <c r="C97" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="D90" s="19"/>
-      <c r="E90" s="19" t="s">
+      <c r="D97" s="19"/>
+      <c r="E97" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="F90" s="77"/>
-      <c r="G90" s="79"/>
-      <c r="H90" s="79"/>
-      <c r="I90" s="77"/>
-      <c r="J90" s="20"/>
-      <c r="K90" s="20"/>
-      <c r="L90" s="27"/>
-      <c r="M90" s="14"/>
-    </row>
-    <row r="91" spans="1:13">
-      <c r="A91" s="18">
-        <f>A90+1</f>
+      <c r="F97" s="77"/>
+      <c r="G97" s="79"/>
+      <c r="H97" s="79"/>
+      <c r="I97" s="77"/>
+      <c r="J97" s="20"/>
+      <c r="K97" s="20"/>
+      <c r="L97" s="27"/>
+      <c r="M97" s="14"/>
+    </row>
+    <row r="98" spans="1:13">
+      <c r="A98" s="18">
+        <f>A97+1</f>
         <v>2</v>
       </c>
-      <c r="B91" s="61" t="s">
+      <c r="B98" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="C91" s="68" t="s">
+      <c r="C98" s="68" t="s">
         <v>90</v>
       </c>
-      <c r="D91" s="19"/>
-      <c r="E91" s="19" t="s">
+      <c r="D98" s="19"/>
+      <c r="E98" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="F91" s="77"/>
-      <c r="G91" s="79"/>
-      <c r="H91" s="79"/>
-      <c r="I91" s="77"/>
-      <c r="J91" s="20"/>
-      <c r="K91" s="20"/>
-      <c r="L91" s="27"/>
-      <c r="M91" s="14"/>
-    </row>
-    <row r="92" spans="1:13">
-      <c r="A92" s="18">
-        <f t="shared" ref="A92:A96" si="1">A91+1</f>
+      <c r="F98" s="77"/>
+      <c r="G98" s="79"/>
+      <c r="H98" s="79"/>
+      <c r="I98" s="77"/>
+      <c r="J98" s="20"/>
+      <c r="K98" s="20"/>
+      <c r="L98" s="27"/>
+      <c r="M98" s="14"/>
+    </row>
+    <row r="99" spans="1:13">
+      <c r="A99" s="18">
+        <f t="shared" ref="A99:A103" si="1">A98+1</f>
         <v>3</v>
       </c>
-      <c r="B92" s="62" t="s">
+      <c r="B99" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="C92" s="69" t="s">
+      <c r="C99" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="D92" s="19" t="s">
+      <c r="D99" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="E92" s="19" t="s">
+      <c r="E99" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="F92" s="77"/>
-      <c r="G92" s="79"/>
-      <c r="H92" s="79"/>
-      <c r="I92" s="77"/>
-      <c r="J92" s="20"/>
-      <c r="K92" s="20"/>
-      <c r="L92" s="21"/>
-      <c r="M92" s="14"/>
-    </row>
-    <row r="93" spans="1:13">
-      <c r="A93" s="18">
+      <c r="F99" s="77"/>
+      <c r="G99" s="79"/>
+      <c r="H99" s="79"/>
+      <c r="I99" s="77"/>
+      <c r="J99" s="20"/>
+      <c r="K99" s="20"/>
+      <c r="L99" s="21"/>
+      <c r="M99" s="14"/>
+    </row>
+    <row r="100" spans="1:13">
+      <c r="A100" s="18">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B93" s="63"/>
-      <c r="C93" s="70"/>
-      <c r="D93" s="19"/>
-      <c r="E93" s="19"/>
-      <c r="F93" s="77"/>
-      <c r="G93" s="79"/>
-      <c r="H93" s="79"/>
-      <c r="I93" s="77"/>
-      <c r="J93" s="20"/>
-      <c r="K93" s="20"/>
-      <c r="L93" s="21"/>
-      <c r="M93" s="14"/>
-    </row>
-    <row r="94" spans="1:13">
-      <c r="A94" s="18">
+      <c r="B100" s="63"/>
+      <c r="C100" s="70"/>
+      <c r="D100" s="19"/>
+      <c r="E100" s="19"/>
+      <c r="F100" s="77"/>
+      <c r="G100" s="79"/>
+      <c r="H100" s="79"/>
+      <c r="I100" s="77"/>
+      <c r="J100" s="20"/>
+      <c r="K100" s="20"/>
+      <c r="L100" s="21"/>
+      <c r="M100" s="14"/>
+    </row>
+    <row r="101" spans="1:13">
+      <c r="A101" s="18">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B94" s="63"/>
-      <c r="C94" s="70"/>
-      <c r="D94" s="19"/>
-      <c r="E94" s="19"/>
-      <c r="F94" s="77"/>
-      <c r="G94" s="79"/>
-      <c r="H94" s="79"/>
-      <c r="I94" s="77"/>
-      <c r="J94" s="20"/>
-      <c r="K94" s="20"/>
-      <c r="L94" s="21"/>
-      <c r="M94" s="14"/>
-    </row>
-    <row r="95" spans="1:13">
-      <c r="A95" s="18">
+      <c r="B101" s="63"/>
+      <c r="C101" s="70"/>
+      <c r="D101" s="19"/>
+      <c r="E101" s="19"/>
+      <c r="F101" s="77"/>
+      <c r="G101" s="79"/>
+      <c r="H101" s="79"/>
+      <c r="I101" s="77"/>
+      <c r="J101" s="20"/>
+      <c r="K101" s="20"/>
+      <c r="L101" s="21"/>
+      <c r="M101" s="14"/>
+    </row>
+    <row r="102" spans="1:13">
+      <c r="A102" s="18">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B95" s="63"/>
-      <c r="C95" s="70"/>
-      <c r="D95" s="64"/>
-      <c r="E95" s="64"/>
-      <c r="F95" s="78"/>
-      <c r="G95" s="80"/>
-      <c r="H95" s="80"/>
-      <c r="I95" s="78"/>
-      <c r="J95" s="66"/>
-      <c r="K95" s="66"/>
-      <c r="L95" s="67"/>
-      <c r="M95" s="14"/>
-    </row>
-    <row r="96" spans="1:13">
-      <c r="A96" s="18">
+      <c r="B102" s="63"/>
+      <c r="C102" s="70"/>
+      <c r="D102" s="64"/>
+      <c r="E102" s="64"/>
+      <c r="F102" s="78"/>
+      <c r="G102" s="80"/>
+      <c r="H102" s="80"/>
+      <c r="I102" s="78"/>
+      <c r="J102" s="66"/>
+      <c r="K102" s="66"/>
+      <c r="L102" s="67"/>
+      <c r="M102" s="14"/>
+    </row>
+    <row r="103" spans="1:13">
+      <c r="A103" s="18">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B96" s="63"/>
-      <c r="C96" s="70"/>
-      <c r="D96" s="19"/>
-      <c r="E96" s="19"/>
-      <c r="F96" s="77"/>
-      <c r="G96" s="79"/>
-      <c r="H96" s="79"/>
-      <c r="I96" s="77"/>
-      <c r="J96" s="20"/>
-      <c r="K96" s="20"/>
-      <c r="L96" s="21"/>
-      <c r="M96" s="14"/>
+      <c r="B103" s="63"/>
+      <c r="C103" s="70"/>
+      <c r="D103" s="19"/>
+      <c r="E103" s="19"/>
+      <c r="F103" s="77"/>
+      <c r="G103" s="79"/>
+      <c r="H103" s="79"/>
+      <c r="I103" s="77"/>
+      <c r="J103" s="20"/>
+      <c r="K103" s="20"/>
+      <c r="L103" s="21"/>
+      <c r="M103" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="I59:J60"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="E59:E60"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="H59:H60"/>
-    <mergeCell ref="F59:F60"/>
-    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="F95:F96"/>
+    <mergeCell ref="H95:H96"/>
+    <mergeCell ref="I95:J96"/>
+    <mergeCell ref="G66:G67"/>
+    <mergeCell ref="G95:G96"/>
+    <mergeCell ref="A95:A96"/>
+    <mergeCell ref="B95:B96"/>
+    <mergeCell ref="C95:C96"/>
+    <mergeCell ref="D95:D96"/>
+    <mergeCell ref="E95:E96"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="C14:E14"/>
-    <mergeCell ref="A88:A89"/>
-    <mergeCell ref="B88:B89"/>
-    <mergeCell ref="C88:C89"/>
-    <mergeCell ref="D88:D89"/>
-    <mergeCell ref="E88:E89"/>
-    <mergeCell ref="F88:F89"/>
-    <mergeCell ref="H88:H89"/>
-    <mergeCell ref="I88:J89"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="G88:G89"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="I66:J67"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="E66:E67"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="H66:H67"/>
+    <mergeCell ref="F66:F67"/>
+    <mergeCell ref="A26:B26"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
-  <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E100:H100" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="8">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E107:H107" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C24:C25" xr:uid="{78FE03A8-B82F-DD42-A5B2-F5AED31EB8E5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C25:C26" xr:uid="{78FE03A8-B82F-DD42-A5B2-F5AED31EB8E5}">
       <formula1>adjustFiledName</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16" xr:uid="{0933AF92-3C0C-2F47-AF58-F84946F39270}">
       <formula1>componentKind</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C17:C22 F61:G78" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F68:G85 C17 C19:C23" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
       <formula1>yesNo</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C23" xr:uid="{CCFC1331-CEEF-574E-9BCC-37D38F486896}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C24" xr:uid="{CCFC1331-CEEF-574E-9BCC-37D38F486896}">
       <formula1>adjustFieldName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C47:C49" xr:uid="{BDE40890-40F7-4E41-B7E1-478CEBD85557}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C54:C56" xr:uid="{BDE40890-40F7-4E41-B7E1-478CEBD85557}">
       <formula1>httpdMethod</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18" xr:uid="{B3BDB514-7849-7346-B29F-0809D4138732}">
+      <formula1>layoutType</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C28:C33" xr:uid="{D073ACF5-A392-2348-B361-3D576C1BA990}">
+      <formula1>adjustFiledName</formula1>
+      <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.59027777777777779" right="0.59027777777777779" top="0.59027777777777779" bottom="0.59027777777777779" header="0.51180555555555562" footer="0.11805555555555557"/>
@@ -3914,10 +4260,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -3927,13 +4273,13 @@
     <col min="5" max="5" width="8.83203125" style="47" customWidth="1"/>
     <col min="6" max="6" width="18.5" style="47" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.83203125" style="47" customWidth="1"/>
-    <col min="8" max="8" width="18.5" style="47" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" style="47" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.83203125" style="47" customWidth="1"/>
     <col min="10" max="10" width="18.6640625" style="47" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.83203125" style="47" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" style="47" bestFit="1" customWidth="1"/>
-    <col min="13" max="253" width="8.83203125" style="47" customWidth="1"/>
-    <col min="254" max="16384" width="10.83203125" style="47"/>
+    <col min="12" max="12" width="14" style="47" customWidth="1"/>
+    <col min="13" max="251" width="8.83203125" style="47" customWidth="1"/>
+    <col min="252" max="16384" width="10.83203125" style="47"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19">
@@ -3948,11 +4294,10 @@
       <c r="G1" s="45"/>
       <c r="H1" s="45"/>
       <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="46" t="s">
+      <c r="J1" s="46" t="s">
         <v>9</v>
       </c>
+      <c r="L1" s="45"/>
     </row>
     <row r="3" spans="1:12">
       <c r="B3" s="48" t="s">
@@ -3962,16 +4307,16 @@
         <v>31</v>
       </c>
       <c r="F3" s="48" t="s">
-        <v>110</v>
+        <v>10</v>
       </c>
       <c r="H3" s="48" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J3" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="L3" s="48" t="s">
         <v>12</v>
+      </c>
+      <c r="L3" s="87" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -3981,18 +4326,18 @@
       <c r="D4" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="81"/>
+      <c r="F4" s="50"/>
       <c r="H4" s="50"/>
       <c r="J4" s="50"/>
-      <c r="L4" s="50"/>
+      <c r="L4" s="88"/>
     </row>
     <row r="5" spans="1:12">
       <c r="B5" s="51" t="s">
         <v>28</v>
       </c>
       <c r="D5" s="52"/>
-      <c r="F5" s="82" t="s">
-        <v>111</v>
+      <c r="F5" s="52" t="s">
+        <v>13</v>
       </c>
       <c r="H5" s="52" t="s">
         <v>13</v>
@@ -4000,24 +4345,19 @@
       <c r="J5" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="52" t="s">
-        <v>13</v>
+      <c r="L5" s="88" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="B6" s="53"/>
-      <c r="F6" s="82" t="s">
-        <v>112</v>
+      <c r="L6" s="51" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="F7" s="83" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="F8" s="84" t="s">
-        <v>114</v>
+      <c r="L7" s="89" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3.0.5: Enable BreadCrumbs issue.
</commit_message>
<xml_diff>
--- a/meta/components/PlainBoxSample.xlsx
+++ b/meta/components/PlainBoxSample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoVueComponent/meta/components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BFEF66-DEBE-254E-B8A0-7FEFD3F8A9FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D359E9F-CBEA-204D-9594-0F9E4F2F80E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9860" yWindow="7560" windowWidth="25200" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
     <definedName name="layoutType">config!$L$3:$L$7</definedName>
     <definedName name="yesNo">config!$D$4:$D$5</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="131">
   <si>
     <t>パッケージ</t>
   </si>
@@ -1022,18 +1022,22 @@
     <t>No.</t>
   </si>
   <si>
-    <t>コンポーネント別名</t>
-    <rPh sb="7" eb="9">
-      <t>ベツメイ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>HOME</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>ボックスサンプルプレイン</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>リンク無し</t>
+    <rPh sb="3" eb="4">
+      <t xml:space="preserve">ナシ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>○</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1155,7 +1159,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="60">
+  <borders count="62">
     <border>
       <left/>
       <right/>
@@ -1898,12 +1902,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2160,6 +2190,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -2573,8 +2606,8 @@
   </sheetPr>
   <dimension ref="A1:M103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2651,7 +2684,7 @@
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="8"/>
@@ -2952,9 +2985,11 @@
         <v>126</v>
       </c>
       <c r="B29" s="94" t="s">
-        <v>127</v>
-      </c>
-      <c r="C29" s="94"/>
+        <v>57</v>
+      </c>
+      <c r="C29" s="84" t="s">
+        <v>129</v>
+      </c>
       <c r="D29" s="94"/>
       <c r="E29" s="95"/>
       <c r="F29" s="57"/>
@@ -2969,9 +3004,9 @@
         <v>1</v>
       </c>
       <c r="B30" s="97" t="s">
-        <v>128</v>
-      </c>
-      <c r="C30" s="98"/>
+        <v>127</v>
+      </c>
+      <c r="C30" s="126"/>
       <c r="D30" s="98"/>
       <c r="E30" s="99"/>
       <c r="F30" s="58"/>
@@ -2982,9 +3017,15 @@
       <c r="L30"/>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="96"/>
-      <c r="B31" s="97"/>
-      <c r="C31" s="100"/>
+      <c r="A31" s="96">
+        <v>2</v>
+      </c>
+      <c r="B31" s="97" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="127" t="s">
+        <v>130</v>
+      </c>
       <c r="D31" s="100"/>
       <c r="E31" s="101"/>
       <c r="F31" s="58"/>
@@ -2997,7 +3038,7 @@
     <row r="32" spans="1:12">
       <c r="A32" s="102"/>
       <c r="B32" s="103"/>
-      <c r="C32" s="104"/>
+      <c r="C32" s="128"/>
       <c r="D32" s="104"/>
       <c r="E32" s="105"/>
       <c r="F32" s="58"/>

</xml_diff>

<commit_message>
3.0.8: Implement pathString option to props. It's enable to bind path parameters to props. Specify path parameter string in the column, like as query parameter strings.
</commit_message>
<xml_diff>
--- a/meta/components/PlainBoxSample.xlsx
+++ b/meta/components/PlainBoxSample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoVueComponent/meta/components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D359E9F-CBEA-204D-9594-0F9E4F2F80E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4D7294-018A-8C44-8774-D92BB04B4B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9860" yWindow="7560" windowWidth="25200" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
     <definedName name="layoutType">config!$L$3:$L$7</definedName>
     <definedName name="yesNo">config!$D$4:$D$5</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="132">
   <si>
     <t>パッケージ</t>
   </si>
@@ -952,19 +952,11 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>/plainbox</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>plainbox</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>fuga</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>fur</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
@@ -1038,6 +1030,18 @@
   </si>
   <si>
     <t>○</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>/plainbox/:secret?</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>パス文字列</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>sec</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -2142,57 +2146,57 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -2604,10 +2608,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M103"/>
+  <dimension ref="A1:N103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="I73" sqref="I73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2615,33 +2619,33 @@
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
     <col min="2" max="5" width="23.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.5" style="1" customWidth="1"/>
-    <col min="7" max="8" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="6.83203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="28" style="1" customWidth="1"/>
-    <col min="12" max="12" width="33.33203125" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9" style="1"/>
+    <col min="7" max="9" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.1640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="6.83203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="28" style="1" customWidth="1"/>
+    <col min="13" max="13" width="33.33203125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19">
+    <row r="1" spans="1:12" ht="19">
       <c r="A1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:12">
       <c r="B2" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:12">
       <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:12">
       <c r="A5" s="3" t="s">
         <v>95</v>
       </c>
@@ -2650,7 +2654,7 @@
       <c r="D5" s="4"/>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:12">
       <c r="A6" s="3" t="s">
         <v>57</v>
       </c>
@@ -2664,7 +2668,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:12">
       <c r="A7" s="3" t="s">
         <v>66</v>
       </c>
@@ -2678,13 +2682,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:12">
       <c r="A8" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="8"/>
@@ -2692,7 +2696,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:12">
       <c r="A9" s="3" t="s">
         <v>0</v>
       </c>
@@ -2706,13 +2710,13 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="118" t="s">
+    <row r="10" spans="1:12">
+      <c r="A10" s="120" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="119"/>
+      <c r="B10" s="121"/>
       <c r="C10" s="10" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="D10" s="31"/>
       <c r="E10" s="11"/>
@@ -2720,13 +2724,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="118" t="s">
+    <row r="11" spans="1:12">
+      <c r="A11" s="120" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="119"/>
+      <c r="B11" s="121"/>
       <c r="C11" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D11" s="31"/>
       <c r="E11" s="11"/>
@@ -2734,11 +2738,11 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="118" t="s">
+    <row r="12" spans="1:12">
+      <c r="A12" s="120" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="119"/>
+      <c r="B12" s="121"/>
       <c r="C12" s="10" t="s">
         <v>21</v>
       </c>
@@ -2748,11 +2752,11 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="118" t="s">
+    <row r="13" spans="1:12">
+      <c r="A13" s="120" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="119"/>
+      <c r="B13" s="121"/>
       <c r="C13" s="76" t="s">
         <v>63</v>
       </c>
@@ -2762,21 +2766,22 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="45" customHeight="1">
+    <row r="14" spans="1:12" ht="45" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="120" t="s">
+      <c r="C14" s="122" t="s">
         <v>71</v>
       </c>
-      <c r="D14" s="121"/>
-      <c r="E14" s="122"/>
+      <c r="D14" s="123"/>
+      <c r="E14" s="124"/>
       <c r="F14" s="56"/>
       <c r="G14" s="56"/>
       <c r="H14" s="56"/>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="I14" s="56"/>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="3" t="s">
         <v>2</v>
       </c>
@@ -2787,7 +2792,7 @@
       <c r="D15" s="12"/>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:12">
       <c r="A16" s="54" t="s">
         <v>25</v>
       </c>
@@ -2803,8 +2808,9 @@
       <c r="G16"/>
       <c r="H16"/>
       <c r="I16"/>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="J16"/>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" s="54" t="s">
         <v>37</v>
       </c>
@@ -2820,22 +2826,24 @@
       <c r="G17"/>
       <c r="H17"/>
       <c r="I17"/>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="J17"/>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="84" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B18" s="85"/>
       <c r="C18" s="86" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D18" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G18"/>
       <c r="H18"/>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="I18"/>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" s="54" t="s">
         <v>38</v>
       </c>
@@ -2849,8 +2857,9 @@
       <c r="G19"/>
       <c r="H19"/>
       <c r="I19"/>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="J19"/>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" s="54" t="s">
         <v>29</v>
       </c>
@@ -2866,8 +2875,9 @@
       <c r="G20"/>
       <c r="H20"/>
       <c r="I20"/>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="J20"/>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21" s="54" t="s">
         <v>46</v>
       </c>
@@ -2883,8 +2893,9 @@
       <c r="G21"/>
       <c r="H21"/>
       <c r="I21"/>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="J21"/>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" s="54" t="s">
         <v>76</v>
       </c>
@@ -2900,12 +2911,13 @@
       <c r="G22"/>
       <c r="H22"/>
       <c r="I22"/>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="A23" s="110" t="s">
+      <c r="J22"/>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="125" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="111"/>
+      <c r="B23" s="126"/>
       <c r="C23" s="55" t="s">
         <v>14</v>
       </c>
@@ -2917,8 +2929,9 @@
       <c r="G23"/>
       <c r="H23"/>
       <c r="I23"/>
-    </row>
-    <row r="24" spans="1:12">
+      <c r="J23"/>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" s="54" t="s">
         <v>15</v>
       </c>
@@ -2932,12 +2945,13 @@
       <c r="G24"/>
       <c r="H24"/>
       <c r="I24"/>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="A25" s="110" t="s">
+      <c r="J24"/>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="125" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="111"/>
+      <c r="B25" s="126"/>
       <c r="C25" s="55" t="s">
         <v>14</v>
       </c>
@@ -2949,12 +2963,13 @@
       <c r="G25"/>
       <c r="H25"/>
       <c r="I25"/>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26" s="110" t="s">
+      <c r="J25"/>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="125" t="s">
         <v>64</v>
       </c>
-      <c r="B26" s="111"/>
+      <c r="B26" s="126"/>
       <c r="C26" s="55" t="s">
         <v>14</v>
       </c>
@@ -2964,31 +2979,32 @@
       <c r="G26"/>
       <c r="H26"/>
       <c r="I26"/>
-    </row>
-    <row r="27" spans="1:12">
+      <c r="J26"/>
+    </row>
+    <row r="27" spans="1:13">
       <c r="B27"/>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:13">
       <c r="A28" s="90" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B28" s="91"/>
       <c r="C28" s="91"/>
       <c r="D28" s="91"/>
       <c r="E28" s="92"/>
       <c r="F28" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29" s="93" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B29" s="94" t="s">
         <v>57</v>
       </c>
       <c r="C29" s="84" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D29" s="94"/>
       <c r="E29" s="95"/>
@@ -2996,66 +3012,71 @@
       <c r="G29" s="57"/>
       <c r="H29" s="57"/>
       <c r="I29" s="57"/>
-      <c r="K29" s="37"/>
+      <c r="J29" s="57"/>
       <c r="L29" s="37"/>
-    </row>
-    <row r="30" spans="1:12">
+      <c r="M29" s="37"/>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30" s="96">
         <v>1</v>
       </c>
       <c r="B30" s="97" t="s">
-        <v>127</v>
-      </c>
-      <c r="C30" s="126"/>
+        <v>125</v>
+      </c>
+      <c r="C30" s="110"/>
       <c r="D30" s="98"/>
       <c r="E30" s="99"/>
       <c r="F30" s="58"/>
       <c r="G30" s="58"/>
       <c r="H30" s="58"/>
-      <c r="J30"/>
+      <c r="I30" s="58"/>
       <c r="K30"/>
       <c r="L30"/>
-    </row>
-    <row r="31" spans="1:12">
+      <c r="M30"/>
+    </row>
+    <row r="31" spans="1:13">
       <c r="A31" s="96">
         <v>2</v>
       </c>
       <c r="B31" s="97" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="127" t="s">
-        <v>130</v>
+      <c r="C31" s="111" t="s">
+        <v>128</v>
       </c>
       <c r="D31" s="100"/>
       <c r="E31" s="101"/>
       <c r="F31" s="58"/>
       <c r="G31" s="58"/>
       <c r="H31" s="58"/>
-      <c r="J31"/>
+      <c r="I31" s="58"/>
       <c r="K31"/>
       <c r="L31"/>
-    </row>
-    <row r="32" spans="1:12">
+      <c r="M31"/>
+    </row>
+    <row r="32" spans="1:13">
       <c r="A32" s="102"/>
       <c r="B32" s="103"/>
-      <c r="C32" s="128"/>
+      <c r="C32" s="112"/>
       <c r="D32" s="104"/>
       <c r="E32" s="105"/>
       <c r="F32" s="58"/>
       <c r="G32" s="58"/>
       <c r="H32" s="58"/>
-      <c r="J32"/>
+      <c r="I32" s="58"/>
       <c r="K32"/>
       <c r="L32"/>
-    </row>
-    <row r="33" spans="1:12" s="108" customFormat="1">
+      <c r="M32"/>
+    </row>
+    <row r="33" spans="1:13" s="108" customFormat="1">
       <c r="A33" s="106"/>
       <c r="B33" s="106"/>
       <c r="C33" s="107"/>
       <c r="G33" s="109"/>
       <c r="H33" s="109"/>
-    </row>
-    <row r="34" spans="1:12">
+      <c r="I33" s="109"/>
+    </row>
+    <row r="34" spans="1:13">
       <c r="A34" s="29" t="s">
         <v>92</v>
       </c>
@@ -3067,7 +3088,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:13">
       <c r="A35" s="39" t="s">
         <v>7</v>
       </c>
@@ -3081,10 +3102,11 @@
       <c r="G35" s="57"/>
       <c r="H35" s="57"/>
       <c r="I35" s="57"/>
-      <c r="K35" s="37"/>
+      <c r="J35" s="57"/>
       <c r="L35" s="37"/>
-    </row>
-    <row r="36" spans="1:12">
+      <c r="M35" s="37"/>
+    </row>
+    <row r="36" spans="1:13">
       <c r="A36" s="43">
         <v>1</v>
       </c>
@@ -3097,11 +3119,12 @@
       <c r="F36" s="58"/>
       <c r="G36" s="58"/>
       <c r="H36" s="58"/>
-      <c r="J36"/>
+      <c r="I36" s="58"/>
       <c r="K36"/>
       <c r="L36"/>
-    </row>
-    <row r="37" spans="1:12">
+      <c r="M36"/>
+    </row>
+    <row r="37" spans="1:13">
       <c r="A37" s="43">
         <v>2</v>
       </c>
@@ -3114,11 +3137,12 @@
       <c r="F37" s="58"/>
       <c r="G37" s="58"/>
       <c r="H37" s="58"/>
-      <c r="J37"/>
+      <c r="I37" s="58"/>
       <c r="K37"/>
       <c r="L37"/>
-    </row>
-    <row r="38" spans="1:12">
+      <c r="M37"/>
+    </row>
+    <row r="38" spans="1:13">
       <c r="A38" s="44"/>
       <c r="B38" s="40"/>
       <c r="C38" s="41"/>
@@ -3127,11 +3151,12 @@
       <c r="F38" s="58"/>
       <c r="G38" s="58"/>
       <c r="H38" s="58"/>
-      <c r="J38"/>
+      <c r="I38" s="58"/>
       <c r="K38"/>
       <c r="L38"/>
-    </row>
-    <row r="39" spans="1:12">
+      <c r="M38"/>
+    </row>
+    <row r="39" spans="1:13">
       <c r="A39"/>
       <c r="B39"/>
       <c r="C39"/>
@@ -3142,8 +3167,9 @@
       <c r="H39"/>
       <c r="I39"/>
       <c r="J39"/>
-    </row>
-    <row r="40" spans="1:12">
+      <c r="K39"/>
+    </row>
+    <row r="40" spans="1:13">
       <c r="A40" s="29" t="s">
         <v>34</v>
       </c>
@@ -3155,7 +3181,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:13">
       <c r="A41" s="39" t="s">
         <v>7</v>
       </c>
@@ -3169,10 +3195,11 @@
       <c r="G41" s="57"/>
       <c r="H41" s="57"/>
       <c r="I41" s="57"/>
-      <c r="K41" s="37"/>
+      <c r="J41" s="57"/>
       <c r="L41" s="37"/>
-    </row>
-    <row r="42" spans="1:12">
+      <c r="M41" s="37"/>
+    </row>
+    <row r="42" spans="1:13">
       <c r="A42" s="43">
         <v>1</v>
       </c>
@@ -3185,11 +3212,12 @@
       <c r="F42" s="58"/>
       <c r="G42" s="58"/>
       <c r="H42" s="58"/>
-      <c r="J42"/>
+      <c r="I42" s="58"/>
       <c r="K42"/>
       <c r="L42"/>
-    </row>
-    <row r="43" spans="1:12">
+      <c r="M42"/>
+    </row>
+    <row r="43" spans="1:13">
       <c r="A43" s="43">
         <v>2</v>
       </c>
@@ -3202,11 +3230,12 @@
       <c r="F43" s="58"/>
       <c r="G43" s="58"/>
       <c r="H43" s="58"/>
-      <c r="J43"/>
+      <c r="I43" s="58"/>
       <c r="K43"/>
       <c r="L43"/>
-    </row>
-    <row r="44" spans="1:12">
+      <c r="M43"/>
+    </row>
+    <row r="44" spans="1:13">
       <c r="A44" s="44"/>
       <c r="B44" s="40"/>
       <c r="C44" s="41"/>
@@ -3215,11 +3244,12 @@
       <c r="F44" s="58"/>
       <c r="G44" s="58"/>
       <c r="H44" s="58"/>
-      <c r="J44"/>
+      <c r="I44" s="58"/>
       <c r="K44"/>
       <c r="L44"/>
-    </row>
-    <row r="45" spans="1:12">
+      <c r="M44"/>
+    </row>
+    <row r="45" spans="1:13">
       <c r="A45" s="73"/>
       <c r="B45" s="74"/>
       <c r="C45" s="75"/>
@@ -3228,11 +3258,12 @@
       <c r="F45" s="58"/>
       <c r="G45" s="58"/>
       <c r="H45" s="58"/>
-      <c r="J45"/>
+      <c r="I45" s="58"/>
       <c r="K45"/>
       <c r="L45"/>
-    </row>
-    <row r="46" spans="1:12">
+      <c r="M45"/>
+    </row>
+    <row r="46" spans="1:13">
       <c r="A46" s="29" t="s">
         <v>93</v>
       </c>
@@ -3244,7 +3275,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:13">
       <c r="A47" s="39" t="s">
         <v>7</v>
       </c>
@@ -3258,10 +3289,11 @@
       <c r="G47" s="57"/>
       <c r="H47" s="57"/>
       <c r="I47" s="57"/>
-      <c r="K47" s="37"/>
+      <c r="J47" s="57"/>
       <c r="L47" s="37"/>
-    </row>
-    <row r="48" spans="1:12">
+      <c r="M47" s="37"/>
+    </row>
+    <row r="48" spans="1:13">
       <c r="A48" s="43"/>
       <c r="B48" s="38"/>
       <c r="C48" s="32"/>
@@ -3270,11 +3302,12 @@
       <c r="F48" s="58"/>
       <c r="G48" s="58"/>
       <c r="H48" s="58"/>
-      <c r="J48"/>
+      <c r="I48" s="58"/>
       <c r="K48"/>
       <c r="L48"/>
-    </row>
-    <row r="49" spans="1:12">
+      <c r="M48"/>
+    </row>
+    <row r="49" spans="1:13">
       <c r="A49" s="43"/>
       <c r="B49" s="38"/>
       <c r="C49" s="34"/>
@@ -3283,11 +3316,12 @@
       <c r="F49" s="58"/>
       <c r="G49" s="58"/>
       <c r="H49" s="58"/>
-      <c r="J49"/>
+      <c r="I49" s="58"/>
       <c r="K49"/>
       <c r="L49"/>
-    </row>
-    <row r="50" spans="1:12">
+      <c r="M49"/>
+    </row>
+    <row r="50" spans="1:13">
       <c r="A50" s="44"/>
       <c r="B50" s="40"/>
       <c r="C50" s="41"/>
@@ -3296,11 +3330,12 @@
       <c r="F50" s="58"/>
       <c r="G50" s="58"/>
       <c r="H50" s="58"/>
-      <c r="J50"/>
+      <c r="I50" s="58"/>
       <c r="K50"/>
       <c r="L50"/>
-    </row>
-    <row r="51" spans="1:12">
+      <c r="M50"/>
+    </row>
+    <row r="51" spans="1:13">
       <c r="A51"/>
       <c r="B51"/>
       <c r="C51"/>
@@ -3311,8 +3346,9 @@
       <c r="H51"/>
       <c r="I51"/>
       <c r="J51"/>
-    </row>
-    <row r="52" spans="1:12">
+      <c r="K51"/>
+    </row>
+    <row r="52" spans="1:13">
       <c r="A52" s="29" t="s">
         <v>79</v>
       </c>
@@ -3324,7 +3360,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:13">
       <c r="A53" s="39" t="s">
         <v>7</v>
       </c>
@@ -3342,10 +3378,11 @@
       <c r="G53" s="57"/>
       <c r="H53" s="57"/>
       <c r="I53" s="57"/>
-      <c r="K53" s="37"/>
+      <c r="J53" s="57"/>
       <c r="L53" s="37"/>
-    </row>
-    <row r="54" spans="1:12">
+      <c r="M53" s="37"/>
+    </row>
+    <row r="54" spans="1:13">
       <c r="A54" s="43"/>
       <c r="B54" s="38"/>
       <c r="C54" s="81"/>
@@ -3354,11 +3391,12 @@
       <c r="F54" s="58"/>
       <c r="G54" s="58"/>
       <c r="H54" s="58"/>
-      <c r="J54"/>
+      <c r="I54" s="58"/>
       <c r="K54"/>
       <c r="L54"/>
-    </row>
-    <row r="55" spans="1:12">
+      <c r="M54"/>
+    </row>
+    <row r="55" spans="1:13">
       <c r="A55" s="43"/>
       <c r="B55" s="38"/>
       <c r="C55" s="82"/>
@@ -3367,11 +3405,12 @@
       <c r="F55" s="58"/>
       <c r="G55" s="58"/>
       <c r="H55" s="58"/>
-      <c r="J55"/>
+      <c r="I55" s="58"/>
       <c r="K55"/>
       <c r="L55"/>
-    </row>
-    <row r="56" spans="1:12">
+      <c r="M55"/>
+    </row>
+    <row r="56" spans="1:13">
       <c r="A56" s="44"/>
       <c r="B56" s="40"/>
       <c r="C56" s="83"/>
@@ -3380,11 +3419,12 @@
       <c r="F56" s="58"/>
       <c r="G56" s="58"/>
       <c r="H56" s="58"/>
-      <c r="J56"/>
+      <c r="I56" s="58"/>
       <c r="K56"/>
       <c r="L56"/>
-    </row>
-    <row r="57" spans="1:12">
+      <c r="M56"/>
+    </row>
+    <row r="57" spans="1:13">
       <c r="A57" s="73"/>
       <c r="B57" s="74"/>
       <c r="C57" s="75"/>
@@ -3393,11 +3433,12 @@
       <c r="F57" s="58"/>
       <c r="G57" s="58"/>
       <c r="H57" s="58"/>
-      <c r="J57"/>
+      <c r="I57" s="58"/>
       <c r="K57"/>
       <c r="L57"/>
-    </row>
-    <row r="58" spans="1:12">
+      <c r="M57"/>
+    </row>
+    <row r="58" spans="1:13">
       <c r="A58" s="29" t="s">
         <v>96</v>
       </c>
@@ -3409,7 +3450,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="1:12">
+    <row r="59" spans="1:13">
       <c r="A59" s="39" t="s">
         <v>7</v>
       </c>
@@ -3425,10 +3466,11 @@
       <c r="G59" s="57"/>
       <c r="H59" s="57"/>
       <c r="I59" s="57"/>
-      <c r="K59" s="37"/>
+      <c r="J59" s="57"/>
       <c r="L59" s="37"/>
-    </row>
-    <row r="60" spans="1:12">
+      <c r="M59" s="37"/>
+    </row>
+    <row r="60" spans="1:13">
       <c r="A60" s="43"/>
       <c r="B60" s="38"/>
       <c r="C60" s="32"/>
@@ -3437,11 +3479,12 @@
       <c r="F60" s="58"/>
       <c r="G60" s="58"/>
       <c r="H60" s="58"/>
-      <c r="J60"/>
+      <c r="I60" s="58"/>
       <c r="K60"/>
       <c r="L60"/>
-    </row>
-    <row r="61" spans="1:12">
+      <c r="M60"/>
+    </row>
+    <row r="61" spans="1:13">
       <c r="A61" s="43"/>
       <c r="B61" s="38"/>
       <c r="C61" s="34"/>
@@ -3450,11 +3493,12 @@
       <c r="F61" s="58"/>
       <c r="G61" s="58"/>
       <c r="H61" s="58"/>
-      <c r="J61"/>
+      <c r="I61" s="58"/>
       <c r="K61"/>
       <c r="L61"/>
-    </row>
-    <row r="62" spans="1:12">
+      <c r="M61"/>
+    </row>
+    <row r="62" spans="1:13">
       <c r="A62" s="44"/>
       <c r="B62" s="40"/>
       <c r="C62" s="41"/>
@@ -3463,11 +3507,12 @@
       <c r="F62" s="58"/>
       <c r="G62" s="58"/>
       <c r="H62" s="58"/>
-      <c r="J62"/>
+      <c r="I62" s="58"/>
       <c r="K62"/>
       <c r="L62"/>
-    </row>
-    <row r="63" spans="1:12">
+      <c r="M62"/>
+    </row>
+    <row r="63" spans="1:13">
       <c r="A63"/>
       <c r="B63"/>
       <c r="C63"/>
@@ -3478,8 +3523,9 @@
       <c r="H63"/>
       <c r="I63"/>
       <c r="J63"/>
-    </row>
-    <row r="64" spans="1:12">
+      <c r="K63"/>
+    </row>
+    <row r="64" spans="1:13">
       <c r="A64"/>
       <c r="B64" t="s">
         <v>78</v>
@@ -3492,8 +3538,9 @@
       <c r="H64"/>
       <c r="I64"/>
       <c r="J64"/>
-    </row>
-    <row r="65" spans="1:13">
+      <c r="K64"/>
+    </row>
+    <row r="65" spans="1:14">
       <c r="A65" s="3" t="s">
         <v>97</v>
       </c>
@@ -3507,58 +3554,63 @@
       <c r="I65" s="13"/>
       <c r="J65" s="13"/>
       <c r="K65" s="13"/>
-      <c r="L65" s="6"/>
-      <c r="M65" s="14"/>
-    </row>
-    <row r="66" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A66" s="113" t="s">
+      <c r="L65" s="13"/>
+      <c r="M65" s="6"/>
+      <c r="N65" s="14"/>
+    </row>
+    <row r="66" spans="1:14" ht="13.5" customHeight="1">
+      <c r="A66" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="B66" s="113" t="s">
+      <c r="B66" s="119" t="s">
         <v>3</v>
       </c>
-      <c r="C66" s="112" t="s">
+      <c r="C66" s="116" t="s">
         <v>4</v>
       </c>
-      <c r="D66" s="112" t="s">
+      <c r="D66" s="116" t="s">
         <v>6</v>
       </c>
-      <c r="E66" s="112" t="s">
+      <c r="E66" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="F66" s="116" t="s">
+      <c r="F66" s="117" t="s">
         <v>33</v>
       </c>
-      <c r="G66" s="116" t="s">
+      <c r="G66" s="117" t="s">
         <v>16</v>
       </c>
-      <c r="H66" s="114" t="s">
+      <c r="H66" s="127" t="s">
+        <v>130</v>
+      </c>
+      <c r="I66" s="127" t="s">
         <v>106</v>
       </c>
-      <c r="I66" s="112" t="s">
+      <c r="J66" s="116" t="s">
         <v>1</v>
       </c>
-      <c r="J66" s="112"/>
-      <c r="K66" s="15"/>
-      <c r="L66" s="16"/>
-      <c r="M66" s="9"/>
-    </row>
-    <row r="67" spans="1:13">
-      <c r="A67" s="113"/>
-      <c r="B67" s="113"/>
-      <c r="C67" s="112"/>
-      <c r="D67" s="112"/>
-      <c r="E67" s="112"/>
-      <c r="F67" s="117"/>
-      <c r="G67" s="117"/>
-      <c r="H67" s="115"/>
-      <c r="I67" s="112"/>
-      <c r="J67" s="112"/>
-      <c r="K67" s="17"/>
-      <c r="L67" s="28"/>
-      <c r="M67" s="14"/>
-    </row>
-    <row r="68" spans="1:13">
+      <c r="K66" s="116"/>
+      <c r="L66" s="15"/>
+      <c r="M66" s="16"/>
+      <c r="N66" s="9"/>
+    </row>
+    <row r="67" spans="1:14">
+      <c r="A67" s="119"/>
+      <c r="B67" s="119"/>
+      <c r="C67" s="116"/>
+      <c r="D67" s="116"/>
+      <c r="E67" s="116"/>
+      <c r="F67" s="118"/>
+      <c r="G67" s="118"/>
+      <c r="H67" s="128"/>
+      <c r="I67" s="128"/>
+      <c r="J67" s="116"/>
+      <c r="K67" s="116"/>
+      <c r="L67" s="17"/>
+      <c r="M67" s="28"/>
+      <c r="N67" s="14"/>
+    </row>
+    <row r="68" spans="1:14">
       <c r="A68" s="18">
         <v>1</v>
       </c>
@@ -3573,15 +3625,16 @@
       <c r="F68" s="19"/>
       <c r="G68" s="59"/>
       <c r="H68" s="59"/>
-      <c r="I68" s="19" t="s">
+      <c r="I68" s="59"/>
+      <c r="J68" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="J68" s="20"/>
       <c r="K68" s="20"/>
-      <c r="L68" s="27"/>
-      <c r="M68" s="14"/>
-    </row>
-    <row r="69" spans="1:13">
+      <c r="L68" s="20"/>
+      <c r="M68" s="27"/>
+      <c r="N68" s="14"/>
+    </row>
+    <row r="69" spans="1:14">
       <c r="A69" s="18">
         <f>A68+1</f>
         <v>2</v>
@@ -3599,15 +3652,16 @@
       <c r="F69" s="19"/>
       <c r="G69" s="59"/>
       <c r="H69" s="59"/>
-      <c r="I69" s="19" t="s">
+      <c r="I69" s="59"/>
+      <c r="J69" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="J69" s="20"/>
       <c r="K69" s="20"/>
-      <c r="L69" s="27"/>
-      <c r="M69" s="14"/>
-    </row>
-    <row r="70" spans="1:13">
+      <c r="L69" s="20"/>
+      <c r="M69" s="27"/>
+      <c r="N69" s="14"/>
+    </row>
+    <row r="70" spans="1:14">
       <c r="A70" s="18">
         <f t="shared" ref="A70:A84" si="0">A69+1</f>
         <v>3</v>
@@ -3629,15 +3683,16 @@
         <v>14</v>
       </c>
       <c r="H70" s="59"/>
-      <c r="I70" s="19" t="s">
+      <c r="I70" s="59"/>
+      <c r="J70" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="J70" s="20"/>
       <c r="K70" s="20"/>
-      <c r="L70" s="21"/>
-      <c r="M70" s="14"/>
-    </row>
-    <row r="71" spans="1:13">
+      <c r="L70" s="20"/>
+      <c r="M70" s="21"/>
+      <c r="N70" s="14"/>
+    </row>
+    <row r="71" spans="1:14">
       <c r="A71" s="18">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -3655,15 +3710,16 @@
         <v>14</v>
       </c>
       <c r="H71" s="59"/>
-      <c r="I71" s="19" t="s">
+      <c r="I71" s="59"/>
+      <c r="J71" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="J71" s="20"/>
       <c r="K71" s="20"/>
-      <c r="L71" s="21"/>
-      <c r="M71" s="14"/>
-    </row>
-    <row r="72" spans="1:13">
+      <c r="L71" s="20"/>
+      <c r="M71" s="21"/>
+      <c r="N71" s="14"/>
+    </row>
+    <row r="72" spans="1:14">
       <c r="A72" s="18">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -3683,45 +3739,49 @@
       <c r="H72" s="59" t="s">
         <v>107</v>
       </c>
-      <c r="I72" s="19" t="s">
+      <c r="I72" s="59" t="s">
+        <v>131</v>
+      </c>
+      <c r="J72" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="J72" s="20"/>
       <c r="K72" s="20"/>
-      <c r="L72" s="21"/>
-      <c r="M72" s="14"/>
-    </row>
-    <row r="73" spans="1:13">
+      <c r="L72" s="20"/>
+      <c r="M72" s="21"/>
+      <c r="N72" s="14"/>
+    </row>
+    <row r="73" spans="1:14">
       <c r="A73" s="18">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B73" s="63" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C73" s="70" t="s">
         <v>48</v>
       </c>
       <c r="D73" s="64"/>
       <c r="E73" s="64" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F73" s="64"/>
       <c r="G73" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="H73" s="65" t="s">
-        <v>115</v>
-      </c>
-      <c r="I73" s="19" t="s">
+      <c r="H73" s="65"/>
+      <c r="I73" s="65" t="s">
+        <v>113</v>
+      </c>
+      <c r="J73" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="J73" s="66"/>
       <c r="K73" s="66"/>
-      <c r="L73" s="67"/>
-      <c r="M73" s="14"/>
-    </row>
-    <row r="74" spans="1:13">
+      <c r="L73" s="66"/>
+      <c r="M73" s="67"/>
+      <c r="N73" s="14"/>
+    </row>
+    <row r="74" spans="1:14">
       <c r="A74" s="18">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3733,13 +3793,14 @@
       <c r="F74" s="19"/>
       <c r="G74" s="59"/>
       <c r="H74" s="59"/>
-      <c r="I74" s="19"/>
-      <c r="J74" s="20"/>
+      <c r="I74" s="59"/>
+      <c r="J74" s="19"/>
       <c r="K74" s="20"/>
-      <c r="L74" s="21"/>
-      <c r="M74" s="14"/>
-    </row>
-    <row r="75" spans="1:13">
+      <c r="L74" s="20"/>
+      <c r="M74" s="21"/>
+      <c r="N74" s="14"/>
+    </row>
+    <row r="75" spans="1:14">
       <c r="A75" s="18">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -3751,13 +3812,14 @@
       <c r="F75" s="64"/>
       <c r="G75" s="65"/>
       <c r="H75" s="65"/>
-      <c r="I75" s="64"/>
-      <c r="J75" s="66"/>
+      <c r="I75" s="65"/>
+      <c r="J75" s="64"/>
       <c r="K75" s="66"/>
-      <c r="L75" s="67"/>
-      <c r="M75" s="14"/>
-    </row>
-    <row r="76" spans="1:13">
+      <c r="L75" s="66"/>
+      <c r="M75" s="67"/>
+      <c r="N75" s="14"/>
+    </row>
+    <row r="76" spans="1:14">
       <c r="A76" s="18">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -3769,13 +3831,14 @@
       <c r="F76" s="64"/>
       <c r="G76" s="65"/>
       <c r="H76" s="65"/>
-      <c r="I76" s="64"/>
-      <c r="J76" s="66"/>
+      <c r="I76" s="65"/>
+      <c r="J76" s="64"/>
       <c r="K76" s="66"/>
-      <c r="L76" s="67"/>
-      <c r="M76" s="14"/>
-    </row>
-    <row r="77" spans="1:13">
+      <c r="L76" s="66"/>
+      <c r="M76" s="67"/>
+      <c r="N76" s="14"/>
+    </row>
+    <row r="77" spans="1:14">
       <c r="A77" s="18">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -3787,13 +3850,14 @@
       <c r="F77" s="19"/>
       <c r="G77" s="59"/>
       <c r="H77" s="59"/>
-      <c r="I77" s="19"/>
-      <c r="J77" s="20"/>
+      <c r="I77" s="59"/>
+      <c r="J77" s="19"/>
       <c r="K77" s="20"/>
-      <c r="L77" s="21"/>
-      <c r="M77" s="14"/>
-    </row>
-    <row r="78" spans="1:13">
+      <c r="L77" s="20"/>
+      <c r="M77" s="21"/>
+      <c r="N77" s="14"/>
+    </row>
+    <row r="78" spans="1:14">
       <c r="A78" s="18">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -3805,13 +3869,14 @@
       <c r="F78" s="64"/>
       <c r="G78" s="65"/>
       <c r="H78" s="65"/>
-      <c r="I78" s="64"/>
-      <c r="J78" s="66"/>
+      <c r="I78" s="65"/>
+      <c r="J78" s="64"/>
       <c r="K78" s="66"/>
-      <c r="L78" s="67"/>
-      <c r="M78" s="14"/>
-    </row>
-    <row r="79" spans="1:13">
+      <c r="L78" s="66"/>
+      <c r="M78" s="67"/>
+      <c r="N78" s="14"/>
+    </row>
+    <row r="79" spans="1:14">
       <c r="A79" s="18">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -3823,13 +3888,14 @@
       <c r="F79" s="64"/>
       <c r="G79" s="65"/>
       <c r="H79" s="65"/>
-      <c r="I79" s="64"/>
-      <c r="J79" s="66"/>
+      <c r="I79" s="65"/>
+      <c r="J79" s="64"/>
       <c r="K79" s="66"/>
-      <c r="L79" s="67"/>
-      <c r="M79" s="14"/>
-    </row>
-    <row r="80" spans="1:13">
+      <c r="L79" s="66"/>
+      <c r="M79" s="67"/>
+      <c r="N79" s="14"/>
+    </row>
+    <row r="80" spans="1:14">
       <c r="A80" s="18">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -3841,13 +3907,14 @@
       <c r="F80" s="19"/>
       <c r="G80" s="59"/>
       <c r="H80" s="59"/>
-      <c r="I80" s="19"/>
-      <c r="J80" s="20"/>
+      <c r="I80" s="59"/>
+      <c r="J80" s="19"/>
       <c r="K80" s="20"/>
-      <c r="L80" s="21"/>
-      <c r="M80" s="14"/>
-    </row>
-    <row r="81" spans="1:13">
+      <c r="L80" s="20"/>
+      <c r="M80" s="21"/>
+      <c r="N80" s="14"/>
+    </row>
+    <row r="81" spans="1:14">
       <c r="A81" s="18">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -3859,13 +3926,14 @@
       <c r="F81" s="64"/>
       <c r="G81" s="65"/>
       <c r="H81" s="65"/>
-      <c r="I81" s="64"/>
-      <c r="J81" s="66"/>
+      <c r="I81" s="65"/>
+      <c r="J81" s="64"/>
       <c r="K81" s="66"/>
-      <c r="L81" s="67"/>
-      <c r="M81" s="14"/>
-    </row>
-    <row r="82" spans="1:13">
+      <c r="L81" s="66"/>
+      <c r="M81" s="67"/>
+      <c r="N81" s="14"/>
+    </row>
+    <row r="82" spans="1:14">
       <c r="A82" s="18">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -3877,13 +3945,14 @@
       <c r="F82" s="64"/>
       <c r="G82" s="65"/>
       <c r="H82" s="65"/>
-      <c r="I82" s="64"/>
-      <c r="J82" s="66"/>
+      <c r="I82" s="65"/>
+      <c r="J82" s="64"/>
       <c r="K82" s="66"/>
-      <c r="L82" s="67"/>
-      <c r="M82" s="14"/>
-    </row>
-    <row r="83" spans="1:13">
+      <c r="L82" s="66"/>
+      <c r="M82" s="67"/>
+      <c r="N82" s="14"/>
+    </row>
+    <row r="83" spans="1:14">
       <c r="A83" s="18">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -3895,13 +3964,14 @@
       <c r="F83" s="19"/>
       <c r="G83" s="59"/>
       <c r="H83" s="59"/>
-      <c r="I83" s="19"/>
-      <c r="J83" s="20"/>
+      <c r="I83" s="59"/>
+      <c r="J83" s="19"/>
       <c r="K83" s="20"/>
-      <c r="L83" s="21"/>
-      <c r="M83" s="14"/>
-    </row>
-    <row r="84" spans="1:13">
+      <c r="L83" s="20"/>
+      <c r="M83" s="21"/>
+      <c r="N83" s="14"/>
+    </row>
+    <row r="84" spans="1:14">
       <c r="A84" s="18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -3913,13 +3983,14 @@
       <c r="F84" s="64"/>
       <c r="G84" s="65"/>
       <c r="H84" s="65"/>
-      <c r="I84" s="64"/>
-      <c r="J84" s="66"/>
+      <c r="I84" s="65"/>
+      <c r="J84" s="64"/>
       <c r="K84" s="66"/>
-      <c r="L84" s="67"/>
-      <c r="M84" s="14"/>
-    </row>
-    <row r="85" spans="1:13">
+      <c r="L84" s="66"/>
+      <c r="M84" s="67"/>
+      <c r="N84" s="14"/>
+    </row>
+    <row r="85" spans="1:14">
       <c r="A85" s="22"/>
       <c r="B85" s="23"/>
       <c r="C85" s="24"/>
@@ -3928,13 +3999,14 @@
       <c r="F85" s="24"/>
       <c r="G85" s="60"/>
       <c r="H85" s="60"/>
-      <c r="I85" s="24"/>
-      <c r="J85" s="25"/>
+      <c r="I85" s="60"/>
+      <c r="J85" s="24"/>
       <c r="K85" s="25"/>
-      <c r="L85" s="26"/>
-      <c r="M85" s="14"/>
-    </row>
-    <row r="87" spans="1:13">
+      <c r="L85" s="25"/>
+      <c r="M85" s="26"/>
+      <c r="N85" s="14"/>
+    </row>
+    <row r="87" spans="1:14">
       <c r="A87" s="29" t="s">
         <v>98</v>
       </c>
@@ -3946,7 +4018,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="88" spans="1:13">
+    <row r="88" spans="1:14">
       <c r="A88" s="39" t="s">
         <v>7</v>
       </c>
@@ -3960,10 +4032,11 @@
       <c r="G88" s="57"/>
       <c r="H88" s="57"/>
       <c r="I88" s="57"/>
-      <c r="K88" s="37"/>
+      <c r="J88" s="57"/>
       <c r="L88" s="37"/>
-    </row>
-    <row r="89" spans="1:13">
+      <c r="M88" s="37"/>
+    </row>
+    <row r="89" spans="1:14">
       <c r="A89" s="43"/>
       <c r="B89" s="38"/>
       <c r="C89" s="32"/>
@@ -3972,11 +4045,12 @@
       <c r="F89" s="58"/>
       <c r="G89" s="58"/>
       <c r="H89" s="58"/>
-      <c r="J89"/>
+      <c r="I89" s="58"/>
       <c r="K89"/>
       <c r="L89"/>
-    </row>
-    <row r="90" spans="1:13">
+      <c r="M89"/>
+    </row>
+    <row r="90" spans="1:14">
       <c r="A90" s="43"/>
       <c r="B90" s="38"/>
       <c r="C90" s="34"/>
@@ -3985,11 +4059,12 @@
       <c r="F90" s="58"/>
       <c r="G90" s="58"/>
       <c r="H90" s="58"/>
-      <c r="J90"/>
+      <c r="I90" s="58"/>
       <c r="K90"/>
       <c r="L90"/>
-    </row>
-    <row r="91" spans="1:13">
+      <c r="M90"/>
+    </row>
+    <row r="91" spans="1:14">
       <c r="A91" s="44"/>
       <c r="B91" s="40"/>
       <c r="C91" s="41"/>
@@ -3998,11 +4073,12 @@
       <c r="F91" s="58"/>
       <c r="G91" s="58"/>
       <c r="H91" s="58"/>
-      <c r="J91"/>
+      <c r="I91" s="58"/>
       <c r="K91"/>
       <c r="L91"/>
-    </row>
-    <row r="92" spans="1:13">
+      <c r="M91"/>
+    </row>
+    <row r="92" spans="1:14">
       <c r="A92"/>
       <c r="B92"/>
       <c r="C92"/>
@@ -4013,8 +4089,9 @@
       <c r="H92"/>
       <c r="I92"/>
       <c r="J92"/>
-    </row>
-    <row r="93" spans="1:13">
+      <c r="K92"/>
+    </row>
+    <row r="93" spans="1:14">
       <c r="A93"/>
       <c r="B93" t="s">
         <v>85</v>
@@ -4027,8 +4104,9 @@
       <c r="H93"/>
       <c r="I93"/>
       <c r="J93"/>
-    </row>
-    <row r="94" spans="1:13">
+      <c r="K93"/>
+    </row>
+    <row r="94" spans="1:14">
       <c r="A94" s="3" t="s">
         <v>83</v>
       </c>
@@ -4042,50 +4120,53 @@
       <c r="I94" s="13"/>
       <c r="J94" s="13"/>
       <c r="K94" s="13"/>
-      <c r="L94" s="6"/>
-      <c r="M94" s="14"/>
-    </row>
-    <row r="95" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A95" s="113" t="s">
+      <c r="L94" s="13"/>
+      <c r="M94" s="6"/>
+      <c r="N94" s="14"/>
+    </row>
+    <row r="95" spans="1:14" ht="13.5" customHeight="1">
+      <c r="A95" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="B95" s="113" t="s">
+      <c r="B95" s="119" t="s">
         <v>84</v>
       </c>
-      <c r="C95" s="112" t="s">
+      <c r="C95" s="116" t="s">
         <v>86</v>
       </c>
-      <c r="D95" s="112" t="s">
+      <c r="D95" s="116" t="s">
         <v>87</v>
       </c>
-      <c r="E95" s="112" t="s">
+      <c r="E95" s="116" t="s">
         <v>81</v>
       </c>
-      <c r="F95" s="123"/>
-      <c r="G95" s="123"/>
-      <c r="H95" s="123"/>
-      <c r="I95" s="125"/>
-      <c r="J95" s="112"/>
-      <c r="K95" s="15"/>
-      <c r="L95" s="16"/>
-      <c r="M95" s="9"/>
-    </row>
-    <row r="96" spans="1:13">
-      <c r="A96" s="113"/>
-      <c r="B96" s="113"/>
-      <c r="C96" s="112"/>
-      <c r="D96" s="112"/>
-      <c r="E96" s="112"/>
-      <c r="F96" s="124"/>
-      <c r="G96" s="124"/>
-      <c r="H96" s="124"/>
-      <c r="I96" s="125"/>
-      <c r="J96" s="112"/>
-      <c r="K96" s="17"/>
-      <c r="L96" s="28"/>
-      <c r="M96" s="14"/>
-    </row>
-    <row r="97" spans="1:13">
+      <c r="F95" s="113"/>
+      <c r="G95" s="113"/>
+      <c r="H95" s="113"/>
+      <c r="I95" s="113"/>
+      <c r="J95" s="115"/>
+      <c r="K95" s="116"/>
+      <c r="L95" s="15"/>
+      <c r="M95" s="16"/>
+      <c r="N95" s="9"/>
+    </row>
+    <row r="96" spans="1:14">
+      <c r="A96" s="119"/>
+      <c r="B96" s="119"/>
+      <c r="C96" s="116"/>
+      <c r="D96" s="116"/>
+      <c r="E96" s="116"/>
+      <c r="F96" s="114"/>
+      <c r="G96" s="114"/>
+      <c r="H96" s="114"/>
+      <c r="I96" s="114"/>
+      <c r="J96" s="115"/>
+      <c r="K96" s="116"/>
+      <c r="L96" s="17"/>
+      <c r="M96" s="28"/>
+      <c r="N96" s="14"/>
+    </row>
+    <row r="97" spans="1:14">
       <c r="A97" s="18">
         <v>1</v>
       </c>
@@ -4102,13 +4183,14 @@
       <c r="F97" s="77"/>
       <c r="G97" s="79"/>
       <c r="H97" s="79"/>
-      <c r="I97" s="77"/>
-      <c r="J97" s="20"/>
+      <c r="I97" s="79"/>
+      <c r="J97" s="77"/>
       <c r="K97" s="20"/>
-      <c r="L97" s="27"/>
-      <c r="M97" s="14"/>
-    </row>
-    <row r="98" spans="1:13">
+      <c r="L97" s="20"/>
+      <c r="M97" s="27"/>
+      <c r="N97" s="14"/>
+    </row>
+    <row r="98" spans="1:14">
       <c r="A98" s="18">
         <f>A97+1</f>
         <v>2</v>
@@ -4126,13 +4208,14 @@
       <c r="F98" s="77"/>
       <c r="G98" s="79"/>
       <c r="H98" s="79"/>
-      <c r="I98" s="77"/>
-      <c r="J98" s="20"/>
+      <c r="I98" s="79"/>
+      <c r="J98" s="77"/>
       <c r="K98" s="20"/>
-      <c r="L98" s="27"/>
-      <c r="M98" s="14"/>
-    </row>
-    <row r="99" spans="1:13">
+      <c r="L98" s="20"/>
+      <c r="M98" s="27"/>
+      <c r="N98" s="14"/>
+    </row>
+    <row r="99" spans="1:14">
       <c r="A99" s="18">
         <f t="shared" ref="A99:A103" si="1">A98+1</f>
         <v>3</v>
@@ -4152,13 +4235,14 @@
       <c r="F99" s="77"/>
       <c r="G99" s="79"/>
       <c r="H99" s="79"/>
-      <c r="I99" s="77"/>
-      <c r="J99" s="20"/>
+      <c r="I99" s="79"/>
+      <c r="J99" s="77"/>
       <c r="K99" s="20"/>
-      <c r="L99" s="21"/>
-      <c r="M99" s="14"/>
-    </row>
-    <row r="100" spans="1:13">
+      <c r="L99" s="20"/>
+      <c r="M99" s="21"/>
+      <c r="N99" s="14"/>
+    </row>
+    <row r="100" spans="1:14">
       <c r="A100" s="18">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -4170,13 +4254,14 @@
       <c r="F100" s="77"/>
       <c r="G100" s="79"/>
       <c r="H100" s="79"/>
-      <c r="I100" s="77"/>
-      <c r="J100" s="20"/>
+      <c r="I100" s="79"/>
+      <c r="J100" s="77"/>
       <c r="K100" s="20"/>
-      <c r="L100" s="21"/>
-      <c r="M100" s="14"/>
-    </row>
-    <row r="101" spans="1:13">
+      <c r="L100" s="20"/>
+      <c r="M100" s="21"/>
+      <c r="N100" s="14"/>
+    </row>
+    <row r="101" spans="1:14">
       <c r="A101" s="18">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -4188,13 +4273,14 @@
       <c r="F101" s="77"/>
       <c r="G101" s="79"/>
       <c r="H101" s="79"/>
-      <c r="I101" s="77"/>
-      <c r="J101" s="20"/>
+      <c r="I101" s="79"/>
+      <c r="J101" s="77"/>
       <c r="K101" s="20"/>
-      <c r="L101" s="21"/>
-      <c r="M101" s="14"/>
-    </row>
-    <row r="102" spans="1:13">
+      <c r="L101" s="20"/>
+      <c r="M101" s="21"/>
+      <c r="N101" s="14"/>
+    </row>
+    <row r="102" spans="1:14">
       <c r="A102" s="18">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -4206,13 +4292,14 @@
       <c r="F102" s="78"/>
       <c r="G102" s="80"/>
       <c r="H102" s="80"/>
-      <c r="I102" s="78"/>
-      <c r="J102" s="66"/>
+      <c r="I102" s="80"/>
+      <c r="J102" s="78"/>
       <c r="K102" s="66"/>
-      <c r="L102" s="67"/>
-      <c r="M102" s="14"/>
-    </row>
-    <row r="103" spans="1:13">
+      <c r="L102" s="66"/>
+      <c r="M102" s="67"/>
+      <c r="N102" s="14"/>
+    </row>
+    <row r="103" spans="1:14">
       <c r="A103" s="18">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -4224,44 +4311,47 @@
       <c r="F103" s="77"/>
       <c r="G103" s="79"/>
       <c r="H103" s="79"/>
-      <c r="I103" s="77"/>
-      <c r="J103" s="20"/>
+      <c r="I103" s="79"/>
+      <c r="J103" s="77"/>
       <c r="K103" s="20"/>
-      <c r="L103" s="21"/>
-      <c r="M103" s="14"/>
+      <c r="L103" s="20"/>
+      <c r="M103" s="21"/>
+      <c r="N103" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="F95:F96"/>
-    <mergeCell ref="H95:H96"/>
-    <mergeCell ref="I95:J96"/>
-    <mergeCell ref="G66:G67"/>
-    <mergeCell ref="G95:G96"/>
+  <mergeCells count="28">
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="J66:K67"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="E66:E67"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="I66:I67"/>
+    <mergeCell ref="F66:F67"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="H66:H67"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C14:E14"/>
     <mergeCell ref="A95:A96"/>
     <mergeCell ref="B95:B96"/>
     <mergeCell ref="C95:C96"/>
     <mergeCell ref="D95:D96"/>
     <mergeCell ref="E95:E96"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="I66:J67"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="E66:E67"/>
-    <mergeCell ref="D66:D67"/>
-    <mergeCell ref="H66:H67"/>
-    <mergeCell ref="F66:F67"/>
-    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="F95:F96"/>
+    <mergeCell ref="I95:I96"/>
+    <mergeCell ref="J95:K96"/>
+    <mergeCell ref="G66:G67"/>
+    <mergeCell ref="G95:G96"/>
+    <mergeCell ref="H95:H96"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="8">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E107:H107" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E107:I107" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4271,7 +4361,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16" xr:uid="{0933AF92-3C0C-2F47-AF58-F84946F39270}">
       <formula1>componentKind</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F68:G85 C17 C19:C23" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19:C23 C17 F68:G85" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
       <formula1>yesNo</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C24" xr:uid="{CCFC1331-CEEF-574E-9BCC-37D38F486896}">
@@ -4357,7 +4447,7 @@
         <v>12</v>
       </c>
       <c r="L3" s="87" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -4387,18 +4477,18 @@
         <v>13</v>
       </c>
       <c r="L5" s="88" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="B6" s="53"/>
       <c r="L6" s="51" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="L7" s="89" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3.0.10: Implement MenuItem and MenuItemInterface generation.         Sort alphabetical order for RouteRecord informations.
</commit_message>
<xml_diff>
--- a/meta/components/PlainBoxSample.xlsx
+++ b/meta/components/PlainBoxSample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoVueComponent/meta/components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4D7294-018A-8C44-8774-D92BB04B4B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C72F9B-ACBA-4D4D-87CB-A99E12B7AA7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9860" yWindow="7560" windowWidth="25200" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1420" yWindow="500" windowWidth="25200" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VueComponent" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="138">
   <si>
     <t>パッケージ</t>
   </si>
@@ -1042,6 +1042,45 @@
   </si>
   <si>
     <t>sec</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>権限種別</t>
+    <rPh sb="0" eb="4">
+      <t xml:space="preserve">ケンゲンシュベツ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Box</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>/* 画面の権限種別 */</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ボックス</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>メニューラベル</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>/* menuLabelプロパティに定義されます。画面コンポーネントのメニューラベルに使用されることを想定しています。 */</t>
+    <rPh sb="18" eb="20">
+      <t xml:space="preserve">テイギ </t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t xml:space="preserve">ガメｎ </t>
+    </rPh>
+    <rPh sb="43" eb="45">
+      <t xml:space="preserve">シヨウ </t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t xml:space="preserve">ソウテイ </t>
+    </rPh>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -2608,10 +2647,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N103"/>
+  <dimension ref="A1:N106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="I73" sqref="I73"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2698,128 +2737,124 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="10" t="s">
+      <c r="B10" s="6"/>
+      <c r="C10" s="10" t="s">
         <v>111</v>
-      </c>
-      <c r="D9" s="31"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="120" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="121"/>
-      <c r="C10" s="10" t="s">
-        <v>129</v>
       </c>
       <c r="D10" s="31"/>
       <c r="E10" s="11"/>
       <c r="F10" s="1" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="120" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="121"/>
       <c r="C11" s="10" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="D11" s="31"/>
       <c r="E11" s="11"/>
       <c r="F11" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="120" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="B12" s="121"/>
       <c r="C12" s="10" t="s">
-        <v>21</v>
+        <v>112</v>
       </c>
       <c r="D12" s="31"/>
       <c r="E12" s="11"/>
       <c r="F12" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="120" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="B13" s="121"/>
-      <c r="C13" s="76" t="s">
-        <v>63</v>
+      <c r="C13" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="D13" s="31"/>
       <c r="E13" s="11"/>
       <c r="F13" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="120" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="121"/>
+      <c r="C14" s="76" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="31"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="45" customHeight="1">
-      <c r="A14" s="3" t="s">
+    <row r="15" spans="1:12" ht="45" customHeight="1">
+      <c r="A15" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="122" t="s">
+      <c r="B15" s="6"/>
+      <c r="C15" s="122" t="s">
         <v>71</v>
       </c>
-      <c r="D14" s="123"/>
-      <c r="E14" s="124"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="56"/>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="3" t="s">
+      <c r="D15" s="123"/>
+      <c r="E15" s="124"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="56"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="7" t="s">
+      <c r="B16" s="6"/>
+      <c r="C16" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D15" s="12"/>
-      <c r="E15" s="8"/>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="54" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="55" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16"/>
-      <c r="F16"/>
-      <c r="G16"/>
-      <c r="H16"/>
-      <c r="I16"/>
-      <c r="J16"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="8"/>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="54" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B17" s="13"/>
       <c r="C17" s="55" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="E17"/>
       <c r="F17"/>
@@ -2829,46 +2864,46 @@
       <c r="J17"/>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" s="84" t="s">
-        <v>115</v>
-      </c>
-      <c r="B18" s="85"/>
-      <c r="C18" s="86" t="s">
-        <v>116</v>
+      <c r="A18" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="55" t="s">
+        <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>117</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="E18"/>
+      <c r="F18"/>
       <c r="G18"/>
       <c r="H18"/>
       <c r="I18"/>
+      <c r="J18"/>
     </row>
     <row r="19" spans="1:13">
-      <c r="A19" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="55"/>
+      <c r="A19" s="84" t="s">
+        <v>115</v>
+      </c>
+      <c r="B19" s="85"/>
+      <c r="C19" s="86" t="s">
+        <v>116</v>
+      </c>
       <c r="D19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19"/>
-      <c r="F19"/>
+        <v>117</v>
+      </c>
       <c r="G19"/>
       <c r="H19"/>
       <c r="I19"/>
-      <c r="J19"/>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="54" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B20" s="13"/>
-      <c r="C20" s="55" t="s">
-        <v>14</v>
-      </c>
+      <c r="C20" s="55"/>
       <c r="D20" t="s">
-        <v>73</v>
+        <v>36</v>
       </c>
       <c r="E20"/>
       <c r="F20"/>
@@ -2879,14 +2914,14 @@
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="54" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="B21" s="13"/>
       <c r="C21" s="55" t="s">
         <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="E21"/>
       <c r="F21"/>
@@ -2897,14 +2932,14 @@
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="54" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="B22" s="13"/>
       <c r="C22" s="55" t="s">
         <v>14</v>
       </c>
       <c r="D22" t="s">
-        <v>74</v>
+        <v>30</v>
       </c>
       <c r="E22"/>
       <c r="F22"/>
@@ -2914,15 +2949,15 @@
       <c r="J22"/>
     </row>
     <row r="23" spans="1:13">
-      <c r="A23" s="125" t="s">
-        <v>77</v>
-      </c>
-      <c r="B23" s="126"/>
+      <c r="A23" s="54" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="13"/>
       <c r="C23" s="55" t="s">
         <v>14</v>
       </c>
       <c r="D23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E23"/>
       <c r="F23"/>
@@ -2932,14 +2967,16 @@
       <c r="J23"/>
     </row>
     <row r="24" spans="1:13">
-      <c r="A24" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24" s="13"/>
+      <c r="A24" s="125" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="126"/>
       <c r="C24" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="D24"/>
+      <c r="D24" t="s">
+        <v>75</v>
+      </c>
       <c r="E24"/>
       <c r="F24"/>
       <c r="G24"/>
@@ -2948,16 +2985,14 @@
       <c r="J24"/>
     </row>
     <row r="25" spans="1:13">
-      <c r="A25" s="125" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" s="126"/>
+      <c r="A25" s="54" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="13"/>
       <c r="C25" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="D25" t="s">
-        <v>19</v>
-      </c>
+      <c r="D25"/>
       <c r="E25"/>
       <c r="F25"/>
       <c r="G25"/>
@@ -2967,13 +3002,15 @@
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="125" t="s">
-        <v>64</v>
+        <v>18</v>
       </c>
       <c r="B26" s="126"/>
       <c r="C26" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="D26"/>
+      <c r="D26" t="s">
+        <v>19</v>
+      </c>
       <c r="E26"/>
       <c r="F26"/>
       <c r="G26"/>
@@ -2982,279 +3019,267 @@
       <c r="J26"/>
     </row>
     <row r="27" spans="1:13">
-      <c r="B27"/>
+      <c r="A27" s="125" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="126"/>
+      <c r="C27" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27"/>
+      <c r="H27"/>
+      <c r="I27"/>
+      <c r="J27"/>
     </row>
     <row r="28" spans="1:13">
-      <c r="A28" s="90" t="s">
+      <c r="A28" s="84" t="s">
+        <v>132</v>
+      </c>
+      <c r="B28" s="85"/>
+      <c r="C28" s="86" t="s">
+        <v>133</v>
+      </c>
+      <c r="D28" t="s">
+        <v>134</v>
+      </c>
+      <c r="G28"/>
+      <c r="H28"/>
+      <c r="I28"/>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="B29"/>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="B30"/>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="90" t="s">
         <v>122</v>
       </c>
-      <c r="B28" s="91"/>
-      <c r="C28" s="91"/>
-      <c r="D28" s="91"/>
-      <c r="E28" s="92"/>
-      <c r="F28" s="1" t="s">
+      <c r="B31" s="91"/>
+      <c r="C31" s="91"/>
+      <c r="D31" s="91"/>
+      <c r="E31" s="92"/>
+      <c r="F31" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
-      <c r="A29" s="93" t="s">
+    <row r="32" spans="1:13">
+      <c r="A32" s="93" t="s">
         <v>124</v>
       </c>
-      <c r="B29" s="94" t="s">
+      <c r="B32" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="84" t="s">
+      <c r="C32" s="84" t="s">
         <v>127</v>
       </c>
-      <c r="D29" s="94"/>
-      <c r="E29" s="95"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="57"/>
-      <c r="H29" s="57"/>
-      <c r="I29" s="57"/>
-      <c r="J29" s="57"/>
-      <c r="L29" s="37"/>
-      <c r="M29" s="37"/>
-    </row>
-    <row r="30" spans="1:13">
-      <c r="A30" s="96">
+      <c r="D32" s="94"/>
+      <c r="E32" s="95"/>
+      <c r="F32" s="57"/>
+      <c r="G32" s="57"/>
+      <c r="H32" s="57"/>
+      <c r="I32" s="57"/>
+      <c r="J32" s="57"/>
+      <c r="L32" s="37"/>
+      <c r="M32" s="37"/>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="96">
         <v>1</v>
       </c>
-      <c r="B30" s="97" t="s">
+      <c r="B33" s="97" t="s">
         <v>125</v>
       </c>
-      <c r="C30" s="110"/>
-      <c r="D30" s="98"/>
-      <c r="E30" s="99"/>
-      <c r="F30" s="58"/>
-      <c r="G30" s="58"/>
-      <c r="H30" s="58"/>
-      <c r="I30" s="58"/>
-      <c r="K30"/>
-      <c r="L30"/>
-      <c r="M30"/>
-    </row>
-    <row r="31" spans="1:13">
-      <c r="A31" s="96">
+      <c r="C33" s="110"/>
+      <c r="D33" s="98"/>
+      <c r="E33" s="99"/>
+      <c r="F33" s="58"/>
+      <c r="G33" s="58"/>
+      <c r="H33" s="58"/>
+      <c r="I33" s="58"/>
+      <c r="K33"/>
+      <c r="L33"/>
+      <c r="M33"/>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="96">
         <v>2</v>
       </c>
-      <c r="B31" s="97" t="s">
+      <c r="B34" s="97" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="111" t="s">
+      <c r="C34" s="111" t="s">
         <v>128</v>
       </c>
-      <c r="D31" s="100"/>
-      <c r="E31" s="101"/>
-      <c r="F31" s="58"/>
-      <c r="G31" s="58"/>
-      <c r="H31" s="58"/>
-      <c r="I31" s="58"/>
-      <c r="K31"/>
-      <c r="L31"/>
-      <c r="M31"/>
-    </row>
-    <row r="32" spans="1:13">
-      <c r="A32" s="102"/>
-      <c r="B32" s="103"/>
-      <c r="C32" s="112"/>
-      <c r="D32" s="104"/>
-      <c r="E32" s="105"/>
-      <c r="F32" s="58"/>
-      <c r="G32" s="58"/>
-      <c r="H32" s="58"/>
-      <c r="I32" s="58"/>
-      <c r="K32"/>
-      <c r="L32"/>
-      <c r="M32"/>
-    </row>
-    <row r="33" spans="1:13" s="108" customFormat="1">
-      <c r="A33" s="106"/>
-      <c r="B33" s="106"/>
-      <c r="C33" s="107"/>
-      <c r="G33" s="109"/>
-      <c r="H33" s="109"/>
-      <c r="I33" s="109"/>
-    </row>
-    <row r="34" spans="1:13">
-      <c r="A34" s="29" t="s">
+      <c r="D34" s="100"/>
+      <c r="E34" s="101"/>
+      <c r="F34" s="58"/>
+      <c r="G34" s="58"/>
+      <c r="H34" s="58"/>
+      <c r="I34" s="58"/>
+      <c r="K34"/>
+      <c r="L34"/>
+      <c r="M34"/>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="102"/>
+      <c r="B35" s="103"/>
+      <c r="C35" s="112"/>
+      <c r="D35" s="104"/>
+      <c r="E35" s="105"/>
+      <c r="F35" s="58"/>
+      <c r="G35" s="58"/>
+      <c r="H35" s="58"/>
+      <c r="I35" s="58"/>
+      <c r="K35"/>
+      <c r="L35"/>
+      <c r="M35"/>
+    </row>
+    <row r="36" spans="1:13" s="108" customFormat="1">
+      <c r="A36" s="106"/>
+      <c r="B36" s="106"/>
+      <c r="C36" s="107"/>
+      <c r="G36" s="109"/>
+      <c r="H36" s="109"/>
+      <c r="I36" s="109"/>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="B34" s="30"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="71"/>
-      <c r="F34" s="1" t="s">
+      <c r="B37" s="30"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="71"/>
+      <c r="F37" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
-      <c r="A35" s="39" t="s">
+    <row r="38" spans="1:13">
+      <c r="A38" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B35" s="36" t="s">
+      <c r="B38" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C35" s="36"/>
-      <c r="D35" s="36"/>
-      <c r="E35" s="72"/>
-      <c r="F35" s="57"/>
-      <c r="G35" s="57"/>
-      <c r="H35" s="57"/>
-      <c r="I35" s="57"/>
-      <c r="J35" s="57"/>
-      <c r="L35" s="37"/>
-      <c r="M35" s="37"/>
-    </row>
-    <row r="36" spans="1:13">
-      <c r="A36" s="43">
+      <c r="C38" s="36"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="72"/>
+      <c r="F38" s="57"/>
+      <c r="G38" s="57"/>
+      <c r="H38" s="57"/>
+      <c r="I38" s="57"/>
+      <c r="J38" s="57"/>
+      <c r="L38" s="37"/>
+      <c r="M38" s="37"/>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="43">
         <v>1</v>
       </c>
-      <c r="B36" s="38" t="s">
+      <c r="B39" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="C36" s="32"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="58"/>
-      <c r="G36" s="58"/>
-      <c r="H36" s="58"/>
-      <c r="I36" s="58"/>
-      <c r="K36"/>
-      <c r="L36"/>
-      <c r="M36"/>
-    </row>
-    <row r="37" spans="1:13">
-      <c r="A37" s="43">
+      <c r="C39" s="32"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="58"/>
+      <c r="G39" s="58"/>
+      <c r="H39" s="58"/>
+      <c r="I39" s="58"/>
+      <c r="K39"/>
+      <c r="L39"/>
+      <c r="M39"/>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" s="43">
         <v>2</v>
       </c>
-      <c r="B37" s="38" t="s">
+      <c r="B40" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="C37" s="34"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="35"/>
-      <c r="F37" s="58"/>
-      <c r="G37" s="58"/>
-      <c r="H37" s="58"/>
-      <c r="I37" s="58"/>
-      <c r="K37"/>
-      <c r="L37"/>
-      <c r="M37"/>
-    </row>
-    <row r="38" spans="1:13">
-      <c r="A38" s="44"/>
-      <c r="B38" s="40"/>
-      <c r="C38" s="41"/>
-      <c r="D38" s="41"/>
-      <c r="E38" s="42"/>
-      <c r="F38" s="58"/>
-      <c r="G38" s="58"/>
-      <c r="H38" s="58"/>
-      <c r="I38" s="58"/>
-      <c r="K38"/>
-      <c r="L38"/>
-      <c r="M38"/>
-    </row>
-    <row r="39" spans="1:13">
-      <c r="A39"/>
-      <c r="B39"/>
-      <c r="C39"/>
-      <c r="D39"/>
-      <c r="E39"/>
-      <c r="F39"/>
-      <c r="G39"/>
-      <c r="H39"/>
-      <c r="I39"/>
-      <c r="J39"/>
-      <c r="K39"/>
-    </row>
-    <row r="40" spans="1:13">
-      <c r="A40" s="29" t="s">
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="58"/>
+      <c r="G40" s="58"/>
+      <c r="H40" s="58"/>
+      <c r="I40" s="58"/>
+      <c r="K40"/>
+      <c r="L40"/>
+      <c r="M40"/>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="44"/>
+      <c r="B41" s="40"/>
+      <c r="C41" s="41"/>
+      <c r="D41" s="41"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="58"/>
+      <c r="G41" s="58"/>
+      <c r="H41" s="58"/>
+      <c r="I41" s="58"/>
+      <c r="K41"/>
+      <c r="L41"/>
+      <c r="M41"/>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42"/>
+      <c r="B42"/>
+      <c r="C42"/>
+      <c r="D42"/>
+      <c r="E42"/>
+      <c r="F42"/>
+      <c r="G42"/>
+      <c r="H42"/>
+      <c r="I42"/>
+      <c r="J42"/>
+      <c r="K42"/>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="B40" s="30"/>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="71"/>
-      <c r="F40" s="1" t="s">
+      <c r="B43" s="30"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="71"/>
+      <c r="F43" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
-      <c r="A41" s="39" t="s">
+    <row r="44" spans="1:13">
+      <c r="A44" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B41" s="36" t="s">
+      <c r="B44" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="72"/>
-      <c r="F41" s="57"/>
-      <c r="G41" s="57"/>
-      <c r="H41" s="57"/>
-      <c r="I41" s="57"/>
-      <c r="J41" s="57"/>
-      <c r="L41" s="37"/>
-      <c r="M41" s="37"/>
-    </row>
-    <row r="42" spans="1:13">
-      <c r="A42" s="43">
+      <c r="C44" s="36"/>
+      <c r="D44" s="36"/>
+      <c r="E44" s="72"/>
+      <c r="F44" s="57"/>
+      <c r="G44" s="57"/>
+      <c r="H44" s="57"/>
+      <c r="I44" s="57"/>
+      <c r="J44" s="57"/>
+      <c r="L44" s="37"/>
+      <c r="M44" s="37"/>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45" s="43">
         <v>1</v>
       </c>
-      <c r="B42" s="38" t="s">
+      <c r="B45" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="C42" s="32"/>
-      <c r="D42" s="32"/>
-      <c r="E42" s="33"/>
-      <c r="F42" s="58"/>
-      <c r="G42" s="58"/>
-      <c r="H42" s="58"/>
-      <c r="I42" s="58"/>
-      <c r="K42"/>
-      <c r="L42"/>
-      <c r="M42"/>
-    </row>
-    <row r="43" spans="1:13">
-      <c r="A43" s="43">
-        <v>2</v>
-      </c>
-      <c r="B43" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="C43" s="34"/>
-      <c r="D43" s="34"/>
-      <c r="E43" s="35"/>
-      <c r="F43" s="58"/>
-      <c r="G43" s="58"/>
-      <c r="H43" s="58"/>
-      <c r="I43" s="58"/>
-      <c r="K43"/>
-      <c r="L43"/>
-      <c r="M43"/>
-    </row>
-    <row r="44" spans="1:13">
-      <c r="A44" s="44"/>
-      <c r="B44" s="40"/>
-      <c r="C44" s="41"/>
-      <c r="D44" s="41"/>
-      <c r="E44" s="42"/>
-      <c r="F44" s="58"/>
-      <c r="G44" s="58"/>
-      <c r="H44" s="58"/>
-      <c r="I44" s="58"/>
-      <c r="K44"/>
-      <c r="L44"/>
-      <c r="M44"/>
-    </row>
-    <row r="45" spans="1:13">
-      <c r="A45" s="73"/>
-      <c r="B45" s="74"/>
-      <c r="C45" s="75"/>
-      <c r="D45" s="75"/>
-      <c r="E45" s="75"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="33"/>
       <c r="F45" s="58"/>
       <c r="G45" s="58"/>
       <c r="H45" s="58"/>
@@ -3264,41 +3289,43 @@
       <c r="M45"/>
     </row>
     <row r="46" spans="1:13">
-      <c r="A46" s="29" t="s">
-        <v>93</v>
-      </c>
-      <c r="B46" s="30"/>
-      <c r="C46" s="30"/>
-      <c r="D46" s="30"/>
-      <c r="E46" s="71"/>
-      <c r="F46" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="A46" s="43">
+        <v>2</v>
+      </c>
+      <c r="B46" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="C46" s="34"/>
+      <c r="D46" s="34"/>
+      <c r="E46" s="35"/>
+      <c r="F46" s="58"/>
+      <c r="G46" s="58"/>
+      <c r="H46" s="58"/>
+      <c r="I46" s="58"/>
+      <c r="K46"/>
+      <c r="L46"/>
+      <c r="M46"/>
     </row>
     <row r="47" spans="1:13">
-      <c r="A47" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="B47" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="C47" s="36"/>
-      <c r="D47" s="36"/>
-      <c r="E47" s="72"/>
-      <c r="F47" s="57"/>
-      <c r="G47" s="57"/>
-      <c r="H47" s="57"/>
-      <c r="I47" s="57"/>
-      <c r="J47" s="57"/>
-      <c r="L47" s="37"/>
-      <c r="M47" s="37"/>
+      <c r="A47" s="44"/>
+      <c r="B47" s="40"/>
+      <c r="C47" s="41"/>
+      <c r="D47" s="41"/>
+      <c r="E47" s="42"/>
+      <c r="F47" s="58"/>
+      <c r="G47" s="58"/>
+      <c r="H47" s="58"/>
+      <c r="I47" s="58"/>
+      <c r="K47"/>
+      <c r="L47"/>
+      <c r="M47"/>
     </row>
     <row r="48" spans="1:13">
-      <c r="A48" s="43"/>
-      <c r="B48" s="38"/>
-      <c r="C48" s="32"/>
-      <c r="D48" s="32"/>
-      <c r="E48" s="33"/>
+      <c r="A48" s="73"/>
+      <c r="B48" s="74"/>
+      <c r="C48" s="75"/>
+      <c r="D48" s="75"/>
+      <c r="E48" s="75"/>
       <c r="F48" s="58"/>
       <c r="G48" s="58"/>
       <c r="H48" s="58"/>
@@ -3308,128 +3335,130 @@
       <c r="M48"/>
     </row>
     <row r="49" spans="1:13">
-      <c r="A49" s="43"/>
-      <c r="B49" s="38"/>
-      <c r="C49" s="34"/>
-      <c r="D49" s="34"/>
-      <c r="E49" s="35"/>
-      <c r="F49" s="58"/>
-      <c r="G49" s="58"/>
-      <c r="H49" s="58"/>
-      <c r="I49" s="58"/>
-      <c r="K49"/>
-      <c r="L49"/>
-      <c r="M49"/>
+      <c r="A49" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="B49" s="30"/>
+      <c r="C49" s="30"/>
+      <c r="D49" s="30"/>
+      <c r="E49" s="71"/>
+      <c r="F49" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="50" spans="1:13">
-      <c r="A50" s="44"/>
-      <c r="B50" s="40"/>
-      <c r="C50" s="41"/>
-      <c r="D50" s="41"/>
-      <c r="E50" s="42"/>
-      <c r="F50" s="58"/>
-      <c r="G50" s="58"/>
-      <c r="H50" s="58"/>
-      <c r="I50" s="58"/>
-      <c r="K50"/>
-      <c r="L50"/>
-      <c r="M50"/>
+      <c r="A50" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" s="36"/>
+      <c r="D50" s="36"/>
+      <c r="E50" s="72"/>
+      <c r="F50" s="57"/>
+      <c r="G50" s="57"/>
+      <c r="H50" s="57"/>
+      <c r="I50" s="57"/>
+      <c r="J50" s="57"/>
+      <c r="L50" s="37"/>
+      <c r="M50" s="37"/>
     </row>
     <row r="51" spans="1:13">
-      <c r="A51"/>
-      <c r="B51"/>
-      <c r="C51"/>
-      <c r="D51"/>
-      <c r="E51"/>
-      <c r="F51"/>
-      <c r="G51"/>
-      <c r="H51"/>
-      <c r="I51"/>
-      <c r="J51"/>
+      <c r="A51" s="43"/>
+      <c r="B51" s="38"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="32"/>
+      <c r="E51" s="33"/>
+      <c r="F51" s="58"/>
+      <c r="G51" s="58"/>
+      <c r="H51" s="58"/>
+      <c r="I51" s="58"/>
       <c r="K51"/>
+      <c r="L51"/>
+      <c r="M51"/>
     </row>
     <row r="52" spans="1:13">
-      <c r="A52" s="29" t="s">
+      <c r="A52" s="43"/>
+      <c r="B52" s="38"/>
+      <c r="C52" s="34"/>
+      <c r="D52" s="34"/>
+      <c r="E52" s="35"/>
+      <c r="F52" s="58"/>
+      <c r="G52" s="58"/>
+      <c r="H52" s="58"/>
+      <c r="I52" s="58"/>
+      <c r="K52"/>
+      <c r="L52"/>
+      <c r="M52"/>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="A53" s="44"/>
+      <c r="B53" s="40"/>
+      <c r="C53" s="41"/>
+      <c r="D53" s="41"/>
+      <c r="E53" s="42"/>
+      <c r="F53" s="58"/>
+      <c r="G53" s="58"/>
+      <c r="H53" s="58"/>
+      <c r="I53" s="58"/>
+      <c r="K53"/>
+      <c r="L53"/>
+      <c r="M53"/>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54"/>
+      <c r="B54"/>
+      <c r="C54"/>
+      <c r="D54"/>
+      <c r="E54"/>
+      <c r="F54"/>
+      <c r="G54"/>
+      <c r="H54"/>
+      <c r="I54"/>
+      <c r="J54"/>
+      <c r="K54"/>
+    </row>
+    <row r="55" spans="1:13">
+      <c r="A55" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="B52" s="30"/>
-      <c r="C52" s="30"/>
-      <c r="D52" s="30"/>
-      <c r="E52" s="71"/>
-      <c r="F52" s="1" t="s">
+      <c r="B55" s="30"/>
+      <c r="C55" s="30"/>
+      <c r="D55" s="30"/>
+      <c r="E55" s="71"/>
+      <c r="F55" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="53" spans="1:13">
-      <c r="A53" s="39" t="s">
+    <row r="56" spans="1:13">
+      <c r="A56" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B53" s="36" t="s">
+      <c r="B56" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="C53" s="39" t="s">
+      <c r="C56" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="36" t="s">
+      <c r="D56" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="E53" s="72"/>
-      <c r="F53" s="57"/>
-      <c r="G53" s="57"/>
-      <c r="H53" s="57"/>
-      <c r="I53" s="57"/>
-      <c r="J53" s="57"/>
-      <c r="L53" s="37"/>
-      <c r="M53" s="37"/>
-    </row>
-    <row r="54" spans="1:13">
-      <c r="A54" s="43"/>
-      <c r="B54" s="38"/>
-      <c r="C54" s="81"/>
-      <c r="D54" s="32"/>
-      <c r="E54" s="33"/>
-      <c r="F54" s="58"/>
-      <c r="G54" s="58"/>
-      <c r="H54" s="58"/>
-      <c r="I54" s="58"/>
-      <c r="K54"/>
-      <c r="L54"/>
-      <c r="M54"/>
-    </row>
-    <row r="55" spans="1:13">
-      <c r="A55" s="43"/>
-      <c r="B55" s="38"/>
-      <c r="C55" s="82"/>
-      <c r="D55" s="34"/>
-      <c r="E55" s="35"/>
-      <c r="F55" s="58"/>
-      <c r="G55" s="58"/>
-      <c r="H55" s="58"/>
-      <c r="I55" s="58"/>
-      <c r="K55"/>
-      <c r="L55"/>
-      <c r="M55"/>
-    </row>
-    <row r="56" spans="1:13">
-      <c r="A56" s="44"/>
-      <c r="B56" s="40"/>
-      <c r="C56" s="83"/>
-      <c r="D56" s="41"/>
-      <c r="E56" s="42"/>
-      <c r="F56" s="58"/>
-      <c r="G56" s="58"/>
-      <c r="H56" s="58"/>
-      <c r="I56" s="58"/>
-      <c r="K56"/>
-      <c r="L56"/>
-      <c r="M56"/>
+      <c r="E56" s="72"/>
+      <c r="F56" s="57"/>
+      <c r="G56" s="57"/>
+      <c r="H56" s="57"/>
+      <c r="I56" s="57"/>
+      <c r="J56" s="57"/>
+      <c r="L56" s="37"/>
+      <c r="M56" s="37"/>
     </row>
     <row r="57" spans="1:13">
-      <c r="A57" s="73"/>
-      <c r="B57" s="74"/>
-      <c r="C57" s="75"/>
-      <c r="D57" s="75"/>
-      <c r="E57" s="75"/>
+      <c r="A57" s="43"/>
+      <c r="B57" s="38"/>
+      <c r="C57" s="81"/>
+      <c r="D57" s="32"/>
+      <c r="E57" s="33"/>
       <c r="F57" s="58"/>
       <c r="G57" s="58"/>
       <c r="H57" s="58"/>
@@ -3439,43 +3468,39 @@
       <c r="M57"/>
     </row>
     <row r="58" spans="1:13">
-      <c r="A58" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="B58" s="30"/>
-      <c r="C58" s="30"/>
-      <c r="D58" s="30"/>
-      <c r="E58" s="71"/>
-      <c r="F58" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="A58" s="43"/>
+      <c r="B58" s="38"/>
+      <c r="C58" s="82"/>
+      <c r="D58" s="34"/>
+      <c r="E58" s="35"/>
+      <c r="F58" s="58"/>
+      <c r="G58" s="58"/>
+      <c r="H58" s="58"/>
+      <c r="I58" s="58"/>
+      <c r="K58"/>
+      <c r="L58"/>
+      <c r="M58"/>
     </row>
     <row r="59" spans="1:13">
-      <c r="A59" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="B59" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="C59" s="36"/>
-      <c r="D59" s="36"/>
-      <c r="E59" s="72"/>
-      <c r="F59" s="57" t="s">
-        <v>103</v>
-      </c>
-      <c r="G59" s="57"/>
-      <c r="H59" s="57"/>
-      <c r="I59" s="57"/>
-      <c r="J59" s="57"/>
-      <c r="L59" s="37"/>
-      <c r="M59" s="37"/>
+      <c r="A59" s="44"/>
+      <c r="B59" s="40"/>
+      <c r="C59" s="83"/>
+      <c r="D59" s="41"/>
+      <c r="E59" s="42"/>
+      <c r="F59" s="58"/>
+      <c r="G59" s="58"/>
+      <c r="H59" s="58"/>
+      <c r="I59" s="58"/>
+      <c r="K59"/>
+      <c r="L59"/>
+      <c r="M59"/>
     </row>
     <row r="60" spans="1:13">
-      <c r="A60" s="43"/>
-      <c r="B60" s="38"/>
-      <c r="C60" s="32"/>
-      <c r="D60" s="32"/>
-      <c r="E60" s="33"/>
+      <c r="A60" s="73"/>
+      <c r="B60" s="74"/>
+      <c r="C60" s="75"/>
+      <c r="D60" s="75"/>
+      <c r="E60" s="75"/>
       <c r="F60" s="58"/>
       <c r="G60" s="58"/>
       <c r="H60" s="58"/>
@@ -3485,316 +3510,281 @@
       <c r="M60"/>
     </row>
     <row r="61" spans="1:13">
-      <c r="A61" s="43"/>
-      <c r="B61" s="38"/>
-      <c r="C61" s="34"/>
-      <c r="D61" s="34"/>
-      <c r="E61" s="35"/>
-      <c r="F61" s="58"/>
-      <c r="G61" s="58"/>
-      <c r="H61" s="58"/>
-      <c r="I61" s="58"/>
-      <c r="K61"/>
-      <c r="L61"/>
-      <c r="M61"/>
+      <c r="A61" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="B61" s="30"/>
+      <c r="C61" s="30"/>
+      <c r="D61" s="30"/>
+      <c r="E61" s="71"/>
+      <c r="F61" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="62" spans="1:13">
-      <c r="A62" s="44"/>
-      <c r="B62" s="40"/>
-      <c r="C62" s="41"/>
-      <c r="D62" s="41"/>
-      <c r="E62" s="42"/>
-      <c r="F62" s="58"/>
-      <c r="G62" s="58"/>
-      <c r="H62" s="58"/>
-      <c r="I62" s="58"/>
-      <c r="K62"/>
-      <c r="L62"/>
-      <c r="M62"/>
+      <c r="A62" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="B62" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" s="36"/>
+      <c r="D62" s="36"/>
+      <c r="E62" s="72"/>
+      <c r="F62" s="57" t="s">
+        <v>103</v>
+      </c>
+      <c r="G62" s="57"/>
+      <c r="H62" s="57"/>
+      <c r="I62" s="57"/>
+      <c r="J62" s="57"/>
+      <c r="L62" s="37"/>
+      <c r="M62" s="37"/>
     </row>
     <row r="63" spans="1:13">
-      <c r="A63"/>
-      <c r="B63"/>
-      <c r="C63"/>
-      <c r="D63"/>
-      <c r="E63"/>
-      <c r="F63"/>
-      <c r="G63"/>
-      <c r="H63"/>
-      <c r="I63"/>
-      <c r="J63"/>
+      <c r="A63" s="43"/>
+      <c r="B63" s="38"/>
+      <c r="C63" s="32"/>
+      <c r="D63" s="32"/>
+      <c r="E63" s="33"/>
+      <c r="F63" s="58"/>
+      <c r="G63" s="58"/>
+      <c r="H63" s="58"/>
+      <c r="I63" s="58"/>
       <c r="K63"/>
+      <c r="L63"/>
+      <c r="M63"/>
     </row>
     <row r="64" spans="1:13">
-      <c r="A64"/>
-      <c r="B64" t="s">
+      <c r="A64" s="43"/>
+      <c r="B64" s="38"/>
+      <c r="C64" s="34"/>
+      <c r="D64" s="34"/>
+      <c r="E64" s="35"/>
+      <c r="F64" s="58"/>
+      <c r="G64" s="58"/>
+      <c r="H64" s="58"/>
+      <c r="I64" s="58"/>
+      <c r="K64"/>
+      <c r="L64"/>
+      <c r="M64"/>
+    </row>
+    <row r="65" spans="1:14">
+      <c r="A65" s="44"/>
+      <c r="B65" s="40"/>
+      <c r="C65" s="41"/>
+      <c r="D65" s="41"/>
+      <c r="E65" s="42"/>
+      <c r="F65" s="58"/>
+      <c r="G65" s="58"/>
+      <c r="H65" s="58"/>
+      <c r="I65" s="58"/>
+      <c r="K65"/>
+      <c r="L65"/>
+      <c r="M65"/>
+    </row>
+    <row r="66" spans="1:14">
+      <c r="A66"/>
+      <c r="B66"/>
+      <c r="C66"/>
+      <c r="D66"/>
+      <c r="E66"/>
+      <c r="F66"/>
+      <c r="G66"/>
+      <c r="H66"/>
+      <c r="I66"/>
+      <c r="J66"/>
+      <c r="K66"/>
+    </row>
+    <row r="67" spans="1:14">
+      <c r="A67"/>
+      <c r="B67" t="s">
         <v>78</v>
       </c>
-      <c r="C64"/>
-      <c r="D64"/>
-      <c r="E64"/>
-      <c r="F64"/>
-      <c r="G64"/>
-      <c r="H64"/>
-      <c r="I64"/>
-      <c r="J64"/>
-      <c r="K64"/>
-    </row>
-    <row r="65" spans="1:14">
-      <c r="A65" s="3" t="s">
+      <c r="C67"/>
+      <c r="D67"/>
+      <c r="E67"/>
+      <c r="F67"/>
+      <c r="G67"/>
+      <c r="H67"/>
+      <c r="I67"/>
+      <c r="J67"/>
+      <c r="K67"/>
+    </row>
+    <row r="68" spans="1:14">
+      <c r="A68" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B65" s="13"/>
-      <c r="C65" s="13"/>
-      <c r="D65" s="13"/>
-      <c r="E65" s="13"/>
-      <c r="F65" s="13"/>
-      <c r="G65" s="13"/>
-      <c r="H65" s="13"/>
-      <c r="I65" s="13"/>
-      <c r="J65" s="13"/>
-      <c r="K65" s="13"/>
-      <c r="L65" s="13"/>
-      <c r="M65" s="6"/>
-      <c r="N65" s="14"/>
-    </row>
-    <row r="66" spans="1:14" ht="13.5" customHeight="1">
-      <c r="A66" s="119" t="s">
+      <c r="B68" s="13"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="13"/>
+      <c r="E68" s="13"/>
+      <c r="F68" s="13"/>
+      <c r="G68" s="13"/>
+      <c r="H68" s="13"/>
+      <c r="I68" s="13"/>
+      <c r="J68" s="13"/>
+      <c r="K68" s="13"/>
+      <c r="L68" s="13"/>
+      <c r="M68" s="6"/>
+      <c r="N68" s="14"/>
+    </row>
+    <row r="69" spans="1:14" ht="13.5" customHeight="1">
+      <c r="A69" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="B66" s="119" t="s">
+      <c r="B69" s="119" t="s">
         <v>3</v>
       </c>
-      <c r="C66" s="116" t="s">
+      <c r="C69" s="116" t="s">
         <v>4</v>
       </c>
-      <c r="D66" s="116" t="s">
+      <c r="D69" s="116" t="s">
         <v>6</v>
       </c>
-      <c r="E66" s="116" t="s">
+      <c r="E69" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="F66" s="117" t="s">
+      <c r="F69" s="117" t="s">
         <v>33</v>
       </c>
-      <c r="G66" s="117" t="s">
+      <c r="G69" s="117" t="s">
         <v>16</v>
       </c>
-      <c r="H66" s="127" t="s">
+      <c r="H69" s="127" t="s">
         <v>130</v>
       </c>
-      <c r="I66" s="127" t="s">
+      <c r="I69" s="127" t="s">
         <v>106</v>
       </c>
-      <c r="J66" s="116" t="s">
+      <c r="J69" s="116" t="s">
         <v>1</v>
       </c>
-      <c r="K66" s="116"/>
-      <c r="L66" s="15"/>
-      <c r="M66" s="16"/>
-      <c r="N66" s="9"/>
-    </row>
-    <row r="67" spans="1:14">
-      <c r="A67" s="119"/>
-      <c r="B67" s="119"/>
-      <c r="C67" s="116"/>
-      <c r="D67" s="116"/>
-      <c r="E67" s="116"/>
-      <c r="F67" s="118"/>
-      <c r="G67" s="118"/>
-      <c r="H67" s="128"/>
-      <c r="I67" s="128"/>
-      <c r="J67" s="116"/>
-      <c r="K67" s="116"/>
-      <c r="L67" s="17"/>
-      <c r="M67" s="28"/>
-      <c r="N67" s="14"/>
-    </row>
-    <row r="68" spans="1:14">
-      <c r="A68" s="18">
-        <v>1</v>
-      </c>
-      <c r="B68" s="61" t="s">
-        <v>47</v>
-      </c>
-      <c r="C68" s="68" t="s">
-        <v>48</v>
-      </c>
-      <c r="D68" s="19"/>
-      <c r="E68" s="19"/>
-      <c r="F68" s="19"/>
-      <c r="G68" s="59"/>
-      <c r="H68" s="59"/>
-      <c r="I68" s="59"/>
-      <c r="J68" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="K68" s="20"/>
-      <c r="L68" s="20"/>
-      <c r="M68" s="27"/>
-      <c r="N68" s="14"/>
-    </row>
-    <row r="69" spans="1:14">
-      <c r="A69" s="18">
-        <f>A68+1</f>
-        <v>2</v>
-      </c>
-      <c r="B69" s="61" t="s">
-        <v>49</v>
-      </c>
-      <c r="C69" s="68" t="s">
-        <v>50</v>
-      </c>
-      <c r="D69" s="19"/>
-      <c r="E69" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="F69" s="19"/>
-      <c r="G69" s="59"/>
-      <c r="H69" s="59"/>
-      <c r="I69" s="59"/>
-      <c r="J69" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="K69" s="20"/>
-      <c r="L69" s="20"/>
-      <c r="M69" s="27"/>
-      <c r="N69" s="14"/>
+      <c r="K69" s="116"/>
+      <c r="L69" s="15"/>
+      <c r="M69" s="16"/>
+      <c r="N69" s="9"/>
     </row>
     <row r="70" spans="1:14">
-      <c r="A70" s="18">
-        <f t="shared" ref="A70:A84" si="0">A69+1</f>
-        <v>3</v>
-      </c>
-      <c r="B70" s="62" t="s">
-        <v>52</v>
-      </c>
-      <c r="C70" s="69" t="s">
-        <v>53</v>
-      </c>
-      <c r="D70" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="E70" s="19"/>
-      <c r="F70" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G70" s="59" t="s">
-        <v>14</v>
-      </c>
-      <c r="H70" s="59"/>
-      <c r="I70" s="59"/>
-      <c r="J70" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="K70" s="20"/>
-      <c r="L70" s="20"/>
-      <c r="M70" s="21"/>
+      <c r="A70" s="119"/>
+      <c r="B70" s="119"/>
+      <c r="C70" s="116"/>
+      <c r="D70" s="116"/>
+      <c r="E70" s="116"/>
+      <c r="F70" s="118"/>
+      <c r="G70" s="118"/>
+      <c r="H70" s="128"/>
+      <c r="I70" s="128"/>
+      <c r="J70" s="116"/>
+      <c r="K70" s="116"/>
+      <c r="L70" s="17"/>
+      <c r="M70" s="28"/>
       <c r="N70" s="14"/>
     </row>
     <row r="71" spans="1:14">
       <c r="A71" s="18">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B71" s="63" t="s">
-        <v>58</v>
-      </c>
-      <c r="C71" s="70" t="s">
-        <v>54</v>
+        <v>1</v>
+      </c>
+      <c r="B71" s="61" t="s">
+        <v>47</v>
+      </c>
+      <c r="C71" s="68" t="s">
+        <v>48</v>
       </c>
       <c r="D71" s="19"/>
       <c r="E71" s="19"/>
       <c r="F71" s="19"/>
-      <c r="G71" s="59" t="s">
-        <v>14</v>
-      </c>
+      <c r="G71" s="59"/>
       <c r="H71" s="59"/>
       <c r="I71" s="59"/>
       <c r="J71" s="19" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K71" s="20"/>
       <c r="L71" s="20"/>
-      <c r="M71" s="21"/>
+      <c r="M71" s="27"/>
       <c r="N71" s="14"/>
     </row>
     <row r="72" spans="1:14">
       <c r="A72" s="18">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B72" s="63" t="s">
-        <v>107</v>
-      </c>
-      <c r="C72" s="70" t="s">
-        <v>48</v>
+        <f>A71+1</f>
+        <v>2</v>
+      </c>
+      <c r="B72" s="61" t="s">
+        <v>49</v>
+      </c>
+      <c r="C72" s="68" t="s">
+        <v>50</v>
       </c>
       <c r="D72" s="19"/>
-      <c r="E72" s="19"/>
+      <c r="E72" s="19" t="b">
+        <v>1</v>
+      </c>
       <c r="F72" s="19"/>
-      <c r="G72" s="59" t="s">
-        <v>14</v>
-      </c>
-      <c r="H72" s="59" t="s">
-        <v>107</v>
-      </c>
-      <c r="I72" s="59" t="s">
-        <v>131</v>
-      </c>
+      <c r="G72" s="59"/>
+      <c r="H72" s="59"/>
+      <c r="I72" s="59"/>
       <c r="J72" s="19" t="s">
-        <v>108</v>
+        <v>51</v>
       </c>
       <c r="K72" s="20"/>
       <c r="L72" s="20"/>
-      <c r="M72" s="21"/>
+      <c r="M72" s="27"/>
       <c r="N72" s="14"/>
     </row>
     <row r="73" spans="1:14">
       <c r="A73" s="18">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B73" s="63" t="s">
-        <v>113</v>
-      </c>
-      <c r="C73" s="70" t="s">
-        <v>48</v>
-      </c>
-      <c r="D73" s="64"/>
-      <c r="E73" s="64" t="s">
-        <v>114</v>
-      </c>
-      <c r="F73" s="64"/>
-      <c r="G73" s="65" t="s">
+        <f t="shared" ref="A73:A87" si="0">A72+1</f>
+        <v>3</v>
+      </c>
+      <c r="B73" s="62" t="s">
+        <v>52</v>
+      </c>
+      <c r="C73" s="69" t="s">
+        <v>53</v>
+      </c>
+      <c r="D73" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E73" s="19"/>
+      <c r="F73" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="H73" s="65"/>
-      <c r="I73" s="65" t="s">
-        <v>113</v>
-      </c>
+      <c r="G73" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="H73" s="59"/>
+      <c r="I73" s="59"/>
       <c r="J73" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="K73" s="66"/>
-      <c r="L73" s="66"/>
-      <c r="M73" s="67"/>
+        <v>55</v>
+      </c>
+      <c r="K73" s="20"/>
+      <c r="L73" s="20"/>
+      <c r="M73" s="21"/>
       <c r="N73" s="14"/>
     </row>
     <row r="74" spans="1:14">
       <c r="A74" s="18">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B74" s="63"/>
-      <c r="C74" s="70"/>
+        <v>4</v>
+      </c>
+      <c r="B74" s="63" t="s">
+        <v>58</v>
+      </c>
+      <c r="C74" s="70" t="s">
+        <v>54</v>
+      </c>
       <c r="D74" s="19"/>
       <c r="E74" s="19"/>
       <c r="F74" s="19"/>
-      <c r="G74" s="59"/>
+      <c r="G74" s="59" t="s">
+        <v>14</v>
+      </c>
       <c r="H74" s="59"/>
       <c r="I74" s="59"/>
-      <c r="J74" s="19"/>
+      <c r="J74" s="19" t="s">
+        <v>59</v>
+      </c>
       <c r="K74" s="20"/>
       <c r="L74" s="20"/>
       <c r="M74" s="21"/>
@@ -3803,36 +3793,60 @@
     <row r="75" spans="1:14">
       <c r="A75" s="18">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B75" s="63"/>
-      <c r="C75" s="70"/>
-      <c r="D75" s="64"/>
-      <c r="E75" s="64"/>
-      <c r="F75" s="64"/>
-      <c r="G75" s="65"/>
-      <c r="H75" s="65"/>
-      <c r="I75" s="65"/>
-      <c r="J75" s="64"/>
-      <c r="K75" s="66"/>
-      <c r="L75" s="66"/>
-      <c r="M75" s="67"/>
+        <v>5</v>
+      </c>
+      <c r="B75" s="63" t="s">
+        <v>107</v>
+      </c>
+      <c r="C75" s="70" t="s">
+        <v>48</v>
+      </c>
+      <c r="D75" s="19"/>
+      <c r="E75" s="19"/>
+      <c r="F75" s="19"/>
+      <c r="G75" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="H75" s="59" t="s">
+        <v>107</v>
+      </c>
+      <c r="I75" s="59" t="s">
+        <v>131</v>
+      </c>
+      <c r="J75" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="K75" s="20"/>
+      <c r="L75" s="20"/>
+      <c r="M75" s="21"/>
       <c r="N75" s="14"/>
     </row>
     <row r="76" spans="1:14">
       <c r="A76" s="18">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B76" s="63"/>
-      <c r="C76" s="70"/>
+        <v>6</v>
+      </c>
+      <c r="B76" s="63" t="s">
+        <v>113</v>
+      </c>
+      <c r="C76" s="70" t="s">
+        <v>48</v>
+      </c>
       <c r="D76" s="64"/>
-      <c r="E76" s="64"/>
+      <c r="E76" s="64" t="s">
+        <v>114</v>
+      </c>
       <c r="F76" s="64"/>
-      <c r="G76" s="65"/>
+      <c r="G76" s="65" t="s">
+        <v>14</v>
+      </c>
       <c r="H76" s="65"/>
-      <c r="I76" s="65"/>
-      <c r="J76" s="64"/>
+      <c r="I76" s="65" t="s">
+        <v>113</v>
+      </c>
+      <c r="J76" s="19" t="s">
+        <v>108</v>
+      </c>
       <c r="K76" s="66"/>
       <c r="L76" s="66"/>
       <c r="M76" s="67"/>
@@ -3841,7 +3855,7 @@
     <row r="77" spans="1:14">
       <c r="A77" s="18">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B77" s="63"/>
       <c r="C77" s="70"/>
@@ -3860,7 +3874,7 @@
     <row r="78" spans="1:14">
       <c r="A78" s="18">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B78" s="63"/>
       <c r="C78" s="70"/>
@@ -3879,7 +3893,7 @@
     <row r="79" spans="1:14">
       <c r="A79" s="18">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B79" s="63"/>
       <c r="C79" s="70"/>
@@ -3898,7 +3912,7 @@
     <row r="80" spans="1:14">
       <c r="A80" s="18">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B80" s="63"/>
       <c r="C80" s="70"/>
@@ -3917,7 +3931,7 @@
     <row r="81" spans="1:14">
       <c r="A81" s="18">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B81" s="63"/>
       <c r="C81" s="70"/>
@@ -3936,7 +3950,7 @@
     <row r="82" spans="1:14">
       <c r="A82" s="18">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B82" s="63"/>
       <c r="C82" s="70"/>
@@ -3955,7 +3969,7 @@
     <row r="83" spans="1:14">
       <c r="A83" s="18">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B83" s="63"/>
       <c r="C83" s="70"/>
@@ -3974,7 +3988,7 @@
     <row r="84" spans="1:14">
       <c r="A84" s="18">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B84" s="63"/>
       <c r="C84" s="70"/>
@@ -3991,266 +4005,252 @@
       <c r="N84" s="14"/>
     </row>
     <row r="85" spans="1:14">
-      <c r="A85" s="22"/>
-      <c r="B85" s="23"/>
-      <c r="C85" s="24"/>
-      <c r="D85" s="24"/>
-      <c r="E85" s="24"/>
-      <c r="F85" s="24"/>
-      <c r="G85" s="60"/>
-      <c r="H85" s="60"/>
-      <c r="I85" s="60"/>
-      <c r="J85" s="24"/>
-      <c r="K85" s="25"/>
-      <c r="L85" s="25"/>
-      <c r="M85" s="26"/>
+      <c r="A85" s="18">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B85" s="63"/>
+      <c r="C85" s="70"/>
+      <c r="D85" s="64"/>
+      <c r="E85" s="64"/>
+      <c r="F85" s="64"/>
+      <c r="G85" s="65"/>
+      <c r="H85" s="65"/>
+      <c r="I85" s="65"/>
+      <c r="J85" s="64"/>
+      <c r="K85" s="66"/>
+      <c r="L85" s="66"/>
+      <c r="M85" s="67"/>
       <c r="N85" s="14"/>
     </row>
+    <row r="86" spans="1:14">
+      <c r="A86" s="18">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B86" s="63"/>
+      <c r="C86" s="70"/>
+      <c r="D86" s="19"/>
+      <c r="E86" s="19"/>
+      <c r="F86" s="19"/>
+      <c r="G86" s="59"/>
+      <c r="H86" s="59"/>
+      <c r="I86" s="59"/>
+      <c r="J86" s="19"/>
+      <c r="K86" s="20"/>
+      <c r="L86" s="20"/>
+      <c r="M86" s="21"/>
+      <c r="N86" s="14"/>
+    </row>
     <row r="87" spans="1:14">
-      <c r="A87" s="29" t="s">
+      <c r="A87" s="18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B87" s="63"/>
+      <c r="C87" s="70"/>
+      <c r="D87" s="64"/>
+      <c r="E87" s="64"/>
+      <c r="F87" s="64"/>
+      <c r="G87" s="65"/>
+      <c r="H87" s="65"/>
+      <c r="I87" s="65"/>
+      <c r="J87" s="64"/>
+      <c r="K87" s="66"/>
+      <c r="L87" s="66"/>
+      <c r="M87" s="67"/>
+      <c r="N87" s="14"/>
+    </row>
+    <row r="88" spans="1:14">
+      <c r="A88" s="22"/>
+      <c r="B88" s="23"/>
+      <c r="C88" s="24"/>
+      <c r="D88" s="24"/>
+      <c r="E88" s="24"/>
+      <c r="F88" s="24"/>
+      <c r="G88" s="60"/>
+      <c r="H88" s="60"/>
+      <c r="I88" s="60"/>
+      <c r="J88" s="24"/>
+      <c r="K88" s="25"/>
+      <c r="L88" s="25"/>
+      <c r="M88" s="26"/>
+      <c r="N88" s="14"/>
+    </row>
+    <row r="90" spans="1:14">
+      <c r="A90" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="B87" s="30"/>
-      <c r="C87" s="30"/>
-      <c r="D87" s="30"/>
-      <c r="E87" s="71"/>
-      <c r="F87" s="1" t="s">
+      <c r="B90" s="30"/>
+      <c r="C90" s="30"/>
+      <c r="D90" s="30"/>
+      <c r="E90" s="71"/>
+      <c r="F90" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="88" spans="1:14">
-      <c r="A88" s="39" t="s">
+    <row r="91" spans="1:14">
+      <c r="A91" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B88" s="36" t="s">
+      <c r="B91" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C88" s="36"/>
-      <c r="D88" s="36"/>
-      <c r="E88" s="72"/>
-      <c r="F88" s="57"/>
-      <c r="G88" s="57"/>
-      <c r="H88" s="57"/>
-      <c r="I88" s="57"/>
-      <c r="J88" s="57"/>
-      <c r="L88" s="37"/>
-      <c r="M88" s="37"/>
-    </row>
-    <row r="89" spans="1:14">
-      <c r="A89" s="43"/>
-      <c r="B89" s="38"/>
-      <c r="C89" s="32"/>
-      <c r="D89" s="32"/>
-      <c r="E89" s="33"/>
-      <c r="F89" s="58"/>
-      <c r="G89" s="58"/>
-      <c r="H89" s="58"/>
-      <c r="I89" s="58"/>
-      <c r="K89"/>
-      <c r="L89"/>
-      <c r="M89"/>
-    </row>
-    <row r="90" spans="1:14">
-      <c r="A90" s="43"/>
-      <c r="B90" s="38"/>
-      <c r="C90" s="34"/>
-      <c r="D90" s="34"/>
-      <c r="E90" s="35"/>
-      <c r="F90" s="58"/>
-      <c r="G90" s="58"/>
-      <c r="H90" s="58"/>
-      <c r="I90" s="58"/>
-      <c r="K90"/>
-      <c r="L90"/>
-      <c r="M90"/>
-    </row>
-    <row r="91" spans="1:14">
-      <c r="A91" s="44"/>
-      <c r="B91" s="40"/>
-      <c r="C91" s="41"/>
-      <c r="D91" s="41"/>
-      <c r="E91" s="42"/>
-      <c r="F91" s="58"/>
-      <c r="G91" s="58"/>
-      <c r="H91" s="58"/>
-      <c r="I91" s="58"/>
-      <c r="K91"/>
-      <c r="L91"/>
-      <c r="M91"/>
+      <c r="C91" s="36"/>
+      <c r="D91" s="36"/>
+      <c r="E91" s="72"/>
+      <c r="F91" s="57"/>
+      <c r="G91" s="57"/>
+      <c r="H91" s="57"/>
+      <c r="I91" s="57"/>
+      <c r="J91" s="57"/>
+      <c r="L91" s="37"/>
+      <c r="M91" s="37"/>
     </row>
     <row r="92" spans="1:14">
-      <c r="A92"/>
-      <c r="B92"/>
-      <c r="C92"/>
-      <c r="D92"/>
-      <c r="E92"/>
-      <c r="F92"/>
-      <c r="G92"/>
-      <c r="H92"/>
-      <c r="I92"/>
-      <c r="J92"/>
+      <c r="A92" s="43"/>
+      <c r="B92" s="38"/>
+      <c r="C92" s="32"/>
+      <c r="D92" s="32"/>
+      <c r="E92" s="33"/>
+      <c r="F92" s="58"/>
+      <c r="G92" s="58"/>
+      <c r="H92" s="58"/>
+      <c r="I92" s="58"/>
       <c r="K92"/>
+      <c r="L92"/>
+      <c r="M92"/>
     </row>
     <row r="93" spans="1:14">
-      <c r="A93"/>
-      <c r="B93" t="s">
+      <c r="A93" s="43"/>
+      <c r="B93" s="38"/>
+      <c r="C93" s="34"/>
+      <c r="D93" s="34"/>
+      <c r="E93" s="35"/>
+      <c r="F93" s="58"/>
+      <c r="G93" s="58"/>
+      <c r="H93" s="58"/>
+      <c r="I93" s="58"/>
+      <c r="K93"/>
+      <c r="L93"/>
+      <c r="M93"/>
+    </row>
+    <row r="94" spans="1:14">
+      <c r="A94" s="44"/>
+      <c r="B94" s="40"/>
+      <c r="C94" s="41"/>
+      <c r="D94" s="41"/>
+      <c r="E94" s="42"/>
+      <c r="F94" s="58"/>
+      <c r="G94" s="58"/>
+      <c r="H94" s="58"/>
+      <c r="I94" s="58"/>
+      <c r="K94"/>
+      <c r="L94"/>
+      <c r="M94"/>
+    </row>
+    <row r="95" spans="1:14">
+      <c r="A95"/>
+      <c r="B95"/>
+      <c r="C95"/>
+      <c r="D95"/>
+      <c r="E95"/>
+      <c r="F95"/>
+      <c r="G95"/>
+      <c r="H95"/>
+      <c r="I95"/>
+      <c r="J95"/>
+      <c r="K95"/>
+    </row>
+    <row r="96" spans="1:14">
+      <c r="A96"/>
+      <c r="B96" t="s">
         <v>85</v>
       </c>
-      <c r="C93"/>
-      <c r="D93"/>
-      <c r="E93"/>
-      <c r="F93"/>
-      <c r="G93"/>
-      <c r="H93"/>
-      <c r="I93"/>
-      <c r="J93"/>
-      <c r="K93"/>
-    </row>
-    <row r="94" spans="1:14">
-      <c r="A94" s="3" t="s">
+      <c r="C96"/>
+      <c r="D96"/>
+      <c r="E96"/>
+      <c r="F96"/>
+      <c r="G96"/>
+      <c r="H96"/>
+      <c r="I96"/>
+      <c r="J96"/>
+      <c r="K96"/>
+    </row>
+    <row r="97" spans="1:14">
+      <c r="A97" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B94" s="13"/>
-      <c r="C94" s="13"/>
-      <c r="D94" s="13"/>
-      <c r="E94" s="13"/>
-      <c r="F94" s="13"/>
-      <c r="G94" s="13"/>
-      <c r="H94" s="13"/>
-      <c r="I94" s="13"/>
-      <c r="J94" s="13"/>
-      <c r="K94" s="13"/>
-      <c r="L94" s="13"/>
-      <c r="M94" s="6"/>
-      <c r="N94" s="14"/>
-    </row>
-    <row r="95" spans="1:14" ht="13.5" customHeight="1">
-      <c r="A95" s="119" t="s">
+      <c r="B97" s="13"/>
+      <c r="C97" s="13"/>
+      <c r="D97" s="13"/>
+      <c r="E97" s="13"/>
+      <c r="F97" s="13"/>
+      <c r="G97" s="13"/>
+      <c r="H97" s="13"/>
+      <c r="I97" s="13"/>
+      <c r="J97" s="13"/>
+      <c r="K97" s="13"/>
+      <c r="L97" s="13"/>
+      <c r="M97" s="6"/>
+      <c r="N97" s="14"/>
+    </row>
+    <row r="98" spans="1:14" ht="13.5" customHeight="1">
+      <c r="A98" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="B95" s="119" t="s">
+      <c r="B98" s="119" t="s">
         <v>84</v>
       </c>
-      <c r="C95" s="116" t="s">
+      <c r="C98" s="116" t="s">
         <v>86</v>
       </c>
-      <c r="D95" s="116" t="s">
+      <c r="D98" s="116" t="s">
         <v>87</v>
       </c>
-      <c r="E95" s="116" t="s">
+      <c r="E98" s="116" t="s">
         <v>81</v>
       </c>
-      <c r="F95" s="113"/>
-      <c r="G95" s="113"/>
-      <c r="H95" s="113"/>
-      <c r="I95" s="113"/>
-      <c r="J95" s="115"/>
-      <c r="K95" s="116"/>
-      <c r="L95" s="15"/>
-      <c r="M95" s="16"/>
-      <c r="N95" s="9"/>
-    </row>
-    <row r="96" spans="1:14">
-      <c r="A96" s="119"/>
-      <c r="B96" s="119"/>
-      <c r="C96" s="116"/>
-      <c r="D96" s="116"/>
-      <c r="E96" s="116"/>
-      <c r="F96" s="114"/>
-      <c r="G96" s="114"/>
-      <c r="H96" s="114"/>
-      <c r="I96" s="114"/>
-      <c r="J96" s="115"/>
-      <c r="K96" s="116"/>
-      <c r="L96" s="17"/>
-      <c r="M96" s="28"/>
-      <c r="N96" s="14"/>
-    </row>
-    <row r="97" spans="1:14">
-      <c r="A97" s="18">
-        <v>1</v>
-      </c>
-      <c r="B97" s="61" t="s">
-        <v>88</v>
-      </c>
-      <c r="C97" s="68" t="s">
-        <v>48</v>
-      </c>
-      <c r="D97" s="19"/>
-      <c r="E97" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="F97" s="77"/>
-      <c r="G97" s="79"/>
-      <c r="H97" s="79"/>
-      <c r="I97" s="79"/>
-      <c r="J97" s="77"/>
-      <c r="K97" s="20"/>
-      <c r="L97" s="20"/>
-      <c r="M97" s="27"/>
-      <c r="N97" s="14"/>
-    </row>
-    <row r="98" spans="1:14">
-      <c r="A98" s="18">
-        <f>A97+1</f>
-        <v>2</v>
-      </c>
-      <c r="B98" s="61" t="s">
-        <v>89</v>
-      </c>
-      <c r="C98" s="68" t="s">
-        <v>90</v>
-      </c>
-      <c r="D98" s="19"/>
-      <c r="E98" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="F98" s="77"/>
-      <c r="G98" s="79"/>
-      <c r="H98" s="79"/>
-      <c r="I98" s="79"/>
-      <c r="J98" s="77"/>
-      <c r="K98" s="20"/>
-      <c r="L98" s="20"/>
-      <c r="M98" s="27"/>
-      <c r="N98" s="14"/>
+      <c r="F98" s="113"/>
+      <c r="G98" s="113"/>
+      <c r="H98" s="113"/>
+      <c r="I98" s="113"/>
+      <c r="J98" s="115"/>
+      <c r="K98" s="116"/>
+      <c r="L98" s="15"/>
+      <c r="M98" s="16"/>
+      <c r="N98" s="9"/>
     </row>
     <row r="99" spans="1:14">
-      <c r="A99" s="18">
-        <f t="shared" ref="A99:A103" si="1">A98+1</f>
-        <v>3</v>
-      </c>
-      <c r="B99" s="62" t="s">
-        <v>101</v>
-      </c>
-      <c r="C99" s="69" t="s">
-        <v>53</v>
-      </c>
-      <c r="D99" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="E99" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="F99" s="77"/>
-      <c r="G99" s="79"/>
-      <c r="H99" s="79"/>
-      <c r="I99" s="79"/>
-      <c r="J99" s="77"/>
-      <c r="K99" s="20"/>
-      <c r="L99" s="20"/>
-      <c r="M99" s="21"/>
+      <c r="A99" s="119"/>
+      <c r="B99" s="119"/>
+      <c r="C99" s="116"/>
+      <c r="D99" s="116"/>
+      <c r="E99" s="116"/>
+      <c r="F99" s="114"/>
+      <c r="G99" s="114"/>
+      <c r="H99" s="114"/>
+      <c r="I99" s="114"/>
+      <c r="J99" s="115"/>
+      <c r="K99" s="116"/>
+      <c r="L99" s="17"/>
+      <c r="M99" s="28"/>
       <c r="N99" s="14"/>
     </row>
     <row r="100" spans="1:14">
       <c r="A100" s="18">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="B100" s="63"/>
-      <c r="C100" s="70"/>
+        <v>1</v>
+      </c>
+      <c r="B100" s="61" t="s">
+        <v>88</v>
+      </c>
+      <c r="C100" s="68" t="s">
+        <v>48</v>
+      </c>
       <c r="D100" s="19"/>
-      <c r="E100" s="19"/>
+      <c r="E100" s="19" t="s">
+        <v>99</v>
+      </c>
       <c r="F100" s="77"/>
       <c r="G100" s="79"/>
       <c r="H100" s="79"/>
@@ -4258,18 +4258,24 @@
       <c r="J100" s="77"/>
       <c r="K100" s="20"/>
       <c r="L100" s="20"/>
-      <c r="M100" s="21"/>
+      <c r="M100" s="27"/>
       <c r="N100" s="14"/>
     </row>
     <row r="101" spans="1:14">
       <c r="A101" s="18">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="B101" s="63"/>
-      <c r="C101" s="70"/>
+        <f>A100+1</f>
+        <v>2</v>
+      </c>
+      <c r="B101" s="61" t="s">
+        <v>89</v>
+      </c>
+      <c r="C101" s="68" t="s">
+        <v>90</v>
+      </c>
       <c r="D101" s="19"/>
-      <c r="E101" s="19"/>
+      <c r="E101" s="19" t="s">
+        <v>100</v>
+      </c>
       <c r="F101" s="77"/>
       <c r="G101" s="79"/>
       <c r="H101" s="79"/>
@@ -4277,32 +4283,40 @@
       <c r="J101" s="77"/>
       <c r="K101" s="20"/>
       <c r="L101" s="20"/>
-      <c r="M101" s="21"/>
+      <c r="M101" s="27"/>
       <c r="N101" s="14"/>
     </row>
     <row r="102" spans="1:14">
       <c r="A102" s="18">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="B102" s="63"/>
-      <c r="C102" s="70"/>
-      <c r="D102" s="64"/>
-      <c r="E102" s="64"/>
-      <c r="F102" s="78"/>
-      <c r="G102" s="80"/>
-      <c r="H102" s="80"/>
-      <c r="I102" s="80"/>
-      <c r="J102" s="78"/>
-      <c r="K102" s="66"/>
-      <c r="L102" s="66"/>
-      <c r="M102" s="67"/>
+        <f t="shared" ref="A102:A106" si="1">A101+1</f>
+        <v>3</v>
+      </c>
+      <c r="B102" s="62" t="s">
+        <v>101</v>
+      </c>
+      <c r="C102" s="69" t="s">
+        <v>53</v>
+      </c>
+      <c r="D102" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E102" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="F102" s="77"/>
+      <c r="G102" s="79"/>
+      <c r="H102" s="79"/>
+      <c r="I102" s="79"/>
+      <c r="J102" s="77"/>
+      <c r="K102" s="20"/>
+      <c r="L102" s="20"/>
+      <c r="M102" s="21"/>
       <c r="N102" s="14"/>
     </row>
     <row r="103" spans="1:14">
       <c r="A103" s="18">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B103" s="63"/>
       <c r="C103" s="70"/>
@@ -4318,62 +4332,119 @@
       <c r="M103" s="21"/>
       <c r="N103" s="14"/>
     </row>
+    <row r="104" spans="1:14">
+      <c r="A104" s="18">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B104" s="63"/>
+      <c r="C104" s="70"/>
+      <c r="D104" s="19"/>
+      <c r="E104" s="19"/>
+      <c r="F104" s="77"/>
+      <c r="G104" s="79"/>
+      <c r="H104" s="79"/>
+      <c r="I104" s="79"/>
+      <c r="J104" s="77"/>
+      <c r="K104" s="20"/>
+      <c r="L104" s="20"/>
+      <c r="M104" s="21"/>
+      <c r="N104" s="14"/>
+    </row>
+    <row r="105" spans="1:14">
+      <c r="A105" s="18">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B105" s="63"/>
+      <c r="C105" s="70"/>
+      <c r="D105" s="64"/>
+      <c r="E105" s="64"/>
+      <c r="F105" s="78"/>
+      <c r="G105" s="80"/>
+      <c r="H105" s="80"/>
+      <c r="I105" s="80"/>
+      <c r="J105" s="78"/>
+      <c r="K105" s="66"/>
+      <c r="L105" s="66"/>
+      <c r="M105" s="67"/>
+      <c r="N105" s="14"/>
+    </row>
+    <row r="106" spans="1:14">
+      <c r="A106" s="18">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B106" s="63"/>
+      <c r="C106" s="70"/>
+      <c r="D106" s="19"/>
+      <c r="E106" s="19"/>
+      <c r="F106" s="77"/>
+      <c r="G106" s="79"/>
+      <c r="H106" s="79"/>
+      <c r="I106" s="79"/>
+      <c r="J106" s="77"/>
+      <c r="K106" s="20"/>
+      <c r="L106" s="20"/>
+      <c r="M106" s="21"/>
+      <c r="N106" s="14"/>
+    </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="J66:K67"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="E66:E67"/>
-    <mergeCell ref="D66:D67"/>
-    <mergeCell ref="I66:I67"/>
-    <mergeCell ref="F66:F67"/>
     <mergeCell ref="A26:B26"/>
-    <mergeCell ref="H66:H67"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="J69:K70"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="D69:D70"/>
+    <mergeCell ref="I69:I70"/>
+    <mergeCell ref="F69:F70"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="H69:H70"/>
+    <mergeCell ref="A14:B14"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="A95:A96"/>
-    <mergeCell ref="B95:B96"/>
-    <mergeCell ref="C95:C96"/>
-    <mergeCell ref="D95:D96"/>
-    <mergeCell ref="E95:E96"/>
-    <mergeCell ref="F95:F96"/>
-    <mergeCell ref="I95:I96"/>
-    <mergeCell ref="J95:K96"/>
-    <mergeCell ref="G66:G67"/>
-    <mergeCell ref="G95:G96"/>
-    <mergeCell ref="H95:H96"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="A98:A99"/>
+    <mergeCell ref="B98:B99"/>
+    <mergeCell ref="C98:C99"/>
+    <mergeCell ref="D98:D99"/>
+    <mergeCell ref="E98:E99"/>
+    <mergeCell ref="F98:F99"/>
+    <mergeCell ref="I98:I99"/>
+    <mergeCell ref="J98:K99"/>
+    <mergeCell ref="G69:G70"/>
+    <mergeCell ref="G98:G99"/>
+    <mergeCell ref="H98:H99"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
-  <dataValidations count="8">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E107:I107" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations disablePrompts="1" count="8">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E110:I110" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C25:C26" xr:uid="{78FE03A8-B82F-DD42-A5B2-F5AED31EB8E5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C26:C27" xr:uid="{78FE03A8-B82F-DD42-A5B2-F5AED31EB8E5}">
       <formula1>adjustFiledName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16" xr:uid="{0933AF92-3C0C-2F47-AF58-F84946F39270}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C17" xr:uid="{0933AF92-3C0C-2F47-AF58-F84946F39270}">
       <formula1>componentKind</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19:C23 C17 F68:G85" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C20:C24 C18 F71:G88" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
       <formula1>yesNo</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C24" xr:uid="{CCFC1331-CEEF-574E-9BCC-37D38F486896}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C25" xr:uid="{CCFC1331-CEEF-574E-9BCC-37D38F486896}">
       <formula1>adjustFieldName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C54:C56" xr:uid="{BDE40890-40F7-4E41-B7E1-478CEBD85557}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C57:C59" xr:uid="{BDE40890-40F7-4E41-B7E1-478CEBD85557}">
       <formula1>httpdMethod</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18" xr:uid="{B3BDB514-7849-7346-B29F-0809D4138732}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19" xr:uid="{B3BDB514-7849-7346-B29F-0809D4138732}">
       <formula1>layoutType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C28:C33" xr:uid="{D073ACF5-A392-2348-B361-3D576C1BA990}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C31:C36" xr:uid="{D073ACF5-A392-2348-B361-3D576C1BA990}">
       <formula1>adjustFiledName</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>